<commit_message>
atualizando projecao abril com as notas
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C5596B-9D5A-8945-9C56-EDE0C747D7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{12C5596B-9D5A-8945-9C56-EDE0C747D7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{101F3572-65CC-4E92-83B5-78C9915A846E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="4" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="108">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -345,7 +345,28 @@
     <t>JOBS - UNIFICADO</t>
   </si>
   <si>
-    <t>JOBS - RETRO SÉRIE: 7864 -FOI PARA UNIFICADA</t>
+    <t>JOBS - RETRO SÉRIE: 7864 - FOI PARA UNIFICADA</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>FICHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NF </t>
+  </si>
+  <si>
+    <t>465 / 132</t>
+  </si>
+  <si>
+    <t>131 / 879</t>
+  </si>
+  <si>
+    <t>886 A 891</t>
+  </si>
+  <si>
+    <t>892 A 896</t>
   </si>
 </sst>
 </file>
@@ -353,9 +374,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
@@ -444,7 +465,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,8 +490,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -808,7 +835,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -817,7 +844,24 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -827,6 +871,62 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -845,9 +945,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -857,9 +955,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -872,12 +968,19 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -887,6 +990,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -902,9 +1018,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -913,10 +1027,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -943,11 +1057,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -989,7 +1103,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1000,7 +1114,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1009,7 +1123,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,31 +1137,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,7 +1177,68 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1089,6 +1249,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1100,10 +1265,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1141,7 +1310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1247,7 +1416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1389,7 +1558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1403,19 +1572,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-    </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="75"/>
+    </row>
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1423,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1431,7 +1600,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1439,7 +1608,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -1447,7 +1616,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -1455,7 +1624,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -1463,7 +1632,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -1471,7 +1640,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -1479,7 +1648,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -1488,7 +1657,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -1496,7 +1665,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -1504,7 +1673,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +1681,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -1520,7 +1689,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -1529,7 +1698,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -1537,7 +1706,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -1545,7 +1714,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1722,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -1561,7 +1730,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -1569,11 +1738,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -1581,7 +1750,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -1589,7 +1758,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -1597,7 +1766,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -1605,7 +1774,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1782,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -1621,7 +1790,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -1629,7 +1798,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -1637,7 +1806,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -1645,7 +1814,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -1653,7 +1822,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -1661,7 +1830,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -1669,11 +1838,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -1702,22 +1871,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="68.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="68.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="83" t="s">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="84"/>
-    </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C1" s="75"/>
+    </row>
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1900,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1746,7 +1915,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1761,7 +1930,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1776,7 +1945,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1791,7 +1960,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1806,7 +1975,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1819,7 +1988,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1834,7 +2003,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1847,8 +2016,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="85">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="76">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1857,23 +2026,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="77" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="76"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="87"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1888,7 +2057,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1901,8 +2070,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="85">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="76">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1911,34 +2080,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="77" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
+    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="76"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="88"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85"/>
+    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="76"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="87"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -1953,7 +2122,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -1968,8 +2137,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="85">
+    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="76">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1978,23 +2147,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="86" t="s">
+      <c r="D20" s="77" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
+    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="76"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="87"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2009,7 +2178,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2024,7 +2193,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2039,7 +2208,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2052,7 +2221,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2067,7 +2236,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2082,7 +2251,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2092,11 +2261,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="89"/>
+      <c r="D28" s="80"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="85">
+    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="76">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2105,43 +2274,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="90"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
+    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="76"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="90"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="85"/>
+    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="76"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="90"/>
+      <c r="D31" s="81"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="85"/>
+    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="76"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="91"/>
+      <c r="D32" s="82"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2187,21 +2356,21 @@
       <selection activeCell="B36" sqref="B36:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="83" t="s">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="84"/>
-    </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C1" s="75"/>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2209,7 +2378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2220,7 +2389,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2231,7 +2400,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2242,7 +2411,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2253,7 +2422,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2265,7 +2434,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2276,7 +2445,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2287,7 +2456,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2298,8 +2467,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="83">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2309,8 +2478,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="83"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2318,7 +2487,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2329,8 +2498,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="92">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="83">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2340,8 +2509,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="83"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2349,8 +2518,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="83"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2358,8 +2527,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="92"/>
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="83"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2367,8 +2536,8 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="92"/>
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="83"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2545,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2387,7 +2556,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2398,8 +2567,8 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="92">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="83">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2409,8 +2578,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="92"/>
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="83"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2418,7 +2587,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2429,7 +2598,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2440,7 +2609,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2451,7 +2620,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2462,7 +2631,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2473,7 +2642,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2484,7 +2653,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2495,7 +2664,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2506,8 +2675,8 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="92">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="83">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2517,8 +2686,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="92"/>
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="83"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -2526,8 +2695,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="92"/>
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="83"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -2535,7 +2704,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -2546,7 +2715,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -2554,7 +2723,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -2562,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -2570,7 +2739,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -2579,7 +2748,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -2587,7 +2756,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -2595,7 +2764,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -2603,7 +2772,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -2611,7 +2780,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -2619,7 +2788,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -2627,7 +2796,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -2660,20 +2829,20 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="83" t="s">
+    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="84"/>
-    </row>
-    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C1" s="75"/>
+    </row>
+    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2681,7 +2850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2692,7 +2861,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2703,7 +2872,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2714,7 +2883,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2725,7 +2894,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2736,7 +2905,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2747,7 +2916,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2758,7 +2927,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2769,8 +2938,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="83">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2780,8 +2949,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="83"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2789,7 +2958,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2800,8 +2969,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="92">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="83">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2811,8 +2980,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="83"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2820,8 +2989,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92"/>
+    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="83"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2829,8 +2998,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="92"/>
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="83"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -2838,8 +3007,8 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="92"/>
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="83"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -2847,7 +3016,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2858,7 +3027,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2869,8 +3038,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="92">
+    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="83">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -2880,8 +3049,8 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="92"/>
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="83"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -2889,7 +3058,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2900,7 +3069,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2911,7 +3080,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2922,7 +3091,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2933,7 +3102,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2944,7 +3113,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2955,7 +3124,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2966,7 +3135,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2977,8 +3146,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="92">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="83">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2988,8 +3157,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="92"/>
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="83"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -2997,8 +3166,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="92"/>
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="83"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3006,7 +3175,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3017,7 +3186,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3028,11 +3197,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3060,379 +3229,438 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="13" style="111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="93" t="s">
+    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="93"/>
-    </row>
-    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="72" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="105"/>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="93"/>
+      <c r="B2" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="94" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="71">
+      <c r="D2" s="104" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="95">
         <v>1</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="74">
+      <c r="C3" s="97">
         <v>67500</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="71">
+      <c r="D3" s="106" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="98">
         <v>2</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="86">
         <v>35000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
+      <c r="D4" s="107">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="99">
         <v>3</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="77">
+      <c r="C5" s="101">
         <v>35000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="71">
+      <c r="D5" s="108"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="90">
         <v>4</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="85">
         <v>341000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="71">
+      <c r="D6" s="109"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="90">
         <v>5</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="84">
         <v>514388</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="71">
+      <c r="D7" s="109"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="98">
         <v>6</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="86">
         <v>168799.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="71">
+      <c r="D8" s="107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="90">
         <v>7</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="84">
         <v>42300</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="71">
+      <c r="D9" s="109"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="90">
         <v>8</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="85">
         <v>42000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="71">
+      <c r="D10" s="109"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="98">
         <v>9</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="80">
+      <c r="C11" s="86">
         <v>63702</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="71">
+      <c r="D11" s="107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="98">
         <v>10</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="86">
         <v>39976</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="71">
+      <c r="D12" s="107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="99">
         <v>11</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="77">
+      <c r="C13" s="101">
         <v>50000</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="71">
+      <c r="D13" s="108"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="90">
         <v>12</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="76">
+      <c r="C14" s="84">
         <v>33291.910000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="71">
+      <c r="D14" s="109"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="90">
         <v>13</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="77">
+      <c r="C15" s="85">
         <v>30000</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="71">
+      <c r="D15" s="109"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="98">
         <v>14</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="77">
+      <c r="C16" s="86">
         <v>27000</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="71">
+      <c r="D16" s="107">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="99">
         <v>15</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="77">
+      <c r="C17" s="101">
         <v>26000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="71">
+      <c r="D17" s="108"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="99">
         <v>16</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="77">
+      <c r="C18" s="101">
         <v>50000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="71">
+      <c r="D18" s="108">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="98">
         <v>17</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="86">
         <v>15000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="71">
+      <c r="D19" s="107">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="99">
         <v>18</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="77">
+      <c r="C20" s="101">
         <v>9000</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="71">
+      <c r="D20" s="108"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="99">
         <v>19</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="77">
+      <c r="C21" s="101">
         <v>14000</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="71">
+      <c r="D21" s="108"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="90">
         <v>20</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="85">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="71">
+      <c r="D22" s="109"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="90">
         <v>21</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="77">
+      <c r="C23" s="85">
         <v>23000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="71">
+      <c r="D23" s="109"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="90">
         <v>22</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="77">
+      <c r="C24" s="85">
         <v>18000</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="71">
+      <c r="D24" s="109"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="90">
         <v>23</v>
       </c>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="77">
+      <c r="C25" s="85">
         <v>12000</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="71">
+      <c r="D25" s="109"/>
+    </row>
+    <row r="26" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="90">
         <v>24</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="82">
+      <c r="C26" s="87">
         <v>39000</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
+      <c r="D26" s="109"/>
+    </row>
+    <row r="27" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="91"/>
       <c r="B27" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="69"/>
+      <c r="D27" s="109"/>
+    </row>
+    <row r="28" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="91"/>
       <c r="B28" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="52">
+      <c r="C28" s="18">
         <v>76525.679999999993</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="69"/>
+      <c r="D28" s="109"/>
+    </row>
+    <row r="29" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="91"/>
       <c r="B29" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C29" s="18">
         <v>27100</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="69"/>
+      <c r="D29" s="109"/>
+    </row>
+    <row r="30" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="91"/>
       <c r="B30" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="52">
+      <c r="C30" s="18">
         <v>191666</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="69"/>
+      <c r="D30" s="109"/>
+    </row>
+    <row r="31" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="91"/>
       <c r="B31" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="52">
+      <c r="C31" s="18">
         <v>29742</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="69"/>
+      <c r="D31" s="109"/>
+    </row>
+    <row r="32" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="91"/>
       <c r="B32" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="52">
+      <c r="C32" s="18">
         <v>119500</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="69"/>
+      <c r="D32" s="109"/>
+    </row>
+    <row r="33" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="91"/>
       <c r="B33" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="47">
+      <c r="C33" s="13">
         <v>12612.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="69"/>
+      <c r="D33" s="109"/>
+    </row>
+    <row r="34" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="92"/>
       <c r="B34" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="52">
+      <c r="C34" s="18">
         <v>33000</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="67"/>
+      <c r="D34" s="110"/>
+    </row>
+    <row r="35" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="103"/>
+      <c r="B35" s="67" t="s">
+        <v>102</v>
+      </c>
       <c r="C35" s="68"/>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="67"/>
+    <row r="36" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="102"/>
+      <c r="B36" s="67" t="s">
+        <v>103</v>
+      </c>
       <c r="C36" s="68"/>
     </row>
-    <row r="37" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B37" s="65" t="s">
         <v>35</v>
       </c>
@@ -3441,7 +3669,7 @@
         <v>2186104.27</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B38" s="65" t="s">
         <v>96</v>
       </c>
@@ -3450,7 +3678,7 @@
         <v>1695957.69</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B39" s="65" t="s">
         <v>97</v>
       </c>
@@ -3459,14 +3687,14 @@
         <v>490146.58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="70"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C43" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inclusao diaria esteira dhl 5k
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246ECFED-069E-AD40-95FD-663400953563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221011BC-5423-8946-BC9A-F766627FE232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="4" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="123">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>GRAND LODGE - MARÇO</t>
+  </si>
+  <si>
+    <t>GREEN DHL - 1 DIARIA ESTEIRA + FRETE</t>
   </si>
 </sst>
 </file>
@@ -1082,6 +1085,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1098,9 +1104,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1902,7 +1905,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="100">
+      <c r="A11" s="94">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1911,20 +1914,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="95" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="100"/>
+      <c r="A12" s="94"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="95"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -1956,7 +1959,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="100">
+      <c r="A15" s="94">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1965,31 +1968,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="95" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
+      <c r="A16" s="94"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="96"/>
+      <c r="D16" s="97"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
+      <c r="A17" s="94"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="95"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2023,7 +2026,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100">
+      <c r="A20" s="94">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2032,20 +2035,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="94" t="s">
+      <c r="D20" s="95" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
+      <c r="A21" s="94"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="95"/>
+      <c r="D21" s="96"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2146,11 +2149,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="97"/>
+      <c r="D28" s="98"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="100">
+      <c r="A29" s="94">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2159,40 +2162,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="98"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="100"/>
+      <c r="A30" s="94"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="98"/>
+      <c r="D30" s="99"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="100"/>
+      <c r="A31" s="94"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="98"/>
+      <c r="D31" s="99"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="100"/>
+      <c r="A32" s="94"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="99"/>
+      <c r="D32" s="100"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2208,6 +2211,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2216,7 +2220,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -3116,7 +3119,7 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -3650,8 +3653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433067E7-40EE-41F6-A8ED-E30D0BB2251C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3774,7 +3777,7 @@
       <c r="A15" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="90">
+      <c r="B15" s="89">
         <v>14000</v>
       </c>
     </row>
@@ -3782,7 +3785,7 @@
       <c r="A16" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="90">
+      <c r="B16" s="89">
         <v>23000</v>
       </c>
     </row>
@@ -3790,7 +3793,7 @@
       <c r="A17" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="90">
+      <c r="B17" s="89">
         <v>17000</v>
       </c>
     </row>
@@ -3798,7 +3801,7 @@
       <c r="A18" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="90">
+      <c r="B18" s="89">
         <v>28600</v>
       </c>
     </row>
@@ -3806,13 +3809,17 @@
       <c r="A19" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="90">
+      <c r="B19" s="89">
         <v>14193.55</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="88"/>
-      <c r="B20" s="90"/>
+      <c r="A20" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="89">
+        <v>5000</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="88"/>
@@ -3824,7 +3831,7 @@
       </c>
       <c r="B22" s="53">
         <f>SUM(B3:B21)</f>
-        <v>620363.55000000005</v>
+        <v>625363.55000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JHSF STATES ERICA TARTOR DE ESTEIRAS MAIO
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/BRYAN MEDIÇÕES - PROJEÇÕES/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{EDBD30DA-2A0A-AA4D-8061-8DDD0A50D676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BADEAB2-48DF-4927-B09C-339628750C4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25180FA0-808A-2B4B-A73F-104C3BBCB56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>906 A 910</t>
+  </si>
+  <si>
+    <t>JHSF STATES - ERICA - TRATOR DE ESTEIRA FOI DIA 29/05</t>
   </si>
 </sst>
 </file>
@@ -426,9 +429,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
@@ -953,7 +956,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="117">
@@ -983,11 +986,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1029,7 +1032,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1040,7 +1043,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1049,7 +1052,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1060,7 +1063,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1093,10 +1096,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,57 +1111,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1166,20 +1118,71 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1510,19 +1513,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="98"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -1578,7 +1581,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -1595,7 +1598,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -1636,7 +1639,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -1676,11 +1679,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -1752,7 +1755,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -1776,11 +1779,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -1809,22 +1812,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="68.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="89" t="s">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="90"/>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="98"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1853,7 +1856,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1868,7 +1871,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1883,7 +1886,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1898,7 +1901,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1913,7 +1916,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1926,7 +1929,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1941,7 +1944,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1954,8 +1957,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="97">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="99">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1964,23 +1967,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="100" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="97"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="99"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="92"/>
+      <c r="D12" s="101"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1995,7 +1998,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2008,8 +2011,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="97">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="99">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2018,34 +2021,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="100" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="97"/>
+    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="99"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="93"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="97"/>
+    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="99"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="101"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -2060,7 +2063,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -2075,8 +2078,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="97">
+    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="99">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2085,23 +2088,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="91" t="s">
+      <c r="D20" s="100" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="97"/>
+    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="99"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="92"/>
+      <c r="D21" s="101"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2116,7 +2119,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2131,7 +2134,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2146,7 +2149,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2159,7 +2162,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2174,7 +2177,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2189,7 +2192,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2199,11 +2202,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="94"/>
+      <c r="D28" s="103"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="97">
+    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="99">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2212,43 +2215,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="95"/>
+      <c r="D29" s="104"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="97"/>
+    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="99"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="95"/>
+      <c r="D30" s="104"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="97"/>
+    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="99"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="95"/>
+      <c r="D31" s="104"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="97"/>
+    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="99"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="96"/>
+      <c r="D32" s="105"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2261,6 +2264,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2269,7 +2273,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2294,21 +2297,21 @@
       <selection activeCell="B36" sqref="B36:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="89" t="s">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="90"/>
-    </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="98"/>
+    </row>
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2372,7 +2375,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2405,8 +2408,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="98">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="106">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2416,8 +2419,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="98"/>
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="106"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2425,7 +2428,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2436,8 +2439,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="98">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="106">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2447,8 +2450,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="98"/>
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="106"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2456,8 +2459,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="98"/>
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="106"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2465,8 +2468,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="98"/>
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="106"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2474,8 +2477,8 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="98"/>
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="106"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2505,8 +2508,8 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="98">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="106">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2516,8 +2519,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="98"/>
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="106"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2580,7 +2583,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2613,8 +2616,8 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="98">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="106">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2624,8 +2627,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="98"/>
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="106"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -2633,8 +2636,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="98"/>
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="106"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -2686,7 +2689,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -2767,20 +2770,20 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="89" t="s">
+    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="90"/>
-    </row>
-    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="98"/>
+    </row>
+    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2799,7 +2802,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2810,7 +2813,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2865,7 +2868,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2876,8 +2879,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="98">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="106">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2887,8 +2890,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="98"/>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="106"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2907,8 +2910,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="98">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="106">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2918,8 +2921,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="98"/>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="106"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2927,8 +2930,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="98"/>
+    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="106"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2936,8 +2939,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="98"/>
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="106"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -2945,8 +2948,8 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="98"/>
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="106"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2976,8 +2979,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="98">
+    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="106">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -2987,8 +2990,8 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="98"/>
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="106"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -3007,7 +3010,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3051,7 +3054,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3073,7 +3076,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3084,8 +3087,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="98">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="106">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3095,8 +3098,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="98"/>
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="106"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3104,8 +3107,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="98"/>
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="106"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3124,7 +3127,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3135,11 +3138,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3173,26 +3176,26 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="13" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-    </row>
-    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A2" s="101" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+    </row>
+    <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="109"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="68">
         <v>2</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="D5" s="75"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -3252,7 +3255,7 @@
       </c>
       <c r="D6" s="79"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="76">
         <v>5</v>
       </c>
@@ -3264,7 +3267,7 @@
       </c>
       <c r="D7" s="79"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="68">
         <v>6</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="76">
         <v>7</v>
       </c>
@@ -3290,7 +3293,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="68">
         <v>8</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="68">
         <v>9</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="68">
         <v>10</v>
       </c>
@@ -3332,7 +3335,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -3344,7 +3347,7 @@
       </c>
       <c r="D13" s="75"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="76">
         <v>12</v>
       </c>
@@ -3356,7 +3359,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>13</v>
       </c>
@@ -3368,7 +3371,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="68">
         <v>14</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -3394,7 +3397,7 @@
       </c>
       <c r="D17" s="75"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -3408,7 +3411,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="68">
         <v>17</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -3434,7 +3437,7 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -3446,7 +3449,7 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="76">
         <v>20</v>
       </c>
@@ -3458,7 +3461,7 @@
       </c>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="76">
         <v>21</v>
       </c>
@@ -3470,7 +3473,7 @@
       </c>
       <c r="D23" s="79"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="76">
         <v>22</v>
       </c>
@@ -3482,7 +3485,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="76">
         <v>23</v>
       </c>
@@ -3494,7 +3497,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="76">
         <v>24</v>
       </c>
@@ -3506,7 +3509,7 @@
       </c>
       <c r="D26" s="79"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="76">
         <v>25</v>
       </c>
@@ -3518,7 +3521,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
       <c r="B28" s="79" t="s">
         <v>81</v>
@@ -3528,7 +3531,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>99</v>
@@ -3538,7 +3541,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>84</v>
@@ -3548,7 +3551,7 @@
       </c>
       <c r="D30" s="79"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>85</v>
@@ -3558,7 +3561,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>117</v>
@@ -3568,7 +3571,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="76"/>
       <c r="B33" s="77" t="s">
         <v>87</v>
@@ -3578,7 +3581,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="76"/>
       <c r="B34" s="77" t="s">
         <v>119</v>
@@ -3588,7 +3591,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="68"/>
       <c r="B35" s="69" t="s">
         <v>26</v>
@@ -3600,7 +3603,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
         <v>120</v>
@@ -3611,7 +3614,7 @@
       <c r="D36" s="78"/>
       <c r="E36" s="79"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
         <v>121</v>
@@ -3621,7 +3624,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="76"/>
       <c r="B38" s="77" t="s">
         <v>115</v>
@@ -3631,7 +3634,7 @@
       </c>
       <c r="D38" s="78"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="76"/>
       <c r="B39" s="77" t="s">
         <v>118</v>
@@ -3641,7 +3644,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="76"/>
       <c r="B40" s="77" t="s">
         <v>116</v>
@@ -3651,43 +3654,43 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A41" s="102" t="s">
+    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A41" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="103"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A42" s="104" t="s">
+    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A42" s="112" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="105"/>
+      <c r="B42" s="113"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A43" s="99" t="s">
+    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="100"/>
+      <c r="B43" s="108"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="66"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="66"/>
     </row>
   </sheetData>
@@ -3705,37 +3708,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433067E7-40EE-41F6-A8ED-E30D0BB2251C}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="76.625" customWidth="1"/>
-    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="112" t="s">
+    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="114"/>
-    </row>
-    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+    </row>
+    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="95" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
@@ -3744,7 +3747,7 @@
       </c>
       <c r="C3" s="30"/>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>7</v>
       </c>
@@ -3753,7 +3756,7 @@
       </c>
       <c r="C4" s="30"/>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>123</v>
       </c>
@@ -3762,166 +3765,176 @@
       </c>
       <c r="C5" s="30"/>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="5">
+        <f>(35000/31)*3</f>
+        <v>3387.0967741935483</v>
+      </c>
+      <c r="C6" s="30"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="6">
         <v>35000</v>
       </c>
-      <c r="C6" s="30"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="106" t="s">
+      <c r="C7" s="30"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B8" s="9">
         <v>79070</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C8" s="96" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>80000</v>
       </c>
-      <c r="C8" s="30"/>
-    </row>
-    <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="40" t="s">
+      <c r="C9" s="30"/>
+    </row>
+    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="5">
         <v>70000</v>
       </c>
-      <c r="C9" s="30"/>
-    </row>
-    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="86" t="s">
+      <c r="C10" s="30"/>
+    </row>
+    <row r="11" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B11" s="91">
         <v>30000</v>
       </c>
-      <c r="C10" s="30"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="56" t="s">
+      <c r="C11" s="30"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="109">
+      <c r="B12" s="92">
         <v>27000</v>
       </c>
-      <c r="C11" s="30"/>
-    </row>
-    <row r="12" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="87" t="s">
+      <c r="C12" s="30"/>
+    </row>
+    <row r="13" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="110">
+      <c r="B13" s="93">
         <v>26000</v>
       </c>
-      <c r="C12" s="30"/>
-    </row>
-    <row r="13" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="87" t="s">
+      <c r="C13" s="30"/>
+    </row>
+    <row r="14" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="110">
+      <c r="B14" s="93">
         <v>50000</v>
       </c>
-      <c r="C13" s="30"/>
-    </row>
-    <row r="14" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="87" t="s">
+      <c r="C14" s="30"/>
+    </row>
+    <row r="15" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="110">
+      <c r="B15" s="93">
         <v>15000</v>
       </c>
-      <c r="C14" s="30"/>
-    </row>
-    <row r="15" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="87" t="s">
+      <c r="C15" s="30"/>
+    </row>
+    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="110">
+      <c r="B16" s="93">
         <v>9000</v>
       </c>
-      <c r="C15" s="30"/>
-    </row>
-    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="87" t="s">
+      <c r="C16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="110">
+      <c r="B17" s="93">
         <v>14000</v>
       </c>
-      <c r="C16" s="30"/>
-    </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="87" t="s">
+      <c r="C17" s="30"/>
+    </row>
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="110">
+      <c r="B18" s="93">
         <v>23000</v>
       </c>
-      <c r="C17" s="30"/>
-    </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="87" t="s">
+      <c r="C18" s="30"/>
+    </row>
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="110">
+      <c r="B19" s="93">
         <v>17000</v>
       </c>
-      <c r="C18" s="30"/>
-    </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="87" t="s">
+      <c r="C19" s="30"/>
+    </row>
+    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="110">
+      <c r="B20" s="93">
         <v>28600</v>
       </c>
-      <c r="C19" s="30"/>
-    </row>
-    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="87" t="s">
+      <c r="C20" s="30"/>
+    </row>
+    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="110">
+      <c r="B21" s="93">
         <v>14193.55</v>
       </c>
-      <c r="C20" s="30"/>
-    </row>
-    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="87" t="s">
+      <c r="C21" s="30"/>
+    </row>
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="110">
+      <c r="B22" s="93">
         <v>5000</v>
       </c>
-      <c r="C21" s="30"/>
-    </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="87"/>
-      <c r="B22" s="111"/>
       <c r="C22" s="30"/>
     </row>
-    <row r="23" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="87"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="30"/>
+    </row>
+    <row r="24" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="22">
-        <f>SUM(B3:B22)</f>
-        <v>666040.97</v>
-      </c>
-      <c r="C23" s="30"/>
+      <c r="B24" s="22">
+        <f>SUM(B3:B23)</f>
+        <v>669428.06677419355</v>
+      </c>
+      <c r="C24" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removi um registro de maio
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25180FA0-808A-2B4B-A73F-104C3BBCB56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88876BBF-4214-5241-A015-220933F9A7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="125">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -410,9 +410,6 @@
   </si>
   <si>
     <t>GRAND LODGE - MARÇO</t>
-  </si>
-  <si>
-    <t>GREEN DHL - 1 DIARIA ESTEIRA + FRETE</t>
   </si>
   <si>
     <t>JHSF - LAGOS</t>
@@ -2264,15 +2261,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D28:D32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -3172,7 +3169,7 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3708,10 +3705,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433067E7-40EE-41F6-A8ED-E30D0BB2251C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="5">
         <v>55000</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="5">
         <f>(35000/31)*3</f>
@@ -3792,7 +3792,7 @@
         <v>79070</v>
       </c>
       <c r="C8" s="96" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -3913,12 +3913,8 @@
       <c r="C21" s="30"/>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="93">
-        <v>5000</v>
-      </c>
+      <c r="A22" s="87"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -3932,7 +3928,7 @@
       </c>
       <c r="B24" s="22">
         <f>SUM(B3:B23)</f>
-        <v>669428.06677419355</v>
+        <v>664428.06677419355</v>
       </c>
       <c r="C24" s="30"/>
     </row>
@@ -3941,6 +3937,6 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JOAO VICTOR ATUALIZADO 39K
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88876BBF-4214-5241-A015-220933F9A7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79039DB2-E135-6C44-981C-8DD335BEDE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -1126,9 +1126,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1145,6 +1142,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1955,7 +1955,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="99">
+      <c r="A11" s="105">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1964,20 +1964,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="99" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="101"/>
+      <c r="D12" s="100"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="99">
+      <c r="A15" s="105">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2018,31 +2018,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="99" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="99"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="102"/>
+      <c r="D16" s="101"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="99"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="101"/>
+      <c r="D17" s="100"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2076,7 +2076,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="99">
+      <c r="A20" s="105">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2085,20 +2085,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="99" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="101"/>
+      <c r="D21" s="100"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2199,11 +2199,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="103"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="99">
+      <c r="A29" s="105">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2212,40 +2212,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="104"/>
+      <c r="D29" s="103"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="99"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="104"/>
+      <c r="D30" s="103"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="99"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="104"/>
+      <c r="D31" s="103"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="99"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="105"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2261,15 +2261,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -3711,7 +3711,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3899,7 +3899,7 @@
         <v>112</v>
       </c>
       <c r="B20" s="93">
-        <v>28600</v>
+        <v>39000</v>
       </c>
       <c r="C20" s="30"/>
     </row>
@@ -3928,7 +3928,7 @@
       </c>
       <c r="B24" s="22">
         <f>SUM(B3:B23)</f>
-        <v>664428.06677419355</v>
+        <v>674828.06677419355</v>
       </c>
       <c r="C24" s="30"/>
     </row>

</xml_diff>

<commit_message>
ALCANCE 1 QUINZENA ALTERADA PARA 49755
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DB987B-7B2F-4C4D-B3B1-B6E7E42413E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8C0EB8-6F70-BE4B-A42D-340730F34BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -1167,66 +1167,6 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1244,6 +1184,66 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1582,10 +1582,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
+      <c r="B1" s="104"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
@@ -1884,10 +1884,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="96"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2020,7 +2020,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="103">
+      <c r="A11" s="105">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2029,20 +2029,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="106" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="103"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="98"/>
+      <c r="D12" s="107"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="103">
+      <c r="A15" s="105">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2083,31 +2083,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="97" t="s">
+      <c r="D15" s="106" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="103"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="99"/>
+      <c r="D16" s="108"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="103"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="98"/>
+      <c r="D17" s="107"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2141,7 +2141,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="103">
+      <c r="A20" s="105">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2150,20 +2150,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="97" t="s">
+      <c r="D20" s="106" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="103"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="98"/>
+      <c r="D21" s="107"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2264,11 +2264,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="100"/>
+      <c r="D28" s="109"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="103">
+      <c r="A29" s="105">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2277,40 +2277,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="101"/>
+      <c r="D29" s="110"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="103"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="101"/>
+      <c r="D30" s="110"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="103"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="101"/>
+      <c r="D31" s="110"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="103"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="102"/>
+      <c r="D32" s="111"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2326,6 +2326,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2334,7 +2335,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2368,10 +2368,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="96"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2471,7 +2471,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="104">
+      <c r="A11" s="112">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2482,7 +2482,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
+      <c r="A12" s="112"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2502,7 +2502,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="104">
+      <c r="A14" s="112">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2513,7 +2513,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
+      <c r="A15" s="112"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2522,7 +2522,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2531,7 +2531,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="104"/>
+      <c r="A17" s="112"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2540,7 +2540,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="104"/>
+      <c r="A18" s="112"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2571,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="104">
+      <c r="A21" s="112">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2582,7 +2582,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104"/>
+      <c r="A22" s="112"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2679,7 +2679,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="104">
+      <c r="A31" s="112">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2690,7 +2690,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="104"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -2699,7 +2699,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="104"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -2840,10 +2840,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="96"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2942,7 +2942,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="104">
+      <c r="A11" s="112">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2953,7 +2953,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
+      <c r="A12" s="112"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2973,7 +2973,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="104">
+      <c r="A14" s="112">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2984,7 +2984,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
+      <c r="A15" s="112"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2993,7 +2993,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="104"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3002,7 +3002,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="104"/>
+      <c r="A17" s="112"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3011,7 +3011,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="104"/>
+      <c r="A18" s="112"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3042,7 +3042,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="104">
+      <c r="A21" s="112">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3053,7 +3053,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104"/>
+      <c r="A22" s="112"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3150,7 +3150,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="104">
+      <c r="A31" s="112">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="104"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3170,7 +3170,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="104"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3246,18 +3246,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
     </row>
     <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="107"/>
+      <c r="B2" s="115"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -3717,10 +3717,10 @@
       <c r="D40" s="79"/>
     </row>
     <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="108" t="s">
+      <c r="A41" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="109"/>
+      <c r="B41" s="117"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
@@ -3728,10 +3728,10 @@
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="110" t="s">
+      <c r="A42" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="111"/>
+      <c r="B42" s="119"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
@@ -3739,10 +3739,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="105" t="s">
+      <c r="A43" s="113" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="106"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
@@ -3776,7 +3776,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3786,11 +3786,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="114"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="122"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3799,12 +3799,12 @@
       <c r="C2" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="95" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120">
+      <c r="A3" s="100">
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -3813,10 +3813,10 @@
       <c r="C3" s="5">
         <v>59951.61</v>
       </c>
-      <c r="D3" s="116"/>
+      <c r="D3" s="96"/>
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120">
+      <c r="A4" s="100">
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -3825,10 +3825,10 @@
       <c r="C4" s="5">
         <v>28225.81</v>
       </c>
-      <c r="D4" s="116"/>
+      <c r="D4" s="96"/>
     </row>
     <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="120">
+      <c r="A5" s="100">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -3837,10 +3837,10 @@
       <c r="C5" s="5">
         <v>55000</v>
       </c>
-      <c r="D5" s="116"/>
+      <c r="D5" s="96"/>
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120">
+      <c r="A6" s="100">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
@@ -3850,10 +3850,10 @@
         <f>(35000/31)*3</f>
         <v>3387.0967741935483</v>
       </c>
-      <c r="D6" s="116"/>
+      <c r="D6" s="96"/>
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="120">
+      <c r="A7" s="100">
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -3862,24 +3862,24 @@
       <c r="C7" s="6">
         <v>35000</v>
       </c>
-      <c r="D7" s="116"/>
+      <c r="D7" s="96"/>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="120">
+      <c r="A8" s="100">
         <v>6</v>
       </c>
       <c r="B8" s="89" t="s">
         <v>107</v>
       </c>
       <c r="C8" s="9">
-        <v>79070</v>
-      </c>
-      <c r="D8" s="117" t="s">
+        <v>49755</v>
+      </c>
+      <c r="D8" s="97" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120">
+      <c r="A9" s="100">
         <v>7</v>
       </c>
       <c r="B9" s="40" t="s">
@@ -3888,10 +3888,10 @@
       <c r="C9" s="5">
         <v>80000</v>
       </c>
-      <c r="D9" s="116"/>
+      <c r="D9" s="96"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120">
+      <c r="A10" s="100">
         <v>8</v>
       </c>
       <c r="B10" s="40" t="s">
@@ -3900,10 +3900,10 @@
       <c r="C10" s="5">
         <v>69612.899999999994</v>
       </c>
-      <c r="D10" s="116"/>
+      <c r="D10" s="96"/>
     </row>
     <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="121">
+      <c r="A11" s="101">
         <v>9</v>
       </c>
       <c r="B11" s="86" t="s">
@@ -3912,10 +3912,10 @@
       <c r="C11" s="91">
         <v>30000</v>
       </c>
-      <c r="D11" s="116"/>
+      <c r="D11" s="96"/>
     </row>
     <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="120">
+      <c r="A12" s="100">
         <v>10</v>
       </c>
       <c r="B12" s="56" t="s">
@@ -3924,10 +3924,10 @@
       <c r="C12" s="92">
         <v>27000</v>
       </c>
-      <c r="D12" s="116"/>
+      <c r="D12" s="96"/>
     </row>
     <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="120">
+      <c r="A13" s="100">
         <v>11</v>
       </c>
       <c r="B13" s="87" t="s">
@@ -3936,10 +3936,10 @@
       <c r="C13" s="93">
         <v>26000</v>
       </c>
-      <c r="D13" s="116"/>
+      <c r="D13" s="96"/>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120">
+      <c r="A14" s="100">
         <v>12</v>
       </c>
       <c r="B14" s="87" t="s">
@@ -3948,10 +3948,10 @@
       <c r="C14" s="93">
         <v>50000</v>
       </c>
-      <c r="D14" s="116"/>
+      <c r="D14" s="96"/>
     </row>
     <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="119">
+      <c r="A15" s="99">
         <v>13</v>
       </c>
       <c r="B15" s="87" t="s">
@@ -3960,10 +3960,10 @@
       <c r="C15" s="93">
         <v>15000</v>
       </c>
-      <c r="D15" s="116"/>
+      <c r="D15" s="96"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="122">
+      <c r="A16" s="102">
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
@@ -3972,10 +3972,10 @@
       <c r="C16" s="93">
         <v>9000</v>
       </c>
-      <c r="D16" s="116"/>
+      <c r="D16" s="96"/>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="120">
+      <c r="A17" s="100">
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
@@ -3984,10 +3984,10 @@
       <c r="C17" s="93">
         <v>14000</v>
       </c>
-      <c r="D17" s="116"/>
+      <c r="D17" s="96"/>
     </row>
     <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="120">
+      <c r="A18" s="100">
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
@@ -3996,10 +3996,10 @@
       <c r="C18" s="93">
         <v>23000</v>
       </c>
-      <c r="D18" s="116"/>
+      <c r="D18" s="96"/>
     </row>
     <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="120">
+      <c r="A19" s="100">
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
@@ -4008,10 +4008,10 @@
       <c r="C19" s="93">
         <v>17000</v>
       </c>
-      <c r="D19" s="116"/>
+      <c r="D19" s="96"/>
     </row>
     <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="120">
+      <c r="A20" s="100">
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
@@ -4020,10 +4020,10 @@
       <c r="C20" s="93">
         <v>39000</v>
       </c>
-      <c r="D20" s="116"/>
+      <c r="D20" s="96"/>
     </row>
     <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="120">
+      <c r="A21" s="100">
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
@@ -4032,17 +4032,17 @@
       <c r="C21" s="93">
         <v>14193.55</v>
       </c>
-      <c r="D21" s="116"/>
+      <c r="D21" s="96"/>
     </row>
     <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="87"/>
       <c r="C22" s="93"/>
-      <c r="D22" s="116"/>
+      <c r="D22" s="96"/>
     </row>
     <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="87"/>
       <c r="C23" s="94"/>
-      <c r="D23" s="116"/>
+      <c r="D23" s="96"/>
     </row>
     <row r="24" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="21" t="s">
@@ -4050,9 +4050,9 @@
       </c>
       <c r="C24" s="22">
         <f>SUM(C3:C23)</f>
-        <v>674440.96677419357</v>
-      </c>
-      <c r="D24" s="118"/>
+        <v>645125.96677419357</v>
+      </c>
+      <c r="D24" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
RFM 106 PARA 105
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E26FBD-9902-4249-A67C-C1EECB72B294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC94BDF1-C66F-0B4B-970F-C70D92C6902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -2348,15 +2348,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D28:D32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -4093,7 +4093,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4176,7 +4176,7 @@
         <v>125</v>
       </c>
       <c r="C7" s="5">
-        <v>106451</v>
+        <v>105000</v>
       </c>
       <c r="D7" s="96"/>
     </row>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="C25" s="22">
         <f>SUM(C3:C24)</f>
-        <v>1052189.8699999999</v>
+        <v>1050738.8699999999</v>
       </c>
       <c r="D25" s="98"/>
     </row>

</xml_diff>

<commit_message>
RETRO DANIEL SAO BENEDITO TERRAP
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC94BDF1-C66F-0B4B-970F-C70D92C6902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA1021-8BA5-5445-B316-3CEF54EB73BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="133">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>ALCANCE - 2º QUINZENA JUNHO DE 2024</t>
+  </si>
+  <si>
+    <t>SÃO BENEDITO TERRAPLENAGEM - RETRO SÉRIE: 89176 - 07/06</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1032,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1213,27 +1216,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1267,6 +1270,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -2042,7 +2046,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="105">
+      <c r="A11" s="111">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2051,20 +2055,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="106" t="s">
+      <c r="D11" s="105" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="107"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2096,7 +2100,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="105">
+      <c r="A15" s="111">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2105,31 +2109,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="106" t="s">
+      <c r="D15" s="105" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="105"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="108"/>
+      <c r="D16" s="107"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="105"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="107"/>
+      <c r="D17" s="106"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2163,7 +2167,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="105">
+      <c r="A20" s="111">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2172,20 +2176,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="106" t="s">
+      <c r="D20" s="105" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="107"/>
+      <c r="D21" s="106"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2286,11 +2290,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="109"/>
+      <c r="D28" s="108"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="105">
+      <c r="A29" s="111">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2299,40 +2303,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="110"/>
+      <c r="D29" s="109"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="105"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="110"/>
+      <c r="D30" s="109"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="105"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="110"/>
+      <c r="D31" s="109"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="105"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="111"/>
+      <c r="D32" s="110"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2348,15 +2352,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -3798,7 +3802,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4090,10 +4094,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4196,13 +4200,13 @@
       <c r="A9" s="100">
         <v>7</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="5">
         <v>49755</v>
       </c>
-      <c r="D9" s="97"/>
+      <c r="D9" s="123"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="100">
@@ -4361,24 +4365,37 @@
       <c r="D22" s="96"/>
     </row>
     <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="100">
+        <v>21</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="93">
+        <f>(17000/30)* 23</f>
+        <v>13033.333333333332</v>
+      </c>
       <c r="D23" s="96"/>
     </row>
     <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="87"/>
-      <c r="C24" s="94"/>
+      <c r="C24" s="93"/>
       <c r="D24" s="96"/>
     </row>
-    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="21" t="s">
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="87"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="96"/>
+    </row>
+    <row r="26" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="22">
-        <f>SUM(C3:C24)</f>
-        <v>1050738.8699999999</v>
-      </c>
-      <c r="D25" s="98"/>
+      <c r="C26" s="22">
+        <f>SUM(C3:C25)</f>
+        <v>1063772.2033333331</v>
+      </c>
+      <c r="D26" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ATUALZIMAOS OS ATRASADOS DAS MEDICOES DE ABRIL
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E9007-C0A7-B048-8EE4-14DD9E4EA3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64183AA1-8F7A-4E4C-870C-514BEE21C4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="140">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -447,6 +447,24 @@
   </si>
   <si>
     <t>JHSF - LAGOS - 13/06</t>
+  </si>
+  <si>
+    <t>ATRASADOS</t>
+  </si>
+  <si>
+    <t>MARÇO</t>
+  </si>
+  <si>
+    <t>VER DAVI</t>
+  </si>
+  <si>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>RECIBO</t>
+  </si>
+  <si>
+    <t>FICHA</t>
   </si>
 </sst>
 </file>
@@ -459,7 +477,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -567,8 +585,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,8 +652,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1029,13 +1070,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1199,7 +1275,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1210,9 +1285,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1220,27 +1292,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,6 +1345,51 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1284,10 +1401,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF9900"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1611,10 +1728,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
+      <c r="B1" s="103"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
@@ -1913,10 +2030,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="105"/>
+      <c r="C1" s="103"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2049,7 +2166,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="106">
+      <c r="A11" s="110">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2058,20 +2175,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="107" t="s">
+      <c r="D11" s="104" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="106"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="108"/>
+      <c r="D12" s="105"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2103,7 +2220,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="106">
+      <c r="A15" s="110">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2112,31 +2229,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="107" t="s">
+      <c r="D15" s="104" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="106"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="109"/>
+      <c r="D16" s="106"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="106"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="108"/>
+      <c r="D17" s="105"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2170,7 +2287,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="106">
+      <c r="A20" s="110">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2179,20 +2296,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="107" t="s">
+      <c r="D20" s="104" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="106"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="108"/>
+      <c r="D21" s="105"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2293,11 +2410,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="110"/>
+      <c r="D28" s="107"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="106">
+      <c r="A29" s="110">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2306,40 +2423,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="111"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="106"/>
+      <c r="A30" s="110"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="111"/>
+      <c r="D30" s="108"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="106"/>
+      <c r="A31" s="110"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="111"/>
+      <c r="D31" s="108"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="106"/>
+      <c r="A32" s="110"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="112"/>
+      <c r="D32" s="109"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2355,15 +2472,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2397,10 +2514,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="105"/>
+      <c r="C1" s="103"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2500,7 +2617,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="113">
+      <c r="A11" s="111">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2511,7 +2628,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="113"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2531,7 +2648,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="113">
+      <c r="A14" s="111">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2542,7 +2659,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2551,7 +2668,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2560,7 +2677,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="113"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2569,7 +2686,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="113"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2600,7 +2717,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="113">
+      <c r="A21" s="111">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2611,7 +2728,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="113"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2708,7 +2825,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113">
+      <c r="A31" s="111">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2719,7 +2836,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="113"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -2728,7 +2845,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="113"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -2869,10 +2986,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="105"/>
+      <c r="C1" s="103"/>
     </row>
     <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2971,7 +3088,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="113">
+      <c r="A11" s="111">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2982,7 +3099,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="113"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3002,7 +3119,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="113">
+      <c r="A14" s="111">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3013,7 +3130,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3022,7 +3139,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="113"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3031,7 +3148,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="113"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3040,7 +3157,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="113"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3071,7 +3188,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="113">
+      <c r="A21" s="111">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3082,7 +3199,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="113"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3179,7 +3296,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113">
+      <c r="A31" s="111">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3190,7 +3307,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="113"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3199,7 +3316,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="113"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3263,8 +3380,8 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -3275,18 +3392,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
     </row>
     <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="116"/>
+      <c r="B2" s="114"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -3589,16 +3706,18 @@
       <c r="D25" s="79"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="76">
+      <c r="A26" s="68">
         <v>24</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="78">
+      <c r="C26" s="70">
         <v>39000</v>
       </c>
-      <c r="D26" s="79"/>
+      <c r="D26" s="71">
+        <v>911</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="76">
@@ -3746,10 +3865,10 @@
       <c r="D40" s="79"/>
     </row>
     <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="117" t="s">
+      <c r="A41" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="118"/>
+      <c r="B41" s="116"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
@@ -3757,10 +3876,10 @@
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="120"/>
+      <c r="B42" s="118"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
@@ -3768,10 +3887,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="114" t="s">
+      <c r="A43" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="115"/>
+      <c r="B43" s="113"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
@@ -3802,24 +3921,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="76.6640625" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="122"/>
-      <c r="D1" s="123"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="121"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3833,7 +3953,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100">
+      <c r="A3" s="99">
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -3842,10 +3962,10 @@
       <c r="C3" s="5">
         <v>54435.48</v>
       </c>
-      <c r="D3" s="96"/>
+      <c r="D3" s="133"/>
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="100">
+      <c r="A4" s="99">
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -3854,10 +3974,10 @@
       <c r="C4" s="5">
         <v>28225.81</v>
       </c>
-      <c r="D4" s="96"/>
+      <c r="D4" s="133"/>
     </row>
     <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100">
+      <c r="A5" s="99">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -3866,10 +3986,10 @@
       <c r="C5" s="5">
         <v>55000</v>
       </c>
-      <c r="D5" s="96"/>
+      <c r="D5" s="133"/>
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100">
+      <c r="A6" s="99">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
@@ -3879,22 +3999,24 @@
         <f>(35000/31)*3</f>
         <v>3387.0967741935483</v>
       </c>
-      <c r="D6" s="96"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100">
+      <c r="A7" s="136">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="138">
         <v>35000</v>
       </c>
-      <c r="D7" s="96"/>
+      <c r="D7" s="139" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100">
+      <c r="A8" s="131">
         <v>6</v>
       </c>
       <c r="B8" s="89" t="s">
@@ -3903,12 +4025,12 @@
       <c r="C8" s="9">
         <v>49755</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="134" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100">
+      <c r="A9" s="99">
         <v>7</v>
       </c>
       <c r="B9" s="40" t="s">
@@ -3917,22 +4039,24 @@
       <c r="C9" s="5">
         <v>80000</v>
       </c>
-      <c r="D9" s="96"/>
+      <c r="D9" s="133"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100">
+      <c r="A10" s="136">
         <v>8</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="138">
         <v>69612.899999999994</v>
       </c>
-      <c r="D10" s="96"/>
+      <c r="D10" s="139" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101">
+      <c r="A11" s="100">
         <v>9</v>
       </c>
       <c r="B11" s="86" t="s">
@@ -3941,10 +4065,10 @@
       <c r="C11" s="91">
         <v>30000</v>
       </c>
-      <c r="D11" s="96"/>
+      <c r="D11" s="133"/>
     </row>
     <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100">
+      <c r="A12" s="99">
         <v>10</v>
       </c>
       <c r="B12" s="56" t="s">
@@ -3953,34 +4077,38 @@
       <c r="C12" s="92">
         <v>27000</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="133"/>
     </row>
     <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100">
+      <c r="A13" s="136">
         <v>11</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="93">
+      <c r="C13" s="141">
         <v>24322.58</v>
       </c>
-      <c r="D13" s="96"/>
+      <c r="D13" s="139" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100">
+      <c r="A14" s="131">
         <v>12</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="93">
+      <c r="C14" s="25">
         <v>50000</v>
       </c>
-      <c r="D14" s="96"/>
+      <c r="D14" s="134">
+        <v>1307</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99">
+      <c r="A15" s="98">
         <v>13</v>
       </c>
       <c r="B15" s="87" t="s">
@@ -3989,104 +4117,408 @@
       <c r="C15" s="93">
         <v>15000</v>
       </c>
-      <c r="D15" s="96"/>
+      <c r="D15" s="133"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="102">
+      <c r="A16" s="142">
         <v>14</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="93">
+      <c r="C16" s="141">
         <v>9000</v>
       </c>
-      <c r="D16" s="96"/>
+      <c r="D16" s="139" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100">
+      <c r="A17" s="136">
         <v>15</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="93">
+      <c r="C17" s="141">
         <v>14000</v>
       </c>
-      <c r="D17" s="96"/>
+      <c r="D17" s="139" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100">
+      <c r="A18" s="136">
         <v>16</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="140" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="93">
+      <c r="C18" s="141">
         <v>23000</v>
       </c>
-      <c r="D18" s="96"/>
+      <c r="D18" s="139" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100">
+      <c r="A19" s="136">
         <v>17</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="140" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="93">
+      <c r="C19" s="141">
         <v>17000</v>
       </c>
-      <c r="D19" s="96"/>
+      <c r="D19" s="139" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100">
+      <c r="A20" s="131">
         <v>18</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="93">
+      <c r="C20" s="25">
         <v>39000</v>
       </c>
-      <c r="D20" s="96"/>
+      <c r="D20" s="134">
+        <v>918</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100">
+      <c r="A21" s="132">
         <v>19</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="93">
+      <c r="C21" s="25">
         <v>20000</v>
       </c>
-      <c r="D21" s="96"/>
+      <c r="D21" s="134">
+        <v>474</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="87"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="96"/>
-    </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="96"/>
-    </row>
-    <row r="24" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="21" t="s">
+      <c r="A22" s="122"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="135"/>
+    </row>
+    <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="125" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="126"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="127"/>
+    </row>
+    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="78">
+        <v>76525.679999999993</v>
+      </c>
+      <c r="D24" s="79"/>
+    </row>
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="78">
+        <v>27100</v>
+      </c>
+      <c r="D25" s="79"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="78">
+        <v>191666</v>
+      </c>
+      <c r="D26" s="79"/>
+    </row>
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="78">
+        <v>29742</v>
+      </c>
+      <c r="D27" s="79"/>
+    </row>
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="78">
+        <v>115000</v>
+      </c>
+      <c r="D28" s="79"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="78">
+        <v>12612.9</v>
+      </c>
+      <c r="D29" s="79"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="88">
+        <v>209620</v>
+      </c>
+      <c r="D30" s="78"/>
+    </row>
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="78">
+        <v>204142.89</v>
+      </c>
+      <c r="D31" s="79"/>
+    </row>
+    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="88">
+        <v>168000</v>
+      </c>
+      <c r="D32" s="78"/>
+    </row>
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="78">
+        <v>141000</v>
+      </c>
+      <c r="D33" s="79"/>
+    </row>
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="78">
+        <v>77000</v>
+      </c>
+      <c r="D34" s="79"/>
+    </row>
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="78">
+        <v>341000</v>
+      </c>
+      <c r="D35" s="79"/>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="81">
+        <v>514388</v>
+      </c>
+      <c r="D36" s="79"/>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="81">
+        <v>42300</v>
+      </c>
+      <c r="D37" s="79"/>
+    </row>
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="81">
+        <v>33291.910000000003</v>
+      </c>
+      <c r="D38" s="79"/>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="78">
+        <v>30000</v>
+      </c>
+      <c r="D39" s="79"/>
+    </row>
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="78">
+        <v>0</v>
+      </c>
+      <c r="D40" s="79"/>
+    </row>
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="78">
+        <v>23000</v>
+      </c>
+      <c r="D41" s="79"/>
+    </row>
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="78">
+        <v>18000</v>
+      </c>
+      <c r="D42" s="79"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="78">
+        <v>12000</v>
+      </c>
+      <c r="D43" s="79"/>
+    </row>
+    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A44" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="128" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="129">
+        <v>13033.33</v>
+      </c>
+      <c r="D44" s="130" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="76"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="79"/>
+    </row>
+    <row r="46" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A46" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="22">
-        <f>SUM(C3:C23)</f>
+      <c r="B46" s="116"/>
+      <c r="C46" s="82">
+        <f>SUM(C3:C22)+SUM(C24:C45)</f>
+        <v>2923161.5767741939</v>
+      </c>
+      <c r="D46" s="79"/>
+    </row>
+    <row r="47" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A47" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="118"/>
+      <c r="C47" s="65">
+        <f>SUM(C3:C21)</f>
         <v>643738.86677419348</v>
       </c>
-      <c r="D24" s="98"/>
+      <c r="D47" s="79"/>
+    </row>
+    <row r="48" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A48" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="113"/>
+      <c r="C48" s="83">
+        <f>SUM(C24:C45)</f>
+        <v>2279422.7100000004</v>
+      </c>
+      <c r="D48" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4099,7 +4531,7 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4110,11 +4542,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="122"/>
-      <c r="D1" s="123"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="121"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -4128,7 +4560,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100">
+      <c r="A3" s="99">
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -4140,7 +4572,7 @@
       <c r="D3" s="96"/>
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="100">
+      <c r="A4" s="99">
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -4152,7 +4584,7 @@
       <c r="D4" s="96"/>
     </row>
     <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100">
+      <c r="A5" s="99">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -4164,7 +4596,7 @@
       <c r="D5" s="96"/>
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100">
+      <c r="A6" s="99">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
@@ -4176,7 +4608,7 @@
       <c r="D6" s="96"/>
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100">
+      <c r="A7" s="99">
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -4188,7 +4620,7 @@
       <c r="D7" s="96"/>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100">
+      <c r="A8" s="99">
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
@@ -4200,7 +4632,7 @@
       <c r="D8" s="96"/>
     </row>
     <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100">
+      <c r="A9" s="99">
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
@@ -4212,7 +4644,7 @@
       <c r="D9" s="96"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100">
+      <c r="A10" s="99">
         <v>8</v>
       </c>
       <c r="B10" s="40" t="s">
@@ -4221,10 +4653,10 @@
       <c r="C10" s="5">
         <v>49755</v>
       </c>
-      <c r="D10" s="103"/>
+      <c r="D10" s="101"/>
     </row>
     <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100">
+      <c r="A11" s="99">
         <v>9</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -4236,7 +4668,7 @@
       <c r="D11" s="96"/>
     </row>
     <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100">
+      <c r="A12" s="99">
         <v>10</v>
       </c>
       <c r="B12" s="40" t="s">
@@ -4248,7 +4680,7 @@
       <c r="D12" s="96"/>
     </row>
     <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100">
+      <c r="A13" s="99">
         <v>11</v>
       </c>
       <c r="B13" s="86" t="s">
@@ -4260,7 +4692,7 @@
       <c r="D13" s="96"/>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100">
+      <c r="A14" s="99">
         <v>12</v>
       </c>
       <c r="B14" s="56" t="s">
@@ -4272,7 +4704,7 @@
       <c r="D14" s="96"/>
     </row>
     <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100">
+      <c r="A15" s="99">
         <v>13</v>
       </c>
       <c r="B15" s="87" t="s">
@@ -4284,7 +4716,7 @@
       <c r="D15" s="96"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100">
+      <c r="A16" s="99">
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
@@ -4296,7 +4728,7 @@
       <c r="D16" s="96"/>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100">
+      <c r="A17" s="99">
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
@@ -4308,7 +4740,7 @@
       <c r="D17" s="96"/>
     </row>
     <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100">
+      <c r="A18" s="99">
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
@@ -4320,7 +4752,7 @@
       <c r="D18" s="96"/>
     </row>
     <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100">
+      <c r="A19" s="99">
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
@@ -4332,7 +4764,7 @@
       <c r="D19" s="96"/>
     </row>
     <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100">
+      <c r="A20" s="99">
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
@@ -4344,7 +4776,7 @@
       <c r="D20" s="96"/>
     </row>
     <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100">
+      <c r="A21" s="99">
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
@@ -4356,7 +4788,7 @@
       <c r="D21" s="96"/>
     </row>
     <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100">
+      <c r="A22" s="99">
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
@@ -4368,7 +4800,7 @@
       <c r="D22" s="96"/>
     </row>
     <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100">
+      <c r="A23" s="99">
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
@@ -4380,7 +4812,7 @@
       <c r="D23" s="96"/>
     </row>
     <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100">
+      <c r="A24" s="99">
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
@@ -4410,7 +4842,7 @@
         <f>SUM(C3:C26)</f>
         <v>1274178.6533333331</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
FBS JUNHO PRORPORCIONAL FRANCISCO MORATO
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64183AA1-8F7A-4E4C-870C-514BEE21C4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A608218D-D657-DD4F-9EC4-866FB0287307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="144">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -465,6 +465,18 @@
   </si>
   <si>
     <t>FICHA</t>
+  </si>
+  <si>
+    <t>PAGO</t>
+  </si>
+  <si>
+    <t>ATRASADOS PAGOS</t>
+  </si>
+  <si>
+    <t>TOTAL PAGO</t>
+  </si>
+  <si>
+    <t>FBS FRANCISCO MORATO - ROLO(17/06) + PATROL(18/06) + 2 MOB</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,14 +664,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="37">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1105,13 +1111,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1286,83 +1363,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1391,6 +1394,106 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1728,10 +1831,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="103"/>
+      <c r="B1" s="118"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
@@ -2030,10 +2133,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="103"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2166,7 +2269,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="110">
+      <c r="A11" s="119">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2175,20 +2278,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="120" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
+      <c r="A12" s="119"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="105"/>
+      <c r="D12" s="121"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2220,7 +2323,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="110">
+      <c r="A15" s="119">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2229,31 +2332,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="120" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="110"/>
+      <c r="A16" s="119"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="106"/>
+      <c r="D16" s="122"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="110"/>
+      <c r="A17" s="119"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="105"/>
+      <c r="D17" s="121"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2287,7 +2390,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="110">
+      <c r="A20" s="119">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2296,20 +2399,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="120" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="110"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="105"/>
+      <c r="D21" s="121"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2410,11 +2513,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="107"/>
+      <c r="D28" s="123"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="110">
+      <c r="A29" s="119">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2423,40 +2526,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="108"/>
+      <c r="D29" s="124"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="110"/>
+      <c r="A30" s="119"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="108"/>
+      <c r="D30" s="124"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="110"/>
+      <c r="A31" s="119"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="108"/>
+      <c r="D31" s="124"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="110"/>
+      <c r="A32" s="119"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="109"/>
+      <c r="D32" s="125"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2472,6 +2575,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2480,7 +2584,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2501,8 +2604,8 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:C44"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2514,10 +2617,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="103"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2617,7 +2720,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="111">
+      <c r="A11" s="126">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2628,7 +2731,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2648,7 +2751,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="111">
+      <c r="A14" s="126">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2659,7 +2762,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2668,7 +2771,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="111"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2677,7 +2780,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2686,7 +2789,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="111"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2717,7 +2820,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="111">
+      <c r="A21" s="126">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2728,7 +2831,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="111"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2825,7 +2928,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111">
+      <c r="A31" s="126">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2836,7 +2939,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="111"/>
+      <c r="A32" s="126"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -2845,7 +2948,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111"/>
+      <c r="A33" s="126"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -2974,8 +3077,8 @@
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2986,10 +3089,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="103"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3088,7 +3191,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="111">
+      <c r="A11" s="126">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3099,7 +3202,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3119,7 +3222,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="111">
+      <c r="A14" s="126">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3130,7 +3233,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3139,7 +3242,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3148,7 +3251,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3157,7 +3260,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="111"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3188,7 +3291,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="111">
+      <c r="A21" s="126">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3199,7 +3302,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="111"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3296,7 +3399,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111">
+      <c r="A31" s="126">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3307,7 +3410,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="111"/>
+      <c r="A32" s="126"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3316,7 +3419,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111"/>
+      <c r="A33" s="126"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3380,8 +3483,8 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D27"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -3392,18 +3495,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
     </row>
     <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="114"/>
+      <c r="B2" s="129"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -3865,10 +3968,10 @@
       <c r="D40" s="79"/>
     </row>
     <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="115" t="s">
+      <c r="A41" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="116"/>
+      <c r="B41" s="131"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
@@ -3876,10 +3979,10 @@
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="117" t="s">
+      <c r="A42" s="132" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="118"/>
+      <c r="B42" s="133"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
@@ -3887,10 +3990,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="127" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="113"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
@@ -3921,10 +4024,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3935,11 +4038,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="121"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="136"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3962,7 +4065,7 @@
       <c r="C3" s="5">
         <v>54435.48</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="107"/>
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="99">
@@ -3974,7 +4077,7 @@
       <c r="C4" s="5">
         <v>28225.81</v>
       </c>
-      <c r="D4" s="133"/>
+      <c r="D4" s="107"/>
     </row>
     <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="99">
@@ -3986,7 +4089,7 @@
       <c r="C5" s="5">
         <v>55000</v>
       </c>
-      <c r="D5" s="133"/>
+      <c r="D5" s="107"/>
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="99">
@@ -3999,24 +4102,24 @@
         <f>(35000/31)*3</f>
         <v>3387.0967741935483</v>
       </c>
-      <c r="D6" s="133"/>
+      <c r="D6" s="107"/>
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136">
+      <c r="A7" s="110">
         <v>5</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="138">
+      <c r="C7" s="112">
         <v>35000</v>
       </c>
-      <c r="D7" s="139" t="s">
+      <c r="D7" s="113" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="131">
+      <c r="A8" s="105">
         <v>6</v>
       </c>
       <c r="B8" s="89" t="s">
@@ -4025,7 +4128,7 @@
       <c r="C8" s="9">
         <v>49755</v>
       </c>
-      <c r="D8" s="134" t="s">
+      <c r="D8" s="108" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4039,19 +4142,19 @@
       <c r="C9" s="5">
         <v>80000</v>
       </c>
-      <c r="D9" s="133"/>
+      <c r="D9" s="107"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="136">
+      <c r="A10" s="110">
         <v>8</v>
       </c>
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="138">
+      <c r="C10" s="112">
         <v>69612.899999999994</v>
       </c>
-      <c r="D10" s="139" t="s">
+      <c r="D10" s="113" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4065,7 +4168,7 @@
       <c r="C11" s="91">
         <v>30000</v>
       </c>
-      <c r="D11" s="133"/>
+      <c r="D11" s="107"/>
     </row>
     <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="99">
@@ -4077,24 +4180,24 @@
       <c r="C12" s="92">
         <v>27000</v>
       </c>
-      <c r="D12" s="133"/>
+      <c r="D12" s="107"/>
     </row>
     <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="136">
+      <c r="A13" s="110">
         <v>11</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="141">
+      <c r="C13" s="115">
         <v>24322.58</v>
       </c>
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="113" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131">
+      <c r="A14" s="105">
         <v>12</v>
       </c>
       <c r="B14" s="59" t="s">
@@ -4103,7 +4206,7 @@
       <c r="C14" s="25">
         <v>50000</v>
       </c>
-      <c r="D14" s="134">
+      <c r="D14" s="108">
         <v>1307</v>
       </c>
     </row>
@@ -4117,66 +4220,66 @@
       <c r="C15" s="93">
         <v>15000</v>
       </c>
-      <c r="D15" s="133"/>
+      <c r="D15" s="107"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="142">
+      <c r="A16" s="116">
         <v>14</v>
       </c>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="141">
+      <c r="C16" s="115">
         <v>9000</v>
       </c>
-      <c r="D16" s="139" t="s">
+      <c r="D16" s="113" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136">
+      <c r="A17" s="110">
         <v>15</v>
       </c>
-      <c r="B17" s="140" t="s">
+      <c r="B17" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="141">
+      <c r="C17" s="115">
         <v>14000</v>
       </c>
-      <c r="D17" s="139" t="s">
+      <c r="D17" s="113" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136">
+      <c r="A18" s="110">
         <v>16</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="114" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="141">
+      <c r="C18" s="115">
         <v>23000</v>
       </c>
-      <c r="D18" s="139" t="s">
+      <c r="D18" s="113" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136">
+      <c r="A19" s="110">
         <v>17</v>
       </c>
-      <c r="B19" s="140" t="s">
+      <c r="B19" s="114" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="141">
+      <c r="C19" s="115">
         <v>17000</v>
       </c>
-      <c r="D19" s="139" t="s">
+      <c r="D19" s="113" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131">
+      <c r="A20" s="105">
         <v>18</v>
       </c>
       <c r="B20" s="59" t="s">
@@ -4185,12 +4288,12 @@
       <c r="C20" s="25">
         <v>39000</v>
       </c>
-      <c r="D20" s="134">
+      <c r="D20" s="108">
         <v>918</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="132">
+      <c r="A21" s="106">
         <v>19</v>
       </c>
       <c r="B21" s="59" t="s">
@@ -4199,23 +4302,23 @@
       <c r="C21" s="25">
         <v>20000</v>
       </c>
-      <c r="D21" s="134">
+      <c r="D21" s="108">
         <v>474</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="122"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="135"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="109"/>
     </row>
     <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="125" t="s">
+      <c r="A23" s="137" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="126"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="127"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="139"/>
     </row>
     <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -4234,10 +4337,10 @@
         <v>135</v>
       </c>
       <c r="B25" s="77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" s="78">
-        <v>27100</v>
+        <v>191666</v>
       </c>
       <c r="D25" s="79"/>
     </row>
@@ -4246,10 +4349,10 @@
         <v>135</v>
       </c>
       <c r="B26" s="77" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C26" s="78">
-        <v>191666</v>
+        <v>29742</v>
       </c>
       <c r="D26" s="79"/>
     </row>
@@ -4258,10 +4361,10 @@
         <v>135</v>
       </c>
       <c r="B27" s="77" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C27" s="78">
-        <v>29742</v>
+        <v>115000</v>
       </c>
       <c r="D27" s="79"/>
     </row>
@@ -4270,22 +4373,22 @@
         <v>135</v>
       </c>
       <c r="B28" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="78">
-        <v>115000</v>
-      </c>
-      <c r="D28" s="79"/>
+        <v>120</v>
+      </c>
+      <c r="C28" s="88">
+        <v>209620</v>
+      </c>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>135</v>
       </c>
       <c r="B29" s="77" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C29" s="78">
-        <v>12612.9</v>
+        <v>223642.86</v>
       </c>
       <c r="D29" s="79"/>
     </row>
@@ -4294,10 +4397,10 @@
         <v>135</v>
       </c>
       <c r="B30" s="77" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C30" s="88">
-        <v>209620</v>
+        <v>168000</v>
       </c>
       <c r="D30" s="78"/>
     </row>
@@ -4306,10 +4409,10 @@
         <v>135</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C31" s="78">
-        <v>204142.89</v>
+        <v>141000</v>
       </c>
       <c r="D31" s="79"/>
     </row>
@@ -4318,34 +4421,34 @@
         <v>135</v>
       </c>
       <c r="B32" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="88">
-        <v>168000</v>
-      </c>
-      <c r="D32" s="78"/>
+        <v>116</v>
+      </c>
+      <c r="C32" s="78">
+        <v>77000</v>
+      </c>
+      <c r="D32" s="79"/>
     </row>
     <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="76" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B33" s="77" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="C33" s="78">
-        <v>141000</v>
+        <v>341000</v>
       </c>
       <c r="D33" s="79"/>
     </row>
     <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="78">
-        <v>77000</v>
+        <v>137</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="81">
+        <v>514388</v>
       </c>
       <c r="D34" s="79"/>
     </row>
@@ -4353,11 +4456,11 @@
       <c r="A35" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="78">
-        <v>341000</v>
+      <c r="B35" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="81">
+        <v>42300</v>
       </c>
       <c r="D35" s="79"/>
     </row>
@@ -4366,10 +4469,10 @@
         <v>137</v>
       </c>
       <c r="B36" s="80" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C36" s="81">
-        <v>514388</v>
+        <v>33291.910000000003</v>
       </c>
       <c r="D36" s="79"/>
     </row>
@@ -4377,11 +4480,11 @@
       <c r="A37" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="81">
-        <v>42300</v>
+      <c r="B37" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="78">
+        <v>30000</v>
       </c>
       <c r="D37" s="79"/>
     </row>
@@ -4389,11 +4492,11 @@
       <c r="A38" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="80" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="81">
-        <v>33291.910000000003</v>
+      <c r="B38" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="78">
+        <v>0</v>
       </c>
       <c r="D38" s="79"/>
     </row>
@@ -4402,10 +4505,10 @@
         <v>137</v>
       </c>
       <c r="B39" s="77" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="C39" s="78">
-        <v>30000</v>
+        <v>18000</v>
       </c>
       <c r="D39" s="79"/>
     </row>
@@ -4414,10 +4517,10 @@
         <v>137</v>
       </c>
       <c r="B40" s="77" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C40" s="78">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="D40" s="79"/>
     </row>
@@ -4425,102 +4528,137 @@
       <c r="A41" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="78">
-        <v>23000</v>
-      </c>
-      <c r="D41" s="79"/>
+      <c r="B41" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="140">
+        <v>13033.33</v>
+      </c>
+      <c r="D41" s="141" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="78">
-        <v>18000</v>
-      </c>
+      <c r="A42" s="76"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43" s="77" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="78">
-        <v>12000</v>
+    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="130" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="131"/>
+      <c r="C43" s="82">
+        <f>SUM(C3:C22)+SUM(C24:C42)</f>
+        <v>2879948.6467741937</v>
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A44" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="B44" s="128" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="129">
-        <v>13033.33</v>
-      </c>
-      <c r="D44" s="130" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
-      <c r="B45" s="77"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="79"/>
-    </row>
-    <row r="46" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A46" s="115" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="82">
-        <f>SUM(C3:C22)+SUM(C24:C45)</f>
-        <v>2923161.5767741939</v>
-      </c>
-      <c r="D46" s="79"/>
-    </row>
-    <row r="47" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A47" s="117" t="s">
+    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A44" s="132" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="118"/>
-      <c r="C47" s="65">
+      <c r="B44" s="133"/>
+      <c r="C44" s="65">
         <f>SUM(C3:C21)</f>
         <v>643738.86677419348</v>
       </c>
-      <c r="D47" s="79"/>
-    </row>
-    <row r="48" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A48" s="112" t="s">
+      <c r="D44" s="79"/>
+    </row>
+    <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="127" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="113"/>
-      <c r="C48" s="83">
-        <f>SUM(C24:C45)</f>
-        <v>2279422.7100000004</v>
-      </c>
-      <c r="D48" s="79"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="83">
+        <f>SUM(C24:C42)</f>
+        <v>2236209.7800000003</v>
+      </c>
+      <c r="D45" s="79"/>
+    </row>
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="137"/>
+      <c r="B46" s="138"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="139"/>
+    </row>
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="137" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="138"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="139"/>
+    </row>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="142" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="74">
+        <v>12000</v>
+      </c>
+      <c r="D48" s="143" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="142" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="74">
+        <v>12612.9</v>
+      </c>
+      <c r="D49" s="143" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="144" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="145" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="146">
+        <v>23000</v>
+      </c>
+      <c r="D50" s="147" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="148" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="149"/>
+      <c r="C51" s="150">
+        <f>SUM(C48:C50)</f>
+        <v>47612.9</v>
+      </c>
+      <c r="D51" s="151"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4529,10 +4667,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4542,11 +4680,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="121"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="136"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -4683,11 +4821,12 @@
       <c r="A13" s="99">
         <v>11</v>
       </c>
-      <c r="B13" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="91">
-        <v>30000</v>
+      <c r="B13" s="152" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="104">
+        <f>((16500/30)*14) + ((36000/30)*13) + 5000</f>
+        <v>28300</v>
       </c>
       <c r="D13" s="96"/>
     </row>
@@ -4695,11 +4834,11 @@
       <c r="A14" s="99">
         <v>12</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="92">
-        <v>27000</v>
+      <c r="B14" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="91">
+        <v>30000</v>
       </c>
       <c r="D14" s="96"/>
     </row>
@@ -4707,11 +4846,11 @@
       <c r="A15" s="99">
         <v>13</v>
       </c>
-      <c r="B15" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="93">
-        <v>26000</v>
+      <c r="B15" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="92">
+        <v>27000</v>
       </c>
       <c r="D15" s="96"/>
     </row>
@@ -4720,10 +4859,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="93">
-        <v>50000</v>
+        <v>26000</v>
       </c>
       <c r="D16" s="96"/>
     </row>
@@ -4732,10 +4871,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C17" s="93">
-        <v>15000</v>
+        <v>50000</v>
       </c>
       <c r="D17" s="96"/>
     </row>
@@ -4744,10 +4883,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C18" s="93">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="D18" s="96"/>
     </row>
@@ -4756,10 +4895,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="93">
-        <v>14000</v>
+        <v>9000</v>
       </c>
       <c r="D19" s="96"/>
     </row>
@@ -4768,10 +4907,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="C20" s="93">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="D20" s="96"/>
     </row>
@@ -4780,10 +4919,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="93">
-        <v>17000</v>
+        <v>23000</v>
       </c>
       <c r="D21" s="96"/>
     </row>
@@ -4792,10 +4931,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C22" s="93">
-        <v>39000</v>
+        <v>17000</v>
       </c>
       <c r="D22" s="96"/>
     </row>
@@ -4804,10 +4943,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C23" s="93">
-        <v>20000</v>
+        <v>39000</v>
       </c>
       <c r="D23" s="96"/>
     </row>
@@ -4816,33 +4955,45 @@
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="93">
+        <v>20000</v>
+      </c>
+      <c r="D24" s="96"/>
+    </row>
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="99">
+        <v>23</v>
+      </c>
+      <c r="B25" s="87" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="93">
+      <c r="C25" s="93">
         <f>(17000/30)* 23</f>
         <v>13033.333333333332</v>
       </c>
-      <c r="D24" s="96"/>
-    </row>
-    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="87"/>
-      <c r="C25" s="93"/>
       <c r="D25" s="96"/>
     </row>
     <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="87"/>
-      <c r="C26" s="94"/>
+      <c r="C26" s="93"/>
       <c r="D26" s="96"/>
     </row>
-    <row r="27" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="21" t="s">
+    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="87"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="96"/>
+    </row>
+    <row r="28" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="22">
-        <f>SUM(C3:C26)</f>
-        <v>1274178.6533333331</v>
-      </c>
-      <c r="D27" s="97"/>
+      <c r="C28" s="22">
+        <f>SUM(C3:C27)</f>
+        <v>1302478.6533333331</v>
+      </c>
+      <c r="D28" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
PRO GOLF ROLO DIA 21 ATE 30
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/BRYAN MEDIÇÕES - PROJEÇÕES/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A608218D-D657-DD4F-9EC4-866FB0287307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F42C221-271D-4446-97B4-E3F8EC067E4A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCB68F5-F821-F144-AE9E-1358FFF113CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -487,9 +487,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
@@ -1188,7 +1188,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="153">
@@ -1218,11 +1218,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1264,7 +1264,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1275,7 +1275,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1284,7 +1284,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1295,7 +1295,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1328,10 +1328,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1350,7 +1350,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1422,27 +1422,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1482,10 +1482,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1827,19 +1827,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="127"/>
     </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -1993,11 +1993,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -2093,11 +2093,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -2126,22 +2126,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="68.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="127"/>
     </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2271,8 +2271,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="128">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="134">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2281,23 +2281,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="129" t="s">
+      <c r="D11" s="128" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="128"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="134"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="130"/>
+      <c r="D12" s="129"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2325,8 +2325,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="128">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="134">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2335,34 +2335,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="129" t="s">
+      <c r="D15" s="128" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="128"/>
+    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="134"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="131"/>
+      <c r="D16" s="130"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="128"/>
+    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="134"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="130"/>
+      <c r="D17" s="129"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -2392,8 +2392,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="128">
+    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="134">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2402,23 +2402,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="129" t="s">
+      <c r="D20" s="128" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="128"/>
+    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="134"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="130"/>
+      <c r="D21" s="129"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2476,7 +2476,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2516,11 +2516,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="132"/>
+      <c r="D28" s="131"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="128">
+    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="134">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2529,43 +2529,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="133"/>
+      <c r="D29" s="132"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="128"/>
+    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="134"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="133"/>
+      <c r="D30" s="132"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="128"/>
+    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="134"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="133"/>
+      <c r="D31" s="132"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="128"/>
+    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="134"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="134"/>
+      <c r="D32" s="133"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2578,15 +2578,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2611,21 +2611,21 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="126" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="127"/>
     </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="135">
         <v>9</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="135"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -2742,7 +2742,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="135">
         <v>12</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="135"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -2773,7 +2773,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="135"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -2782,7 +2782,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="135"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
@@ -2791,7 +2791,7 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="135"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
@@ -2800,7 +2800,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="135">
         <v>15</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="135"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
@@ -2842,7 +2842,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="135">
         <v>24</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="135"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
@@ -2950,7 +2950,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="135"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
@@ -2959,7 +2959,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -3084,20 +3084,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="127"/>
     </row>
-    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="135">
         <v>9</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="135"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -3213,7 +3213,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="135">
         <v>12</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="135"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -3244,7 +3244,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="135"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -3253,7 +3253,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="135"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
@@ -3262,7 +3262,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="135"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
@@ -3271,7 +3271,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="135">
         <v>15</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="135"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
@@ -3313,7 +3313,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="135">
         <v>24</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="135"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
@@ -3421,7 +3421,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="135"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
@@ -3430,7 +3430,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3452,11 +3452,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3490,14 +3490,14 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="13" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="C1" s="138"/>
       <c r="D1" s="138"/>
     </row>
-    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="138" t="s">
         <v>89</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="68">
         <v>2</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="D5" s="75"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="D6" s="79"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="76">
         <v>5</v>
       </c>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="D7" s="79"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="68">
         <v>6</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="76">
         <v>7</v>
       </c>
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="68">
         <v>8</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="68">
         <v>9</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="68">
         <v>10</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="D13" s="75"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="76">
         <v>12</v>
       </c>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>13</v>
       </c>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="68">
         <v>14</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="D17" s="75"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="68">
         <v>17</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="76">
         <v>20</v>
       </c>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="76">
         <v>21</v>
       </c>
@@ -3787,7 +3787,7 @@
       </c>
       <c r="D23" s="79"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="76">
         <v>22</v>
       </c>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="76">
         <v>23</v>
       </c>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="68">
         <v>24</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="76">
         <v>25</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
       <c r="B28" s="79" t="s">
         <v>81</v>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>99</v>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>84</v>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="D30" s="79"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>85</v>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>117</v>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="76"/>
       <c r="B33" s="77" t="s">
         <v>87</v>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="76"/>
       <c r="B34" s="77" t="s">
         <v>119</v>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="68"/>
       <c r="B35" s="69" t="s">
         <v>26</v>
@@ -3919,7 +3919,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
         <v>120</v>
@@ -3930,7 +3930,7 @@
       <c r="D36" s="78"/>
       <c r="E36" s="79"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
         <v>121</v>
@@ -3940,7 +3940,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="76"/>
       <c r="B38" s="77" t="s">
         <v>115</v>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="D38" s="78"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="76"/>
       <c r="B39" s="77" t="s">
         <v>118</v>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="76"/>
       <c r="B40" s="77" t="s">
         <v>116</v>
@@ -3970,7 +3970,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A41" s="139" t="s">
         <v>35</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A42" s="141" t="s">
         <v>96</v>
       </c>
@@ -3992,7 +3992,7 @@
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="136" t="s">
         <v>97</v>
       </c>
@@ -4003,10 +4003,10 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="66"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="66"/>
     </row>
   </sheetData>
@@ -4029,25 +4029,25 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="76.625" customWidth="1"/>
-    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="150" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="151"/>
       <c r="D1" s="152"/>
     </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>106</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="105">
         <v>1</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105">
         <v>2</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="99">
         <v>3</v>
       </c>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D5" s="107"/>
     </row>
-    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="99">
         <v>4</v>
       </c>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="D6" s="107"/>
     </row>
-    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="110">
         <v>5</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="105">
         <v>6</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="99">
         <v>7</v>
       </c>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="D9" s="107"/>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="110">
         <v>8</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100">
         <v>9</v>
       </c>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="D11" s="107"/>
     </row>
-    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="99">
         <v>10</v>
       </c>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="D12" s="107"/>
     </row>
-    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="110">
         <v>11</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="105">
         <v>12</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="98">
         <v>13</v>
       </c>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="D15" s="107"/>
     </row>
-    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="116">
         <v>14</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="110">
         <v>15</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="110">
         <v>16</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="110">
         <v>17</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="105">
         <v>18</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="106">
         <v>19</v>
       </c>
@@ -4313,13 +4313,13 @@
         <v>474</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="102"/>
       <c r="B22" s="103"/>
       <c r="C22" s="104"/>
       <c r="D22" s="109"/>
     </row>
-    <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="143" t="s">
         <v>134</v>
       </c>
@@ -4327,7 +4327,7 @@
       <c r="C23" s="144"/>
       <c r="D23" s="145"/>
     </row>
-    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
         <v>135</v>
       </c>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="76" t="s">
         <v>135</v>
       </c>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="76" t="s">
         <v>135</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="D26" s="79"/>
     </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="76" t="s">
         <v>135</v>
       </c>
@@ -4375,7 +4375,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="76" t="s">
         <v>135</v>
       </c>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="D28" s="78"/>
     </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>135</v>
       </c>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>135</v>
       </c>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>135</v>
       </c>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>135</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="76" t="s">
         <v>137</v>
       </c>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
         <v>137</v>
       </c>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>137</v>
       </c>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="D35" s="79"/>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>137</v>
       </c>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="D36" s="79"/>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="76" t="s">
         <v>137</v>
       </c>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
         <v>137</v>
       </c>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="D38" s="79"/>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="76" t="s">
         <v>137</v>
       </c>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
         <v>137</v>
       </c>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="76" t="s">
         <v>137</v>
       </c>
@@ -4545,13 +4545,13 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="76"/>
       <c r="B42" s="77"/>
       <c r="C42" s="78"/>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="139" t="s">
         <v>35</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A44" s="141" t="s">
         <v>96</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="D44" s="79"/>
     </row>
-    <row r="45" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="136" t="s">
         <v>97</v>
       </c>
@@ -4584,13 +4584,13 @@
       </c>
       <c r="D45" s="79"/>
     </row>
-    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="143"/>
       <c r="B46" s="144"/>
       <c r="C46" s="144"/>
       <c r="D46" s="145"/>
     </row>
-    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="143" t="s">
         <v>141</v>
       </c>
@@ -4598,7 +4598,7 @@
       <c r="C47" s="144"/>
       <c r="D47" s="145"/>
     </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="119" t="s">
         <v>135</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="119" t="s">
         <v>135</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="121" t="s">
         <v>137</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="146" t="s">
         <v>142</v>
       </c>
@@ -4676,24 +4676,24 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="76.625" customWidth="1"/>
-    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B1" s="150" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="151"/>
       <c r="D1" s="152"/>
     </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="99">
         <v>1</v>
       </c>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="D3" s="96"/>
     </row>
-    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="99">
         <v>2</v>
       </c>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="D4" s="96"/>
     </row>
-    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="99">
         <v>3</v>
       </c>
@@ -4736,11 +4736,11 @@
         <v>11</v>
       </c>
       <c r="C5" s="5">
-        <v>324000</v>
+        <v>334000</v>
       </c>
       <c r="D5" s="96"/>
     </row>
-    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="99">
         <v>4</v>
       </c>
@@ -4752,7 +4752,7 @@
       </c>
       <c r="D6" s="96"/>
     </row>
-    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="99">
         <v>5</v>
       </c>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="D7" s="96"/>
     </row>
-    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="99">
         <v>6</v>
       </c>
@@ -4776,7 +4776,7 @@
       </c>
       <c r="D8" s="96"/>
     </row>
-    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="99">
         <v>7</v>
       </c>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="D9" s="96"/>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="99">
         <v>8</v>
       </c>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="D10" s="101"/>
     </row>
-    <row r="11" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99">
         <v>9</v>
       </c>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="D11" s="96"/>
     </row>
-    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="99">
         <v>10</v>
       </c>
@@ -4824,7 +4824,7 @@
       </c>
       <c r="D12" s="96"/>
     </row>
-    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="99">
         <v>11</v>
       </c>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="D13" s="96"/>
     </row>
-    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="99">
         <v>12</v>
       </c>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="D14" s="96"/>
     </row>
-    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="99">
         <v>13</v>
       </c>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="D15" s="96"/>
     </row>
-    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="99">
         <v>14</v>
       </c>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="D16" s="96"/>
     </row>
-    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="99">
         <v>15</v>
       </c>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="D17" s="96"/>
     </row>
-    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="99">
         <v>16</v>
       </c>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="D18" s="96"/>
     </row>
-    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="99">
         <v>17</v>
       </c>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="D19" s="96"/>
     </row>
-    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="99">
         <v>18</v>
       </c>
@@ -4921,7 +4921,7 @@
       </c>
       <c r="D20" s="96"/>
     </row>
-    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="99">
         <v>19</v>
       </c>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="D21" s="96"/>
     </row>
-    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="99">
         <v>20</v>
       </c>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="D22" s="96"/>
     </row>
-    <row r="23" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="99">
         <v>21</v>
       </c>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="D23" s="96"/>
     </row>
-    <row r="24" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="99">
         <v>22</v>
       </c>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="D24" s="96"/>
     </row>
-    <row r="25" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="99">
         <v>23</v>
       </c>
@@ -4982,23 +4982,23 @@
       </c>
       <c r="D25" s="96"/>
     </row>
-    <row r="26" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="87"/>
       <c r="C26" s="93"/>
       <c r="D26" s="96"/>
     </row>
-    <row r="27" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="87"/>
       <c r="C27" s="94"/>
       <c r="D27" s="96"/>
     </row>
-    <row r="28" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="22">
         <f>SUM(C3:C27)</f>
-        <v>1302478.6533333331</v>
+        <v>1312478.6533333331</v>
       </c>
       <c r="D28" s="97"/>
     </row>

</xml_diff>

<commit_message>
ATUALIZACAO DE MAIO E JUNHO
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/BRYAN MEDIÇÕES - PROJEÇÕES/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC586834-44AE-4A4C-B98C-FCB33F1B1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{FC586834-44AE-4A4C-B98C-FCB33F1B1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80332A27-4032-4D8F-BD1B-0B81DEF6C517}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -434,9 +434,6 @@
     <t xml:space="preserve">AVANTE - ROLO DYNAPAC SÉRIE 8547 </t>
   </si>
   <si>
-    <t>JOÃO VICTOR  - PATROL 140 K  SÉRIE 5531 09/05 - 08/06</t>
-  </si>
-  <si>
     <t>ALCANCE - 1º QUINZENA JUNHO DE 2024</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   </si>
   <si>
     <t>FBS FRANCISCO MORATO - ROLO(17/06) + PATROL(18/06) + 4 MOB + 2 ROLO(24/06)</t>
+  </si>
+  <si>
+    <t>JOÃO VICTOR  - PATROL 140 K  SÉRIE 5531 09/06 - 24/06</t>
   </si>
 </sst>
 </file>
@@ -496,9 +496,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -1220,10 +1220,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1250,11 +1250,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,7 +1296,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1307,7 +1307,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1316,7 +1316,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1327,7 +1327,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1360,10 +1360,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,19 +1382,14 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
@@ -1453,7 +1448,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1464,33 +1458,45 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1530,10 +1536,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1545,6 +1551,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1570,6 +1581,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1875,19 +1890,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="135"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1895,7 +1910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1911,7 +1926,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -1919,7 +1934,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +1942,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -1935,7 +1950,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1958,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -1951,7 +1966,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -1960,7 +1975,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -1968,7 +1983,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -1976,7 +1991,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -1984,7 +1999,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +2007,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -2001,7 +2016,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -2009,7 +2024,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -2017,7 +2032,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -2025,7 +2040,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -2033,7 +2048,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -2041,11 +2056,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -2053,7 +2068,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -2061,7 +2076,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -2069,7 +2084,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -2077,7 +2092,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -2085,7 +2100,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -2093,7 +2108,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -2101,7 +2116,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -2109,7 +2124,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -2117,7 +2132,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -2125,7 +2140,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -2133,7 +2148,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -2141,11 +2156,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -2174,22 +2189,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="68.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="68.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="135"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2203,7 +2218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2218,7 +2233,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2233,7 +2248,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2248,7 +2263,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2263,7 +2278,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2278,7 +2293,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2291,7 +2306,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2306,7 +2321,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2319,8 +2334,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="136">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="142">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2329,23 +2344,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="137" t="s">
+      <c r="D11" s="136" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="142"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="138"/>
+      <c r="D12" s="137"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2360,7 +2375,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2373,8 +2388,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="136">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="142">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2383,34 +2398,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="137" t="s">
+      <c r="D15" s="136" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="136"/>
+    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="142"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="139"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
+    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="142"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="138"/>
+      <c r="D17" s="137"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -2425,7 +2440,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -2440,8 +2455,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136">
+    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="142">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2450,23 +2465,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="137" t="s">
+      <c r="D20" s="136" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="136"/>
+    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="142"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="138"/>
+      <c r="D21" s="137"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2481,7 +2496,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2496,7 +2511,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2511,7 +2526,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2524,7 +2539,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2539,7 +2554,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2554,7 +2569,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2564,11 +2579,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="140"/>
+      <c r="D28" s="139"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="136">
+    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="142">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2577,43 +2592,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="141"/>
+      <c r="D29" s="140"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="136"/>
+    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="142"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="141"/>
+      <c r="D30" s="140"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="136"/>
+    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="142"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="141"/>
+      <c r="D31" s="140"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="136"/>
+    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="142"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="142"/>
+      <c r="D32" s="141"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2626,7 +2641,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2635,6 +2649,7 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2659,21 +2674,21 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="134" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="135"/>
     </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2681,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2692,7 +2707,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2703,7 +2718,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2714,7 +2729,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2725,7 +2740,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2737,7 +2752,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2748,7 +2763,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2759,7 +2774,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2770,7 +2785,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="143">
         <v>9</v>
       </c>
@@ -2781,7 +2796,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="143"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -2790,7 +2805,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2801,7 +2816,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="143">
         <v>12</v>
       </c>
@@ -2812,7 +2827,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="143"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -2821,7 +2836,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="143"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -2830,7 +2845,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="143"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
@@ -2839,7 +2854,7 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="143"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
@@ -2848,7 +2863,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2859,7 +2874,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="143">
         <v>15</v>
       </c>
@@ -2881,7 +2896,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="143"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
@@ -2890,7 +2905,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2901,7 +2916,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2912,7 +2927,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2923,7 +2938,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2934,7 +2949,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2945,7 +2960,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2956,7 +2971,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2967,7 +2982,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2978,7 +2993,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="143">
         <v>24</v>
       </c>
@@ -2989,7 +3004,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="143"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
@@ -2998,7 +3013,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="143"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
@@ -3007,7 +3022,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3018,7 +3033,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -3026,7 +3041,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -3034,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -3042,7 +3057,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -3051,7 +3066,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -3059,7 +3074,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -3067,7 +3082,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -3075,7 +3090,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -3083,7 +3098,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -3091,7 +3106,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -3099,7 +3114,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -3132,20 +3147,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="135"/>
     </row>
-    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3153,7 +3168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -3175,7 +3190,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -3186,7 +3201,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -3197,7 +3212,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -3208,7 +3223,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -3219,7 +3234,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -3230,7 +3245,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -3241,7 +3256,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="143">
         <v>9</v>
       </c>
@@ -3252,7 +3267,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="143"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -3261,7 +3276,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -3272,7 +3287,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="143">
         <v>12</v>
       </c>
@@ -3283,7 +3298,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="143"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -3292,7 +3307,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="143"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -3301,7 +3316,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="143"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
@@ -3310,7 +3325,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="143"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
@@ -3319,7 +3334,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -3330,7 +3345,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -3341,7 +3356,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="143">
         <v>15</v>
       </c>
@@ -3352,7 +3367,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="143"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
@@ -3361,7 +3376,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -3372,7 +3387,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -3383,7 +3398,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3394,7 +3409,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3405,7 +3420,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3416,7 +3431,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3427,7 +3442,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3438,7 +3453,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3449,7 +3464,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="143">
         <v>24</v>
       </c>
@@ -3460,7 +3475,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="143"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
@@ -3469,7 +3484,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="143"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
@@ -3478,7 +3493,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3489,7 +3504,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3500,11 +3515,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3538,14 +3553,14 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="13" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
@@ -3553,7 +3568,7 @@
       <c r="C1" s="146"/>
       <c r="D1" s="146"/>
     </row>
-    <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A2" s="146" t="s">
         <v>89</v>
       </c>
@@ -3565,7 +3580,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -3579,7 +3594,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="68">
         <v>2</v>
       </c>
@@ -3593,7 +3608,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -3605,7 +3620,7 @@
       </c>
       <c r="D5" s="75"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -3617,7 +3632,7 @@
       </c>
       <c r="D6" s="79"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="76">
         <v>5</v>
       </c>
@@ -3629,7 +3644,7 @@
       </c>
       <c r="D7" s="79"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="68">
         <v>6</v>
       </c>
@@ -3643,7 +3658,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="76">
         <v>7</v>
       </c>
@@ -3655,7 +3670,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="68">
         <v>8</v>
       </c>
@@ -3669,7 +3684,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="68">
         <v>9</v>
       </c>
@@ -3683,7 +3698,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="68">
         <v>10</v>
       </c>
@@ -3697,7 +3712,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -3709,7 +3724,7 @@
       </c>
       <c r="D13" s="75"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="76">
         <v>12</v>
       </c>
@@ -3721,7 +3736,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="76">
         <v>13</v>
       </c>
@@ -3733,7 +3748,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="68">
         <v>14</v>
       </c>
@@ -3747,7 +3762,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -3759,7 +3774,7 @@
       </c>
       <c r="D17" s="75"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -3773,7 +3788,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="68">
         <v>17</v>
       </c>
@@ -3787,7 +3802,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -3799,7 +3814,7 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -3811,7 +3826,7 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="76">
         <v>20</v>
       </c>
@@ -3823,7 +3838,7 @@
       </c>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="76">
         <v>21</v>
       </c>
@@ -3835,7 +3850,7 @@
       </c>
       <c r="D23" s="79"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="76">
         <v>22</v>
       </c>
@@ -3847,7 +3862,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="76">
         <v>23</v>
       </c>
@@ -3859,7 +3874,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="68">
         <v>24</v>
       </c>
@@ -3873,7 +3888,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="76">
         <v>25</v>
       </c>
@@ -3885,7 +3900,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="76"/>
       <c r="B28" s="79" t="s">
         <v>81</v>
@@ -3895,7 +3910,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>99</v>
@@ -3905,7 +3920,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>84</v>
@@ -3915,7 +3930,7 @@
       </c>
       <c r="D30" s="79"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>85</v>
@@ -3925,7 +3940,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>117</v>
@@ -3935,7 +3950,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="76"/>
       <c r="B33" s="77" t="s">
         <v>87</v>
@@ -3945,7 +3960,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="76"/>
       <c r="B34" s="77" t="s">
         <v>119</v>
@@ -3955,7 +3970,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="68"/>
       <c r="B35" s="69" t="s">
         <v>26</v>
@@ -3967,7 +3982,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
         <v>120</v>
@@ -3978,7 +3993,7 @@
       <c r="D36" s="78"/>
       <c r="E36" s="79"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
         <v>121</v>
@@ -3988,7 +4003,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="76"/>
       <c r="B38" s="77" t="s">
         <v>115</v>
@@ -3998,7 +4013,7 @@
       </c>
       <c r="D38" s="78"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="76"/>
       <c r="B39" s="77" t="s">
         <v>118</v>
@@ -4008,7 +4023,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="76"/>
       <c r="B40" s="77" t="s">
         <v>116</v>
@@ -4018,7 +4033,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A41" s="147" t="s">
         <v>35</v>
       </c>
@@ -4029,7 +4044,7 @@
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A42" s="149" t="s">
         <v>96</v>
       </c>
@@ -4040,7 +4055,7 @@
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A43" s="144" t="s">
         <v>97</v>
       </c>
@@ -4051,10 +4066,10 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C45" s="66"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C47" s="66"/>
     </row>
   </sheetData>
@@ -4077,25 +4092,25 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="158" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="159"/>
       <c r="D1" s="160"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>106</v>
       </c>
@@ -4106,8 +4121,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="104">
+    <row r="3" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="101">
         <v>1</v>
       </c>
       <c r="B3" s="89" t="s">
@@ -4116,12 +4131,12 @@
       <c r="C3" s="9">
         <v>54435.48</v>
       </c>
-      <c r="D3" s="107" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104">
+      <c r="D3" s="104" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="101">
         <v>2</v>
       </c>
       <c r="B4" s="89" t="s">
@@ -4130,12 +4145,12 @@
       <c r="C4" s="9">
         <v>28225.81</v>
       </c>
-      <c r="D4" s="107">
+      <c r="D4" s="104">
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99">
+    <row r="5" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="97">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -4144,10 +4159,10 @@
       <c r="C5" s="5">
         <v>55000</v>
       </c>
-      <c r="D5" s="106"/>
-    </row>
-    <row r="6" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="99">
+      <c r="D5" s="103"/>
+    </row>
+    <row r="6" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
@@ -4157,24 +4172,24 @@
         <f>(35000/31)*3</f>
         <v>3387.0967741935483</v>
       </c>
-      <c r="D6" s="106"/>
-    </row>
-    <row r="7" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="109">
+      <c r="D6" s="103"/>
+    </row>
+    <row r="7" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="106">
         <v>5</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="111">
+      <c r="C7" s="108">
         <v>35000</v>
       </c>
-      <c r="D7" s="112" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="104">
+      <c r="D7" s="109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="101">
         <v>6</v>
       </c>
       <c r="B8" s="89" t="s">
@@ -4183,12 +4198,12 @@
       <c r="C8" s="9">
         <v>49755</v>
       </c>
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="104" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104">
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="101">
         <v>7</v>
       </c>
       <c r="B9" s="89" t="s">
@@ -4197,66 +4212,68 @@
       <c r="C9" s="9">
         <v>57604</v>
       </c>
-      <c r="D9" s="107" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="109">
+      <c r="D9" s="104" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="106">
         <v>8</v>
       </c>
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="111">
+      <c r="C10" s="108">
         <v>69612.899999999994</v>
       </c>
-      <c r="D10" s="112" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100">
+      <c r="D10" s="109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="161">
         <v>9</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="91">
+      <c r="C11" s="163">
         <v>30000</v>
       </c>
-      <c r="D11" s="106"/>
-    </row>
-    <row r="12" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="104">
+      <c r="D11" s="104">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="101">
         <v>10</v>
       </c>
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="125">
+      <c r="C12" s="122">
         <v>27000</v>
       </c>
-      <c r="D12" s="107">
+      <c r="D12" s="104">
         <v>921</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109">
+    <row r="13" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="106">
         <v>11</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="114">
+      <c r="C13" s="111">
         <v>24322.58</v>
       </c>
-      <c r="D13" s="112" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104">
+      <c r="D13" s="109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="101">
         <v>12</v>
       </c>
       <c r="B14" s="59" t="s">
@@ -4265,13 +4282,13 @@
       <c r="C14" s="25">
         <v>50000</v>
       </c>
-      <c r="D14" s="107">
+      <c r="D14" s="104">
         <v>1307</v>
       </c>
-      <c r="E14" s="130"/>
-    </row>
-    <row r="15" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98">
+      <c r="E14" s="126"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="96">
         <v>13</v>
       </c>
       <c r="B15" s="87" t="s">
@@ -4280,66 +4297,66 @@
       <c r="C15" s="93">
         <v>15000</v>
       </c>
-      <c r="D15" s="106"/>
-    </row>
-    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115">
+      <c r="D15" s="103"/>
+    </row>
+    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="112">
         <v>14</v>
       </c>
-      <c r="B16" s="113" t="s">
+      <c r="B16" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="114">
+      <c r="C16" s="111">
         <v>9000</v>
       </c>
-      <c r="D16" s="112" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109">
+      <c r="D16" s="109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="106">
         <v>15</v>
       </c>
-      <c r="B17" s="113" t="s">
+      <c r="B17" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="114">
+      <c r="C17" s="111">
         <v>14000</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="109">
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109">
+    <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="106">
         <v>16</v>
       </c>
-      <c r="B18" s="113" t="s">
+      <c r="B18" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="114">
+      <c r="C18" s="111">
         <v>23000</v>
       </c>
-      <c r="D18" s="112" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109">
+      <c r="D18" s="109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="106">
         <v>17</v>
       </c>
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="114">
+      <c r="C19" s="111">
         <v>17000</v>
       </c>
-      <c r="D19" s="112" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="104">
+      <c r="D19" s="109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="101">
         <v>18</v>
       </c>
       <c r="B20" s="59" t="s">
@@ -4348,12 +4365,12 @@
       <c r="C20" s="25">
         <v>39000</v>
       </c>
-      <c r="D20" s="107">
+      <c r="D20" s="104">
         <v>918</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105">
+    <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="102">
         <v>19</v>
       </c>
       <c r="B21" s="59" t="s">
@@ -4362,27 +4379,27 @@
       <c r="C21" s="25">
         <v>20000</v>
       </c>
-      <c r="D21" s="107">
+      <c r="D21" s="104">
         <v>474</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="101"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="108"/>
-    </row>
-    <row r="23" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="98"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="105"/>
+    </row>
+    <row r="23" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="151" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="152"/>
       <c r="C23" s="152"/>
       <c r="D23" s="153"/>
     </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="77" t="s">
         <v>99</v>
@@ -4392,23 +4409,23 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="126" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" s="127" t="s">
+    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="123" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="128">
+      <c r="C25" s="125">
         <v>191666</v>
       </c>
-      <c r="D25" s="131" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="D25" s="127" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" s="77" t="s">
         <v>117</v>
@@ -4418,21 +4435,23 @@
       </c>
       <c r="D26" s="79"/>
     </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="77" t="s">
+    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="78">
+      <c r="C27" s="70">
         <v>115000</v>
       </c>
-      <c r="D27" s="79"/>
-    </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="D27" s="71">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="77" t="s">
         <v>120</v>
@@ -4442,9 +4461,9 @@
       </c>
       <c r="D28" s="78"/>
     </row>
-    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B29" s="77" t="s">
         <v>121</v>
@@ -4453,11 +4472,11 @@
         <v>223642.86</v>
       </c>
       <c r="D29" s="79"/>
-      <c r="F29" s="130"/>
-    </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="F29" s="126"/>
+    </row>
+    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="77" t="s">
         <v>115</v>
@@ -4467,9 +4486,9 @@
       </c>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B31" s="77" t="s">
         <v>118</v>
@@ -4479,9 +4498,9 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="77" t="s">
         <v>116</v>
@@ -4491,9 +4510,9 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" s="77" t="s">
         <v>51</v>
@@ -4503,9 +4522,9 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="80" t="s">
         <v>11</v>
@@ -4515,9 +4534,9 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35" s="80" t="s">
         <v>79</v>
@@ -4527,9 +4546,9 @@
       </c>
       <c r="D35" s="79"/>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B36" s="69" t="s">
         <v>17</v>
@@ -4541,9 +4560,9 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="69" t="s">
         <v>20</v>
@@ -4555,9 +4574,9 @@
         <v>920</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B38" s="77" t="s">
         <v>100</v>
@@ -4567,9 +4586,9 @@
       </c>
       <c r="D38" s="79"/>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" s="77" t="s">
         <v>94</v>
@@ -4579,9 +4598,9 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" s="69" t="s">
         <v>98</v>
@@ -4593,27 +4612,27 @@
         <v>481</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="116">
+      <c r="C41" s="113">
         <v>13033.33</v>
       </c>
-      <c r="D41" s="117" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="D41" s="114" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="76"/>
       <c r="B42" s="77"/>
       <c r="C42" s="78"/>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A43" s="147" t="s">
         <v>35</v>
       </c>
@@ -4624,7 +4643,7 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A44" s="149" t="s">
         <v>96</v>
       </c>
@@ -4635,7 +4654,7 @@
       </c>
       <c r="D44" s="79"/>
     </row>
-    <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="144" t="s">
         <v>97</v>
       </c>
@@ -4646,23 +4665,23 @@
       </c>
       <c r="D45" s="79"/>
     </row>
-    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="151"/>
       <c r="B46" s="152"/>
       <c r="C46" s="152"/>
       <c r="D46" s="153"/>
     </row>
-    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="151" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="152"/>
       <c r="C47" s="152"/>
       <c r="D47" s="153"/>
     </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A48" s="118" t="s">
-        <v>135</v>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A48" s="115" t="s">
+        <v>134</v>
       </c>
       <c r="B48" s="73" t="s">
         <v>84</v>
@@ -4670,13 +4689,13 @@
       <c r="C48" s="74">
         <v>12000</v>
       </c>
-      <c r="D48" s="119" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="118" t="s">
-        <v>135</v>
+      <c r="D48" s="116" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A49" s="115" t="s">
+        <v>134</v>
       </c>
       <c r="B49" s="73" t="s">
         <v>119</v>
@@ -4684,27 +4703,27 @@
       <c r="C49" s="74">
         <v>12612.9</v>
       </c>
-      <c r="D49" s="119" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="120" t="s">
-        <v>137</v>
-      </c>
-      <c r="B50" s="121" t="s">
+      <c r="D49" s="116" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="117" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="122">
+      <c r="C50" s="119">
         <v>23000</v>
       </c>
-      <c r="D50" s="123" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D50" s="120" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="154" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B51" s="155"/>
       <c r="C51" s="156">
@@ -4738,24 +4757,25 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="158" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="159"/>
       <c r="D1" s="160"/>
     </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
@@ -4766,8 +4786,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="99">
+    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="97">
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -4776,10 +4796,10 @@
       <c r="C3" s="5">
         <v>59951.61</v>
       </c>
-      <c r="D3" s="96"/>
-    </row>
-    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99">
+      <c r="D3" s="130"/>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="97">
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -4788,10 +4808,10 @@
       <c r="C4" s="5">
         <v>28225.81</v>
       </c>
-      <c r="D4" s="96"/>
-    </row>
-    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99">
+      <c r="D4" s="130"/>
+    </row>
+    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="97">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -4800,10 +4820,10 @@
       <c r="C5" s="5">
         <v>334000</v>
       </c>
-      <c r="D5" s="96"/>
-    </row>
-    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="99">
+      <c r="D5" s="130"/>
+    </row>
+    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
@@ -4812,22 +4832,22 @@
       <c r="C6" s="5">
         <v>35000</v>
       </c>
-      <c r="D6" s="96"/>
-    </row>
-    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="99">
+      <c r="D6" s="130"/>
+    </row>
+    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="97">
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="5">
         <v>204600</v>
       </c>
-      <c r="D7" s="96"/>
-    </row>
-    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99">
+      <c r="D7" s="130"/>
+    </row>
+    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="97">
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
@@ -4836,10 +4856,10 @@
       <c r="C8" s="5">
         <v>105000</v>
       </c>
-      <c r="D8" s="96"/>
-    </row>
-    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99">
+      <c r="D8" s="130"/>
+    </row>
+    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="97">
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
@@ -4848,36 +4868,36 @@
       <c r="C9" s="6">
         <v>35000</v>
       </c>
-      <c r="D9" s="96"/>
-    </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="104">
+      <c r="D9" s="130"/>
+    </row>
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="101">
         <v>8</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="9">
         <v>41750</v>
       </c>
-      <c r="D10" s="129" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99">
+      <c r="D10" s="131" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="97">
         <v>9</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="5">
         <v>80000</v>
       </c>
-      <c r="D11" s="96"/>
-    </row>
-    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="99">
+      <c r="D11" s="130"/>
+    </row>
+    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="97">
         <v>10</v>
       </c>
       <c r="B12" s="40" t="s">
@@ -4886,22 +4906,22 @@
       <c r="C12" s="5">
         <v>69612.899999999994</v>
       </c>
-      <c r="D12" s="96"/>
-    </row>
-    <row r="13" spans="1:4" ht="45" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99">
+      <c r="D12" s="130"/>
+    </row>
+    <row r="13" spans="1:4" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="97">
         <v>11</v>
       </c>
-      <c r="B13" s="132" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="133">
+      <c r="B13" s="128" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="129">
         <v>41000</v>
       </c>
-      <c r="D13" s="96"/>
-    </row>
-    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="99">
+      <c r="D13" s="130"/>
+    </row>
+    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="97">
         <v>12</v>
       </c>
       <c r="B14" s="86" t="s">
@@ -4910,10 +4930,10 @@
       <c r="C14" s="91">
         <v>30000</v>
       </c>
-      <c r="D14" s="96"/>
-    </row>
-    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99">
+      <c r="D14" s="130"/>
+    </row>
+    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="97">
         <v>13</v>
       </c>
       <c r="B15" s="56" t="s">
@@ -4922,10 +4942,10 @@
       <c r="C15" s="92">
         <v>27000</v>
       </c>
-      <c r="D15" s="96"/>
-    </row>
-    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="99">
+      <c r="D15" s="130"/>
+    </row>
+    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="97">
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
@@ -4934,10 +4954,10 @@
       <c r="C16" s="93">
         <v>26000</v>
       </c>
-      <c r="D16" s="96"/>
-    </row>
-    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="99">
+      <c r="D16" s="130"/>
+    </row>
+    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="97">
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
@@ -4946,10 +4966,10 @@
       <c r="C17" s="93">
         <v>50000</v>
       </c>
-      <c r="D17" s="96"/>
-    </row>
-    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="99">
+      <c r="D17" s="130"/>
+    </row>
+    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="97">
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
@@ -4958,10 +4978,10 @@
       <c r="C18" s="93">
         <v>15000</v>
       </c>
-      <c r="D18" s="96"/>
-    </row>
-    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="99">
+      <c r="D18" s="130"/>
+    </row>
+    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="97">
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
@@ -4970,10 +4990,10 @@
       <c r="C19" s="93">
         <v>9000</v>
       </c>
-      <c r="D19" s="96"/>
-    </row>
-    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="99">
+      <c r="D19" s="130"/>
+    </row>
+    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="97">
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
@@ -4982,10 +5002,10 @@
       <c r="C20" s="93">
         <v>14000</v>
       </c>
-      <c r="D20" s="96"/>
-    </row>
-    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99">
+      <c r="D20" s="130"/>
+    </row>
+    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="97">
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
@@ -4994,10 +5014,10 @@
       <c r="C21" s="93">
         <v>23000</v>
       </c>
-      <c r="D21" s="96"/>
-    </row>
-    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99">
+      <c r="D21" s="130"/>
+    </row>
+    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="97">
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
@@ -5006,22 +5026,24 @@
       <c r="C22" s="93">
         <v>17000</v>
       </c>
-      <c r="D22" s="96"/>
-    </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="99">
+      <c r="D22" s="130"/>
+    </row>
+    <row r="23" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="101">
         <v>21</v>
       </c>
-      <c r="B23" s="87" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" s="93">
-        <v>39000</v>
-      </c>
-      <c r="D23" s="96"/>
-    </row>
-    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="99">
+      <c r="B23" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="25">
+        <v>19500</v>
+      </c>
+      <c r="D23" s="131">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="97">
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
@@ -5030,40 +5052,40 @@
       <c r="C24" s="93">
         <v>20000</v>
       </c>
-      <c r="D24" s="96"/>
-    </row>
-    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="99">
+      <c r="D24" s="130"/>
+    </row>
+    <row r="25" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="97">
         <v>23</v>
       </c>
       <c r="B25" s="87" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="93">
         <f>(17000/30)* 23</f>
         <v>13033.333333333332</v>
       </c>
-      <c r="D25" s="96"/>
-    </row>
-    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="130"/>
+    </row>
+    <row r="26" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="87"/>
       <c r="C26" s="93"/>
-      <c r="D26" s="96"/>
-    </row>
-    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="130"/>
+    </row>
+    <row r="27" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="87"/>
       <c r="C27" s="94"/>
-      <c r="D27" s="96"/>
-    </row>
-    <row r="28" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D27" s="130"/>
+    </row>
+    <row r="28" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="22">
         <f>SUM(C3:C27)</f>
-        <v>1317173.6533333331</v>
-      </c>
-      <c r="D28" s="97"/>
+        <v>1297673.6533333331</v>
+      </c>
+      <c r="D28" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
PROJECAO DE JUNHO ALTERADA
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/BRYAN MEDIÇÕES - PROJEÇÕES/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{FC586834-44AE-4A4C-B98C-FCB33F1B1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80332A27-4032-4D8F-BD1B-0B81DEF6C517}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFC7FB3-FE38-D348-A2D5-1A6B33377AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ABRIL" sheetId="4" r:id="rId5"/>
     <sheet name="MAIO" sheetId="6" r:id="rId6"/>
     <sheet name="JUNHO" sheetId="7" r:id="rId7"/>
+    <sheet name="JULHO" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FEVEREIRO!$A$1:$E$33</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="152">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -489,6 +490,18 @@
   </si>
   <si>
     <t>JOÃO VICTOR  - PATROL 140 K  SÉRIE 5531 09/06 - 24/06</t>
+  </si>
+  <si>
+    <t>JULHO DE 2024 - MUDAR</t>
+  </si>
+  <si>
+    <t>JHSF VILLAFE - ERICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBS FRANCISCO MORATO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SÃO BENEDITO TERRAPLENAGEM - RETRO SÉRIE: 89176 </t>
   </si>
 </sst>
 </file>
@@ -496,9 +509,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -700,7 +713,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1217,13 +1230,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1250,11 +1278,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,7 +1324,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1307,7 +1335,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1316,7 +1344,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1327,7 +1355,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1360,10 +1388,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,7 +1410,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1470,12 +1498,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1494,9 +1540,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1536,10 +1579,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1551,11 +1594,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1581,10 +1619,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1890,19 +1924,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="134" t="s">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B1" s="142"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1910,7 +1944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1918,7 +1952,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1926,7 +1960,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -1934,7 +1968,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -1942,7 +1976,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -1950,7 +1984,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1992,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -1966,7 +2000,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -1975,7 +2009,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -1983,7 +2017,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -1991,7 +2025,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -1999,7 +2033,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -2007,7 +2041,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -2016,7 +2050,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -2024,7 +2058,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -2032,7 +2066,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -2040,7 +2074,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -2048,7 +2082,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -2056,11 +2090,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2102,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -2076,7 +2110,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -2084,7 +2118,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -2092,7 +2126,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -2100,7 +2134,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -2108,7 +2142,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -2116,7 +2150,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -2124,7 +2158,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -2132,7 +2166,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -2140,7 +2174,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -2148,7 +2182,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -2156,11 +2190,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -2189,22 +2223,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="68.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="134" t="s">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="135"/>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="142"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2218,7 +2252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2233,7 +2267,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2248,7 +2282,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2263,7 +2297,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2278,7 +2312,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2293,7 +2327,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2306,7 +2340,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2321,7 +2355,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2334,8 +2368,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="142">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="143">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2344,23 +2378,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="136" t="s">
+      <c r="D11" s="144" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="142"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="143"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="137"/>
+      <c r="D12" s="145"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2375,7 +2409,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2388,8 +2422,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="142">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="143">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2398,34 +2432,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="136" t="s">
+      <c r="D15" s="144" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="142"/>
+    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="143"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="138"/>
+      <c r="D16" s="146"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="142"/>
+    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="143"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="137"/>
+      <c r="D17" s="145"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -2440,7 +2474,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -2455,8 +2489,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="142">
+    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="143">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2465,23 +2499,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="136" t="s">
+      <c r="D20" s="144" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="142"/>
+    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="143"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="137"/>
+      <c r="D21" s="145"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2496,7 +2530,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2511,7 +2545,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2526,7 +2560,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2539,7 +2573,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2554,7 +2588,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2569,7 +2603,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2579,11 +2613,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="139"/>
+      <c r="D28" s="147"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="142">
+    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="143">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2592,43 +2626,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="140"/>
+      <c r="D29" s="148"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="142"/>
+    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="143"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="140"/>
+      <c r="D30" s="148"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="142"/>
+    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="143"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="140"/>
+      <c r="D31" s="148"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="142"/>
+    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="143"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="141"/>
+      <c r="D32" s="149"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2641,15 +2675,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2674,21 +2708,21 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="134" t="s">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="135"/>
-    </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="142"/>
+    </row>
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2696,7 +2730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2707,7 +2741,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2718,7 +2752,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2729,7 +2763,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2740,7 +2774,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2752,7 +2786,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2763,7 +2797,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2774,7 +2808,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2785,8 +2819,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="143">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="150">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2796,8 +2830,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="143"/>
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="150"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2805,7 +2839,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2816,8 +2850,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="143">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="150">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2827,8 +2861,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="143"/>
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="150"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2836,8 +2870,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="143"/>
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="150"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2845,8 +2879,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="143"/>
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="150"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2854,8 +2888,8 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="143"/>
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="150"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2863,7 +2897,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2874,7 +2908,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2885,8 +2919,8 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="143">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="150">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2896,8 +2930,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="143"/>
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="150"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -2905,7 +2939,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2916,7 +2950,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2927,7 +2961,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -2938,7 +2972,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -2949,7 +2983,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -2960,7 +2994,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -2971,7 +3005,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -2982,7 +3016,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -2993,8 +3027,8 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="143">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="150">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3004,8 +3038,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="143"/>
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="150"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -3013,8 +3047,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="143"/>
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="150"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -3022,7 +3056,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3033,7 +3067,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -3041,7 +3075,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -3049,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -3057,7 +3091,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -3066,7 +3100,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -3074,7 +3108,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -3082,7 +3116,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -3090,7 +3124,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -3098,7 +3132,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -3106,7 +3140,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -3114,7 +3148,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -3147,20 +3181,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="61"/>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
-    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="61"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="134" t="s">
+    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="135"/>
-    </row>
-    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="142"/>
+    </row>
+    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3168,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -3179,7 +3213,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -3190,7 +3224,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -3201,7 +3235,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -3212,7 +3246,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -3223,7 +3257,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -3234,7 +3268,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -3245,7 +3279,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -3256,8 +3290,8 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="143">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="150">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3267,8 +3301,8 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="143"/>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="150"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3276,7 +3310,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -3287,8 +3321,8 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="143">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="150">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3298,8 +3332,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="143"/>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="150"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3307,8 +3341,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="143"/>
+    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="150"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3316,8 +3350,8 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="143"/>
+    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="150"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3325,8 +3359,8 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="143"/>
+    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="150"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3334,7 +3368,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -3345,7 +3379,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -3356,8 +3390,8 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="143">
+    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="150">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3367,8 +3401,8 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="143"/>
+    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="150"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3376,7 +3410,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -3387,7 +3421,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -3398,7 +3432,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3409,7 +3443,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3420,7 +3454,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3431,7 +3465,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3442,7 +3476,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3453,7 +3487,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3464,8 +3498,8 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="143">
+    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="150">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3475,8 +3509,8 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="143"/>
+    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="150"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3484,8 +3518,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="143"/>
+    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="150"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3493,7 +3527,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3504,7 +3538,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3515,11 +3549,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3549,30 +3583,30 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="2" max="2" width="72.1640625" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="13" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="146" t="s">
+    <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-    </row>
-    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A2" s="146" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+    </row>
+    <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -3580,7 +3614,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -3594,7 +3628,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="68">
         <v>2</v>
       </c>
@@ -3608,7 +3642,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -3620,7 +3654,7 @@
       </c>
       <c r="D5" s="75"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -3632,7 +3666,7 @@
       </c>
       <c r="D6" s="79"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="76">
         <v>5</v>
       </c>
@@ -3644,7 +3678,7 @@
       </c>
       <c r="D7" s="79"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="68">
         <v>6</v>
       </c>
@@ -3658,7 +3692,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="76">
         <v>7</v>
       </c>
@@ -3670,7 +3704,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="68">
         <v>8</v>
       </c>
@@ -3684,7 +3718,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="68">
         <v>9</v>
       </c>
@@ -3698,7 +3732,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="68">
         <v>10</v>
       </c>
@@ -3712,7 +3746,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -3724,7 +3758,7 @@
       </c>
       <c r="D13" s="75"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="76">
         <v>12</v>
       </c>
@@ -3736,7 +3770,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>13</v>
       </c>
@@ -3748,7 +3782,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="68">
         <v>14</v>
       </c>
@@ -3762,7 +3796,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -3774,7 +3808,7 @@
       </c>
       <c r="D17" s="75"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -3788,7 +3822,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="68">
         <v>17</v>
       </c>
@@ -3802,7 +3836,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -3814,7 +3848,7 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -3826,7 +3860,7 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="76">
         <v>20</v>
       </c>
@@ -3838,7 +3872,7 @@
       </c>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="76">
         <v>21</v>
       </c>
@@ -3850,7 +3884,7 @@
       </c>
       <c r="D23" s="79"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="76">
         <v>22</v>
       </c>
@@ -3862,7 +3896,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="76">
         <v>23</v>
       </c>
@@ -3874,7 +3908,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="68">
         <v>24</v>
       </c>
@@ -3888,7 +3922,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="76">
         <v>25</v>
       </c>
@@ -3900,7 +3934,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
       <c r="B28" s="79" t="s">
         <v>81</v>
@@ -3910,7 +3944,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>99</v>
@@ -3920,7 +3954,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>84</v>
@@ -3930,7 +3964,7 @@
       </c>
       <c r="D30" s="79"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>85</v>
@@ -3940,7 +3974,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>117</v>
@@ -3950,7 +3984,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="76"/>
       <c r="B33" s="77" t="s">
         <v>87</v>
@@ -3960,7 +3994,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="76"/>
       <c r="B34" s="77" t="s">
         <v>119</v>
@@ -3970,7 +4004,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="68"/>
       <c r="B35" s="69" t="s">
         <v>26</v>
@@ -3982,7 +4016,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
         <v>120</v>
@@ -3993,7 +4027,7 @@
       <c r="D36" s="78"/>
       <c r="E36" s="79"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
         <v>121</v>
@@ -4003,7 +4037,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="76"/>
       <c r="B38" s="77" t="s">
         <v>115</v>
@@ -4013,7 +4047,7 @@
       </c>
       <c r="D38" s="78"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="76"/>
       <c r="B39" s="77" t="s">
         <v>118</v>
@@ -4023,7 +4057,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="76"/>
       <c r="B40" s="77" t="s">
         <v>116</v>
@@ -4033,43 +4067,43 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A41" s="147" t="s">
+    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A41" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="148"/>
+      <c r="B41" s="155"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A42" s="149" t="s">
+    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A42" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="150"/>
+      <c r="B42" s="157"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A43" s="144" t="s">
+    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="151" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="145"/>
+      <c r="B43" s="152"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="66"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="66"/>
     </row>
   </sheetData>
@@ -4092,25 +4126,25 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="76.625" customWidth="1"/>
-    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="158" t="s">
+    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="160"/>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="166"/>
+      <c r="D1" s="167"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>106</v>
       </c>
@@ -4121,7 +4155,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="101">
         <v>1</v>
       </c>
@@ -4135,7 +4169,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="101">
         <v>2</v>
       </c>
@@ -4149,7 +4183,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="97">
         <v>3</v>
       </c>
@@ -4161,7 +4195,7 @@
       </c>
       <c r="D5" s="103"/>
     </row>
-    <row r="6" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="97">
         <v>4</v>
       </c>
@@ -4174,7 +4208,7 @@
       </c>
       <c r="D6" s="103"/>
     </row>
-    <row r="7" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="106">
         <v>5</v>
       </c>
@@ -4188,7 +4222,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="101">
         <v>6</v>
       </c>
@@ -4202,7 +4236,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="101">
         <v>7</v>
       </c>
@@ -4216,7 +4250,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="106">
         <v>8</v>
       </c>
@@ -4230,21 +4264,21 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="161">
+    <row r="11" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="134">
         <v>9</v>
       </c>
-      <c r="B11" s="162" t="s">
+      <c r="B11" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="163">
+      <c r="C11" s="136">
         <v>30000</v>
       </c>
       <c r="D11" s="104">
         <v>933</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="101">
         <v>10</v>
       </c>
@@ -4258,7 +4292,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="106">
         <v>11</v>
       </c>
@@ -4272,7 +4306,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="101">
         <v>12</v>
       </c>
@@ -4287,7 +4321,7 @@
       </c>
       <c r="E14" s="126"/>
     </row>
-    <row r="15" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="96">
         <v>13</v>
       </c>
@@ -4299,7 +4333,7 @@
       </c>
       <c r="D15" s="103"/>
     </row>
-    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="112">
         <v>14</v>
       </c>
@@ -4313,7 +4347,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="106">
         <v>15</v>
       </c>
@@ -4327,7 +4361,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="106">
         <v>16</v>
       </c>
@@ -4341,7 +4375,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="106">
         <v>17</v>
       </c>
@@ -4355,7 +4389,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="101">
         <v>18</v>
       </c>
@@ -4369,7 +4403,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="102">
         <v>19</v>
       </c>
@@ -4383,21 +4417,21 @@
         <v>474</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="98"/>
       <c r="B22" s="99"/>
       <c r="C22" s="100"/>
       <c r="D22" s="105"/>
     </row>
-    <row r="23" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="151" t="s">
+    <row r="23" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="158" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="153"/>
-    </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="160"/>
+    </row>
+    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
         <v>134</v>
       </c>
@@ -4409,7 +4443,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="123" t="s">
         <v>134</v>
       </c>
@@ -4423,7 +4457,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="76" t="s">
         <v>134</v>
       </c>
@@ -4435,7 +4469,7 @@
       </c>
       <c r="D26" s="79"/>
     </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="68" t="s">
         <v>134</v>
       </c>
@@ -4449,7 +4483,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="76" t="s">
         <v>134</v>
       </c>
@@ -4461,7 +4495,7 @@
       </c>
       <c r="D28" s="78"/>
     </row>
-    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="76" t="s">
         <v>134</v>
       </c>
@@ -4474,7 +4508,7 @@
       <c r="D29" s="79"/>
       <c r="F29" s="126"/>
     </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>134</v>
       </c>
@@ -4486,7 +4520,7 @@
       </c>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>134</v>
       </c>
@@ -4498,7 +4532,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>134</v>
       </c>
@@ -4510,7 +4544,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="76" t="s">
         <v>136</v>
       </c>
@@ -4522,7 +4556,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
         <v>136</v>
       </c>
@@ -4534,7 +4568,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
         <v>136</v>
       </c>
@@ -4546,7 +4580,7 @@
       </c>
       <c r="D35" s="79"/>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="68" t="s">
         <v>136</v>
       </c>
@@ -4560,7 +4594,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="68" t="s">
         <v>136</v>
       </c>
@@ -4574,7 +4608,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
         <v>136</v>
       </c>
@@ -4586,7 +4620,7 @@
       </c>
       <c r="D38" s="79"/>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="76" t="s">
         <v>136</v>
       </c>
@@ -4598,7 +4632,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="68" t="s">
         <v>136</v>
       </c>
@@ -4612,7 +4646,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="76" t="s">
         <v>136</v>
       </c>
@@ -4626,60 +4660,60 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="76"/>
       <c r="B42" s="77"/>
       <c r="C42" s="78"/>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A43" s="147" t="s">
+    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="148"/>
+      <c r="B43" s="155"/>
       <c r="C43" s="82">
         <f>SUM(C3:C22)+SUM(C24:C42)</f>
         <v>2854994.0667741937</v>
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A44" s="149" t="s">
+    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A44" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="150"/>
+      <c r="B44" s="157"/>
       <c r="C44" s="65">
         <f>SUM(C3:C21)</f>
         <v>621342.86677419348</v>
       </c>
       <c r="D44" s="79"/>
     </row>
-    <row r="45" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="144" t="s">
+    <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="151" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="145"/>
+      <c r="B45" s="152"/>
       <c r="C45" s="83">
         <f>SUM(C24:C42)</f>
         <v>2233651.2000000002</v>
       </c>
       <c r="D45" s="79"/>
     </row>
-    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="151"/>
-      <c r="B46" s="152"/>
-      <c r="C46" s="152"/>
-      <c r="D46" s="153"/>
-    </row>
-    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="151" t="s">
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="158"/>
+      <c r="B46" s="159"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="160"/>
+    </row>
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="158" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="152"/>
-      <c r="C47" s="152"/>
-      <c r="D47" s="153"/>
-    </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B47" s="159"/>
+      <c r="C47" s="159"/>
+      <c r="D47" s="160"/>
+    </row>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="115" t="s">
         <v>134</v>
       </c>
@@ -4693,7 +4727,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="115" t="s">
         <v>134</v>
       </c>
@@ -4707,7 +4741,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="117" t="s">
         <v>136</v>
       </c>
@@ -4721,16 +4755,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="154" t="s">
+    <row r="51" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="161" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="155"/>
-      <c r="C51" s="156">
+      <c r="B51" s="162"/>
+      <c r="C51" s="163">
         <f>SUM(C48:C50)</f>
         <v>47612.9</v>
       </c>
-      <c r="D51" s="157"/>
+      <c r="D51" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4755,27 +4789,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="76.625" customWidth="1"/>
-    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="133"/>
+    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B1" s="158" t="s">
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="160"/>
-    </row>
-    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="166"/>
+      <c r="D1" s="167"/>
+    </row>
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
@@ -4786,306 +4820,270 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="97">
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5">
-        <v>59951.61</v>
+        <v>334000</v>
       </c>
       <c r="D3" s="130"/>
     </row>
-    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="97">
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="C4" s="5">
-        <v>28225.81</v>
+        <v>35000</v>
       </c>
       <c r="D4" s="130"/>
     </row>
-    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="97">
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="C5" s="5">
-        <v>334000</v>
+        <v>204600</v>
       </c>
       <c r="D5" s="130"/>
     </row>
-    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="97">
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="5">
-        <v>35000</v>
+        <v>105000</v>
       </c>
       <c r="D6" s="130"/>
     </row>
-    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="97">
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="5">
-        <v>204600</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>35000</v>
       </c>
       <c r="D7" s="130"/>
     </row>
-    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="97">
         <v>6</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="5">
-        <v>105000</v>
-      </c>
-      <c r="D8" s="130"/>
-    </row>
-    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="9">
+        <v>41750</v>
+      </c>
+      <c r="D8" s="131" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="97">
         <v>7</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6">
-        <v>35000</v>
+      <c r="B9" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="5">
+        <v>80000</v>
       </c>
       <c r="D9" s="130"/>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="101">
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="97">
         <v>8</v>
       </c>
-      <c r="B10" s="89" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="9">
-        <v>41750</v>
-      </c>
-      <c r="D10" s="131" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
+        <v>73000</v>
+      </c>
+      <c r="D10" s="130"/>
+    </row>
+    <row r="11" spans="1:4" ht="45" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="97">
         <v>9</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="5">
-        <v>80000</v>
+      <c r="B11" s="128" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="129">
+        <v>41000</v>
       </c>
       <c r="D11" s="130"/>
     </row>
-    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="97">
         <v>10</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="5">
-        <v>69612.899999999994</v>
+      <c r="B12" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="91">
+        <v>30000</v>
       </c>
       <c r="D12" s="130"/>
     </row>
-    <row r="13" spans="1:4" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="97">
         <v>11</v>
       </c>
-      <c r="B13" s="128" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="129">
-        <v>41000</v>
+      <c r="B13" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="92">
+        <v>27000</v>
       </c>
       <c r="D13" s="130"/>
     </row>
-    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="97">
         <v>12</v>
       </c>
-      <c r="B14" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="91">
-        <v>30000</v>
+      <c r="B14" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="93">
+        <v>26000</v>
       </c>
       <c r="D14" s="130"/>
     </row>
-    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="97">
         <v>13</v>
       </c>
-      <c r="B15" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="92">
-        <v>27000</v>
+      <c r="B15" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="93">
+        <v>50000</v>
       </c>
       <c r="D15" s="130"/>
     </row>
-    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="97">
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="C16" s="93">
-        <v>26000</v>
+        <v>15000</v>
       </c>
       <c r="D16" s="130"/>
     </row>
-    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="97">
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C17" s="93">
-        <v>50000</v>
+        <v>14000</v>
       </c>
       <c r="D17" s="130"/>
     </row>
-    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="97">
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C18" s="93">
-        <v>15000</v>
+        <v>23000</v>
       </c>
       <c r="D18" s="130"/>
     </row>
-    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="97">
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="C19" s="93">
-        <v>9000</v>
+        <v>17000</v>
       </c>
       <c r="D19" s="130"/>
     </row>
-    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="97">
         <v>18</v>
       </c>
-      <c r="B20" s="87" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="93">
-        <v>14000</v>
-      </c>
-      <c r="D20" s="130"/>
-    </row>
-    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="25">
+        <v>19500</v>
+      </c>
+      <c r="D20" s="131">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="97">
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C21" s="93">
-        <v>23000</v>
+        <v>20000</v>
       </c>
       <c r="D21" s="130"/>
     </row>
-    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="97">
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C22" s="93">
-        <v>17000</v>
-      </c>
-      <c r="D22" s="130"/>
-    </row>
-    <row r="23" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="101">
-        <v>21</v>
-      </c>
-      <c r="B23" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="25">
-        <v>19500</v>
-      </c>
-      <c r="D23" s="131">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="97">
-        <v>22</v>
-      </c>
-      <c r="B24" s="87" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="93">
-        <v>20000</v>
-      </c>
-      <c r="D24" s="130"/>
-    </row>
-    <row r="25" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="97">
-        <v>23</v>
-      </c>
-      <c r="B25" s="87" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="93">
         <f>(17000/30)* 23</f>
         <v>13033.333333333332</v>
       </c>
-      <c r="D25" s="130"/>
-    </row>
-    <row r="26" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="87"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="130"/>
-    </row>
-    <row r="27" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="87"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="130"/>
-    </row>
-    <row r="28" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="21" t="s">
+      <c r="D22" s="130"/>
+    </row>
+    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="87"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="130"/>
+    </row>
+    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="87"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="130"/>
+    </row>
+    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="22">
-        <f>SUM(C3:C27)</f>
-        <v>1297673.6533333331</v>
-      </c>
-      <c r="D28" s="132"/>
+      <c r="C25" s="22">
+        <f>SUM(C3:C24)</f>
+        <v>1203883.3333333333</v>
+      </c>
+      <c r="D25" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5094,4 +5092,307 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC478FF9-46FF-474D-AED6-95EDDA18EE1E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="133"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="166"/>
+      <c r="D1" s="167"/>
+    </row>
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="138" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="97">
+        <v>3</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5">
+        <v>324000</v>
+      </c>
+      <c r="D3" s="130"/>
+    </row>
+    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="97">
+        <v>4</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5">
+        <v>35000</v>
+      </c>
+      <c r="D4" s="130"/>
+    </row>
+    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="97">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="5">
+        <v>341000</v>
+      </c>
+      <c r="D5" s="130"/>
+    </row>
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="97">
+        <v>6</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="5">
+        <v>85000</v>
+      </c>
+      <c r="D6" s="130"/>
+    </row>
+    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="97">
+        <v>7</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>35000</v>
+      </c>
+      <c r="D7" s="130"/>
+    </row>
+    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="97">
+        <v>8</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="137">
+        <v>41750</v>
+      </c>
+      <c r="D8" s="130"/>
+    </row>
+    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="97">
+        <v>9</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="5">
+        <v>80000</v>
+      </c>
+      <c r="D9" s="130"/>
+    </row>
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="97">
+        <v>10</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
+        <v>69612.899999999994</v>
+      </c>
+      <c r="D10" s="130"/>
+    </row>
+    <row r="11" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="139">
+        <v>11</v>
+      </c>
+      <c r="B11" s="128" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="129">
+        <v>85500</v>
+      </c>
+      <c r="D11" s="140"/>
+    </row>
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="97">
+        <v>12</v>
+      </c>
+      <c r="B12" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="91">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="130"/>
+    </row>
+    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="97">
+        <v>13</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="92">
+        <v>27000</v>
+      </c>
+      <c r="D13" s="130"/>
+    </row>
+    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="97">
+        <v>14</v>
+      </c>
+      <c r="B14" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="93">
+        <v>26000</v>
+      </c>
+      <c r="D14" s="130"/>
+    </row>
+    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="97">
+        <v>15</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="93">
+        <v>50000</v>
+      </c>
+      <c r="D15" s="130"/>
+    </row>
+    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="97">
+        <v>16</v>
+      </c>
+      <c r="B16" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="93">
+        <v>15000</v>
+      </c>
+      <c r="D16" s="130"/>
+    </row>
+    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="97">
+        <v>17</v>
+      </c>
+      <c r="B17" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="93">
+        <v>9000</v>
+      </c>
+      <c r="D17" s="130"/>
+    </row>
+    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="97">
+        <v>18</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="93">
+        <v>14000</v>
+      </c>
+      <c r="D18" s="130"/>
+    </row>
+    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="97">
+        <v>19</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="93">
+        <v>23000</v>
+      </c>
+      <c r="D19" s="130"/>
+    </row>
+    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="97">
+        <v>20</v>
+      </c>
+      <c r="B20" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D20" s="130"/>
+    </row>
+    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="97">
+        <v>22</v>
+      </c>
+      <c r="B21" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="93">
+        <v>20000</v>
+      </c>
+      <c r="D21" s="130"/>
+    </row>
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="139">
+        <v>23</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D22" s="140"/>
+    </row>
+    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="87"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="130"/>
+    </row>
+    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="87"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="130"/>
+    </row>
+    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="22">
+        <f>SUM(C3:C24)</f>
+        <v>1344862.9</v>
+      </c>
+      <c r="D25" s="132"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ATUALIZACAO PROJ JULHO - FBS E GATHI
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFC7FB3-FE38-D348-A2D5-1A6B33377AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BD3152-14C1-0F4B-A8C6-852FB884BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="154">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -495,13 +495,19 @@
     <t>JULHO DE 2024 - MUDAR</t>
   </si>
   <si>
-    <t>JHSF VILLAFE - ERICA</t>
-  </si>
-  <si>
     <t xml:space="preserve">FBS FRANCISCO MORATO </t>
   </si>
   <si>
     <t xml:space="preserve">SÃO BENEDITO TERRAPLENAGEM - RETRO SÉRIE: 89176 </t>
+  </si>
+  <si>
+    <t>FBS VIADUTO - ROLO DIA 01/07 + ROLO DIA 03/07</t>
+  </si>
+  <si>
+    <t>GATHI - TRATOR DE ESTEIRAS + MOBILIZACAO</t>
+  </si>
+  <si>
+    <t>JHSF VILLAGE - ERICA</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1257,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1507,9 +1513,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1519,9 +1522,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1538,6 +1538,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1931,10 +1934,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="142"/>
+      <c r="B1" s="141"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
@@ -2233,10 +2236,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="142"/>
+      <c r="C1" s="141"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2369,7 +2372,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="143">
+      <c r="A11" s="148">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2378,20 +2381,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="144" t="s">
+      <c r="D11" s="142" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
+      <c r="A12" s="148"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="145"/>
+      <c r="D12" s="143"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2423,7 +2426,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="143">
+      <c r="A15" s="148">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2432,31 +2435,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="144" t="s">
+      <c r="D15" s="142" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143"/>
+      <c r="A16" s="148"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="146"/>
+      <c r="D16" s="144"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
+      <c r="A17" s="148"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="145"/>
+      <c r="D17" s="143"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2490,7 +2493,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143">
+      <c r="A20" s="148">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2499,20 +2502,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="144" t="s">
+      <c r="D20" s="142" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
+      <c r="A21" s="148"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="145"/>
+      <c r="D21" s="143"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2613,11 +2616,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="147"/>
+      <c r="D28" s="145"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="143">
+      <c r="A29" s="148">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2626,40 +2629,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="148"/>
+      <c r="D29" s="146"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="143"/>
+      <c r="A30" s="148"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="148"/>
+      <c r="D30" s="146"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="143"/>
+      <c r="A31" s="148"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="148"/>
+      <c r="D31" s="146"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="143"/>
+      <c r="A32" s="148"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="149"/>
+      <c r="D32" s="147"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2675,15 +2678,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2717,10 +2720,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="142"/>
+      <c r="C1" s="141"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2820,7 +2823,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="150">
+      <c r="A11" s="149">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2831,7 +2834,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2851,7 +2854,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="150">
+      <c r="A14" s="149">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2862,7 +2865,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
+      <c r="A15" s="149"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -2871,7 +2874,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="150"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2880,7 +2883,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="150"/>
+      <c r="A17" s="149"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -2889,7 +2892,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="150"/>
+      <c r="A18" s="149"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2920,7 +2923,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="150">
+      <c r="A21" s="149">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -2931,7 +2934,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="150"/>
+      <c r="A22" s="149"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -3028,7 +3031,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="150">
+      <c r="A31" s="149">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3039,7 +3042,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="150"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -3048,7 +3051,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
+      <c r="A33" s="149"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -3189,10 +3192,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="142"/>
+      <c r="C1" s="141"/>
     </row>
     <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3291,7 +3294,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="150">
+      <c r="A11" s="149">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3302,7 +3305,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3322,7 +3325,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="150">
+      <c r="A14" s="149">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3333,7 +3336,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
+      <c r="A15" s="149"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3342,7 +3345,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="150"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3351,7 +3354,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="150"/>
+      <c r="A17" s="149"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3360,7 +3363,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="150"/>
+      <c r="A18" s="149"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3391,7 +3394,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="150">
+      <c r="A21" s="149">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3402,7 +3405,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="150"/>
+      <c r="A22" s="149"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3499,7 +3502,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="150">
+      <c r="A31" s="149">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3510,7 +3513,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="150"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3519,7 +3522,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
+      <c r="A33" s="149"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3595,18 +3598,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
     </row>
     <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="152" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="153"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -4068,10 +4071,10 @@
       <c r="D40" s="79"/>
     </row>
     <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="154" t="s">
+      <c r="A41" s="153" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="155"/>
+      <c r="B41" s="154"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
@@ -4079,10 +4082,10 @@
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="156" t="s">
+      <c r="A42" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="157"/>
+      <c r="B42" s="156"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
@@ -4090,10 +4093,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="151" t="s">
+      <c r="A43" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="152"/>
+      <c r="B43" s="151"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
@@ -4138,11 +4141,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="167"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="166"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -4424,12 +4427,12 @@
       <c r="D22" s="105"/>
     </row>
     <row r="23" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="158" t="s">
+      <c r="A23" s="157" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="160"/>
+      <c r="B23" s="158"/>
+      <c r="C23" s="158"/>
+      <c r="D23" s="159"/>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -4667,10 +4670,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="154" t="s">
+      <c r="A43" s="153" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="155"/>
+      <c r="B43" s="154"/>
       <c r="C43" s="82">
         <f>SUM(C3:C22)+SUM(C24:C42)</f>
         <v>2854994.0667741937</v>
@@ -4678,10 +4681,10 @@
       <c r="D43" s="79"/>
     </row>
     <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A44" s="156" t="s">
+      <c r="A44" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="157"/>
+      <c r="B44" s="156"/>
       <c r="C44" s="65">
         <f>SUM(C3:C21)</f>
         <v>621342.86677419348</v>
@@ -4689,10 +4692,10 @@
       <c r="D44" s="79"/>
     </row>
     <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="151" t="s">
+      <c r="A45" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="152"/>
+      <c r="B45" s="151"/>
       <c r="C45" s="83">
         <f>SUM(C24:C42)</f>
         <v>2233651.2000000002</v>
@@ -4700,18 +4703,18 @@
       <c r="D45" s="79"/>
     </row>
     <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="158"/>
-      <c r="B46" s="159"/>
-      <c r="C46" s="159"/>
-      <c r="D46" s="160"/>
+      <c r="A46" s="157"/>
+      <c r="B46" s="158"/>
+      <c r="C46" s="158"/>
+      <c r="D46" s="159"/>
     </row>
     <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="158" t="s">
+      <c r="A47" s="157" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="159"/>
-      <c r="C47" s="159"/>
-      <c r="D47" s="160"/>
+      <c r="B47" s="158"/>
+      <c r="C47" s="158"/>
+      <c r="D47" s="159"/>
     </row>
     <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="115" t="s">
@@ -4756,15 +4759,15 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="161" t="s">
+      <c r="A51" s="160" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="162"/>
-      <c r="C51" s="163">
+      <c r="B51" s="161"/>
+      <c r="C51" s="162">
         <f>SUM(C48:C50)</f>
         <v>47612.9</v>
       </c>
-      <c r="D51" s="164"/>
+      <c r="D51" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4791,8 +4794,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4803,11 +4806,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="167"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="166"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -5096,10 +5099,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC478FF9-46FF-474D-AED6-95EDDA18EE1E}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5111,11 +5114,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="167"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="166"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -5130,7 +5133,7 @@
     </row>
     <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="97">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>11</v>
@@ -5142,10 +5145,10 @@
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C4" s="5">
         <v>35000</v>
@@ -5154,7 +5157,7 @@
     </row>
     <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="97">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>132</v>
@@ -5166,7 +5169,7 @@
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="97">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>125</v>
@@ -5178,7 +5181,7 @@
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="97">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>9</v>
@@ -5190,7 +5193,7 @@
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="97">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>129</v>
@@ -5202,7 +5205,7 @@
     </row>
     <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="97">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>130</v>
@@ -5214,7 +5217,7 @@
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="97">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="40" t="s">
         <v>16</v>
@@ -5225,168 +5228,188 @@
       <c r="D10" s="130"/>
     </row>
     <row r="11" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="139">
-        <v>11</v>
+      <c r="A11" s="97">
+        <v>9</v>
       </c>
       <c r="B11" s="128" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="129">
         <v>85500</v>
       </c>
-      <c r="D11" s="140"/>
+      <c r="D11" s="139"/>
     </row>
     <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="97">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="86" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C12" s="91">
-        <v>30000</v>
-      </c>
-      <c r="D12" s="130"/>
+        <v>31935.48</v>
+      </c>
+      <c r="D12" s="139"/>
     </row>
     <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="97">
-        <v>13</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="92">
-        <v>27000</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="91">
+        <v>30000</v>
       </c>
       <c r="D13" s="130"/>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="97">
-        <v>14</v>
-      </c>
-      <c r="B14" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="93">
-        <v>26000</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="92">
+        <v>27000</v>
       </c>
       <c r="D14" s="130"/>
     </row>
     <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="97">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="93">
-        <v>50000</v>
+        <v>26000</v>
       </c>
       <c r="D15" s="130"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="97">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C16" s="93">
-        <v>15000</v>
+        <v>50000</v>
       </c>
       <c r="D16" s="130"/>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="97">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C17" s="93">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="D17" s="130"/>
     </row>
     <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="97">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="93">
-        <v>14000</v>
+        <v>9000</v>
       </c>
       <c r="D18" s="130"/>
     </row>
     <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="97">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="C19" s="93">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="D19" s="130"/>
     </row>
     <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="97">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="93">
-        <v>17000</v>
+        <v>23000</v>
       </c>
       <c r="D20" s="130"/>
     </row>
     <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="97">
+        <v>19</v>
+      </c>
+      <c r="B21" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D21" s="130"/>
+    </row>
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="97">
+        <v>20</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="93">
+        <v>20000</v>
+      </c>
+      <c r="D22" s="130"/>
+    </row>
+    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="97">
+        <v>21</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D23" s="139"/>
+    </row>
+    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="97">
         <v>22</v>
       </c>
-      <c r="B21" s="87" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="93">
-        <v>20000</v>
-      </c>
-      <c r="D21" s="130"/>
-    </row>
-    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139">
-        <v>23</v>
-      </c>
-      <c r="B22" s="87" t="s">
-        <v>151</v>
-      </c>
-      <c r="C22" s="93">
-        <v>17000</v>
-      </c>
-      <c r="D22" s="140"/>
-    </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="130"/>
-    </row>
-    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="87"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="130"/>
-    </row>
-    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="21" t="s">
+      <c r="B24" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="93">
+        <f>40000+5000</f>
+        <v>45000</v>
+      </c>
+      <c r="D24" s="139"/>
+    </row>
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="87"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="130"/>
+    </row>
+    <row r="26" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="22">
-        <f>SUM(C3:C24)</f>
-        <v>1344862.9</v>
-      </c>
-      <c r="D25" s="132"/>
+      <c r="C26" s="22">
+        <f>SUM(C3:C25)</f>
+        <v>1421798.38</v>
+      </c>
+      <c r="D26" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
JUNHO RFM GRAND LODGE
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BD3152-14C1-0F4B-A8C6-852FB884BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D3304-CEC7-8445-B13E-457B43C10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="154">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -1522,6 +1522,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1538,9 +1541,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2372,7 +2372,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="148">
+      <c r="A11" s="142">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2381,20 +2381,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="142" t="s">
+      <c r="D11" s="143" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="148"/>
+      <c r="A12" s="142"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="143"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="148">
+      <c r="A15" s="142">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2435,31 +2435,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="142" t="s">
+      <c r="D15" s="143" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="148"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="144"/>
+      <c r="D16" s="145"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="148"/>
+      <c r="A17" s="142"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="143"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2493,7 +2493,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="148">
+      <c r="A20" s="142">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2502,20 +2502,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="142" t="s">
+      <c r="D20" s="143" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="148"/>
+      <c r="A21" s="142"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="143"/>
+      <c r="D21" s="144"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2616,11 +2616,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="145"/>
+      <c r="D28" s="146"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="148">
+      <c r="A29" s="142">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2629,40 +2629,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="146"/>
+      <c r="D29" s="147"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="148"/>
+      <c r="A30" s="142"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="146"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="148"/>
+      <c r="A31" s="142"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="146"/>
+      <c r="D31" s="147"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="148"/>
+      <c r="A32" s="142"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="147"/>
+      <c r="D32" s="148"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2678,6 +2678,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -2686,7 +2687,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -4795,7 +4795,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4860,15 +4860,9 @@
       <c r="D5" s="130"/>
     </row>
     <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="97">
-        <v>4</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="5">
-        <v>105000</v>
-      </c>
+      <c r="A6" s="97"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="130"/>
     </row>
     <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -4905,7 +4899,7 @@
         <v>130</v>
       </c>
       <c r="C9" s="5">
-        <v>80000</v>
+        <v>40000</v>
       </c>
       <c r="D9" s="130"/>
     </row>
@@ -5084,7 +5078,7 @@
       </c>
       <c r="C25" s="22">
         <f>SUM(C3:C24)</f>
-        <v>1203883.3333333333</v>
+        <v>1058883.3333333333</v>
       </c>
       <c r="D25" s="132"/>
     </row>
@@ -5099,10 +5093,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC478FF9-46FF-474D-AED6-95EDDA18EE1E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5211,7 +5208,7 @@
         <v>130</v>
       </c>
       <c r="C9" s="5">
-        <v>80000</v>
+        <v>40000</v>
       </c>
       <c r="D9" s="130"/>
     </row>
@@ -5407,7 +5404,7 @@
       </c>
       <c r="C26" s="22">
         <f>SUM(C3:C25)</f>
-        <v>1421798.38</v>
+        <v>1381798.38</v>
       </c>
       <c r="D26" s="132"/>
     </row>
@@ -5416,6 +5413,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizando notas de junho
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a95ce6011a9c105/Desktop/BRYAN MEDIÇÕES - PROJEÇÕES/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE1A308-A612-1B49-A0F6-4462FDFDB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{1EE1A308-A612-1B49-A0F6-4462FDFDB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591CB7F6-69C7-4112-BF99-D96BC4343D92}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="165">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>JHSF STATES - ERICA - PAGO PARCIALMENTE - R$ 22.166,67</t>
+  </si>
+  <si>
+    <t>DISEL</t>
   </si>
 </sst>
 </file>
@@ -545,9 +548,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -1278,10 +1281,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1308,11 +1311,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1354,7 +1357,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1365,7 +1368,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1374,7 +1377,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1385,7 +1388,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1418,10 +1421,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1440,7 +1443,7 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1551,27 +1554,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1611,10 +1614,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1624,6 +1627,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1636,8 +1642,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF9900"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF66"/>
     </mruColors>
@@ -1956,19 +1962,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="141" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="142"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>57</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>7258</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
         <v>58</v>
       </c>
@@ -1992,7 +1998,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>70535.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
@@ -2024,7 +2030,7 @@
         <v>42500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
@@ -2032,7 +2038,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -2041,7 +2047,7 @@
       </c>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>63</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="40" t="s">
         <v>11</v>
       </c>
@@ -2057,7 +2063,7 @@
         <v>406226</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>392500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="40" t="s">
         <v>64</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>63737</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="40" t="s">
         <v>65</v>
       </c>
@@ -2082,7 +2088,7 @@
       </c>
       <c r="D15" s="58"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
@@ -2090,7 +2096,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
@@ -2122,11 +2128,11 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="46"/>
       <c r="B21" s="47"/>
     </row>
-    <row r="22" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="46" t="s">
         <v>19</v>
       </c>
@@ -2134,7 +2140,7 @@
         <v>7983</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="48" t="s">
         <v>21</v>
       </c>
@@ -2142,7 +2148,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="40" t="s">
         <v>66</v>
       </c>
@@ -2150,7 +2156,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="50" t="s">
         <v>22</v>
       </c>
@@ -2158,7 +2164,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="50" t="s">
         <v>23</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
         <v>24</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41" t="s">
         <v>26</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>58365.57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="59" t="s">
         <v>68</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="41" t="s">
         <v>69</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="41" t="s">
         <v>70</v>
       </c>
@@ -2222,11 +2228,11 @@
         <v>14666.66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
     </row>
-    <row r="35" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -2255,22 +2261,22 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="68.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="68.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="142"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2299,7 +2305,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2314,7 +2320,7 @@
       </c>
       <c r="E4" s="30"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2329,7 +2335,7 @@
       </c>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2344,7 +2350,7 @@
       </c>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2359,7 +2365,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2372,7 +2378,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2387,7 +2393,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2400,8 +2406,8 @@
       <c r="D10" s="28"/>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="143">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="149">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2410,23 +2416,23 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="144" t="s">
+      <c r="D11" s="143" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="149"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="145"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="30"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2441,7 +2447,7 @@
       </c>
       <c r="E13" s="30"/>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2454,8 +2460,8 @@
       <c r="D14" s="28"/>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="143">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="149">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2464,34 +2470,34 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="144" t="s">
+      <c r="D15" s="143" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143"/>
+    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="149"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="146"/>
+      <c r="D16" s="145"/>
       <c r="E16" s="30"/>
     </row>
-    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
+    <row r="17" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="149"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="145"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="30"/>
     </row>
-    <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -2506,7 +2512,7 @@
       </c>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -2521,8 +2527,8 @@
       </c>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143">
+    <row r="20" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="149">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2531,23 +2537,23 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="144" t="s">
+      <c r="D20" s="143" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
+    <row r="21" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="149"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="145"/>
+      <c r="D21" s="144"/>
       <c r="E21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -2562,7 +2568,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -2577,7 +2583,7 @@
       </c>
       <c r="E23" s="30"/>
     </row>
-    <row r="24" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -2592,7 +2598,7 @@
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23">
         <v>17</v>
       </c>
@@ -2605,7 +2611,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -2620,7 +2626,7 @@
       </c>
       <c r="E26" s="30"/>
     </row>
-    <row r="27" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -2645,11 +2651,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="147"/>
+      <c r="D28" s="146"/>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="143">
+    <row r="29" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="149">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2658,43 +2664,43 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="148"/>
+      <c r="D29" s="147"/>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="143"/>
+    <row r="30" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="149"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="148"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="143"/>
+    <row r="31" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="149"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="148"/>
+      <c r="D31" s="147"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="143"/>
+    <row r="32" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="149"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="149"/>
+      <c r="D32" s="148"/>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="21" t="s">
         <v>35</v>
       </c>
@@ -2707,15 +2713,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2740,21 +2746,21 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="86.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="141" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="142"/>
     </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -2806,7 +2812,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -2818,7 +2824,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -2829,7 +2835,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -2840,7 +2846,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="150">
         <v>9</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="150"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -2871,7 +2877,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -2882,7 +2888,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="150">
         <v>12</v>
       </c>
@@ -2893,7 +2899,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="150"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -2902,7 +2908,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="150"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -2911,7 +2917,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="150"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
@@ -2920,7 +2926,7 @@
         <v>3189.58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="150"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
@@ -2929,7 +2935,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -2940,7 +2946,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="150">
         <v>15</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="150"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
@@ -2971,7 +2977,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3037,7 +3043,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3059,7 +3065,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="150">
         <v>24</v>
       </c>
@@ -3070,7 +3076,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="150"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
@@ -3079,7 +3085,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="150"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
@@ -3088,7 +3094,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3099,7 +3105,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="46" t="s">
         <v>51</v>
       </c>
@@ -3107,7 +3113,7 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="63" t="s">
         <v>81</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>16859</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="41" t="s">
         <v>85</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>191666</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="41" t="s">
         <v>86</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>29742</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="41" t="s">
         <v>87</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>119500</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="19" t="s">
         <v>77</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="19" t="s">
         <v>26</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="21" t="s">
         <v>35</v>
       </c>
@@ -3213,20 +3219,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="61"/>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="61"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="3" max="3" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="141" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="142"/>
     </row>
-    <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3234,7 +3240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="62">
         <v>1</v>
       </c>
@@ -3245,7 +3251,7 @@
         <v>67500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="62">
         <v>2</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="62">
         <v>3</v>
       </c>
@@ -3267,7 +3273,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4</v>
       </c>
@@ -3278,7 +3284,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="62">
         <v>5</v>
       </c>
@@ -3289,7 +3295,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="62">
         <v>6</v>
       </c>
@@ -3300,7 +3306,7 @@
         <v>406222</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>7</v>
       </c>
@@ -3311,7 +3317,7 @@
         <v>364500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="62">
         <v>8</v>
       </c>
@@ -3322,7 +3328,7 @@
         <v>115500</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="150">
         <v>9</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>79070</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="150"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -3342,7 +3348,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>11</v>
       </c>
@@ -3353,7 +3359,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="150">
         <v>12</v>
       </c>
@@ -3364,7 +3370,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="150"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
@@ -3373,7 +3379,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="150"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
@@ -3382,7 +3388,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="150"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
@@ -3391,7 +3397,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="150"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
@@ -3400,7 +3406,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="62">
         <v>13</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="62">
         <v>14</v>
       </c>
@@ -3422,7 +3428,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="150">
         <v>15</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>4258.0600000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="150"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
@@ -3442,7 +3448,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62">
         <v>16</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="62">
         <v>17</v>
       </c>
@@ -3464,7 +3470,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="62">
         <v>18</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="62">
         <v>19</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="62">
         <v>20</v>
       </c>
@@ -3497,7 +3503,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="62">
         <v>21</v>
       </c>
@@ -3508,7 +3514,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="62">
         <v>22</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>17600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="62">
         <v>23</v>
       </c>
@@ -3530,7 +3536,7 @@
         <v>11612.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="150">
         <v>24</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="150"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
@@ -3550,7 +3556,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="150"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
@@ -3559,7 +3565,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="62">
         <v>25</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>12612.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="62">
         <v>26</v>
       </c>
@@ -3581,11 +3587,11 @@
         <v>77000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
     </row>
-    <row r="37" spans="1:3" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
@@ -3619,14 +3625,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="72.1640625" customWidth="1"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="13" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
@@ -3634,7 +3640,7 @@
       <c r="C1" s="153"/>
       <c r="D1" s="153"/>
     </row>
-    <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A2" s="153" t="s">
         <v>89</v>
       </c>
@@ -3646,7 +3652,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="68">
         <v>2</v>
       </c>
@@ -3674,7 +3680,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -3686,7 +3692,7 @@
       </c>
       <c r="D5" s="75"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -3698,7 +3704,7 @@
       </c>
       <c r="D6" s="79"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="76">
         <v>5</v>
       </c>
@@ -3710,7 +3716,7 @@
       </c>
       <c r="D7" s="79"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="68">
         <v>6</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="76">
         <v>7</v>
       </c>
@@ -3736,7 +3742,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="68">
         <v>8</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="68">
         <v>9</v>
       </c>
@@ -3764,7 +3770,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="68">
         <v>10</v>
       </c>
@@ -3778,7 +3784,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -3790,7 +3796,7 @@
       </c>
       <c r="D13" s="75"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="76">
         <v>12</v>
       </c>
@@ -3802,7 +3808,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="76">
         <v>13</v>
       </c>
@@ -3814,7 +3820,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="68">
         <v>14</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -3840,7 +3846,7 @@
       </c>
       <c r="D17" s="75"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="68">
         <v>17</v>
       </c>
@@ -3868,7 +3874,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -3880,7 +3886,7 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -3892,7 +3898,7 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="76">
         <v>20</v>
       </c>
@@ -3904,7 +3910,7 @@
       </c>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="76">
         <v>21</v>
       </c>
@@ -3916,7 +3922,7 @@
       </c>
       <c r="D23" s="79"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="76">
         <v>22</v>
       </c>
@@ -3928,7 +3934,7 @@
       </c>
       <c r="D24" s="79"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="76">
         <v>23</v>
       </c>
@@ -3940,7 +3946,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="68">
         <v>24</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="76">
         <v>25</v>
       </c>
@@ -3966,7 +3972,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="76"/>
       <c r="B28" s="79" t="s">
         <v>81</v>
@@ -3976,7 +3982,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="76"/>
       <c r="B29" s="77" t="s">
         <v>99</v>
@@ -3986,7 +3992,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="76"/>
       <c r="B30" s="77" t="s">
         <v>84</v>
@@ -3996,7 +4002,7 @@
       </c>
       <c r="D30" s="79"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
         <v>85</v>
@@ -4006,7 +4012,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
         <v>117</v>
@@ -4016,7 +4022,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="76"/>
       <c r="B33" s="77" t="s">
         <v>87</v>
@@ -4026,7 +4032,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="76"/>
       <c r="B34" s="77" t="s">
         <v>119</v>
@@ -4036,7 +4042,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="68"/>
       <c r="B35" s="69" t="s">
         <v>26</v>
@@ -4048,7 +4054,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
         <v>120</v>
@@ -4059,7 +4065,7 @@
       <c r="D36" s="78"/>
       <c r="E36" s="79"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
         <v>121</v>
@@ -4069,7 +4075,7 @@
       </c>
       <c r="D37" s="79"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="76"/>
       <c r="B38" s="77" t="s">
         <v>115</v>
@@ -4079,7 +4085,7 @@
       </c>
       <c r="D38" s="78"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="76"/>
       <c r="B39" s="77" t="s">
         <v>118</v>
@@ -4089,7 +4095,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="76"/>
       <c r="B40" s="77" t="s">
         <v>116</v>
@@ -4099,7 +4105,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A41" s="154" t="s">
         <v>35</v>
       </c>
@@ -4110,7 +4116,7 @@
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A42" s="156" t="s">
         <v>96</v>
       </c>
@@ -4121,7 +4127,7 @@
       </c>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A43" s="151" t="s">
         <v>97</v>
       </c>
@@ -4132,10 +4138,10 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C45" s="66"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C47" s="66"/>
     </row>
   </sheetData>
@@ -4162,21 +4168,21 @@
       <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="165" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="166"/>
       <c r="D1" s="167"/>
     </row>
-    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>106</v>
       </c>
@@ -4187,7 +4193,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="101">
         <v>1</v>
       </c>
@@ -4201,7 +4207,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="101">
         <v>2</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="97">
         <v>3</v>
       </c>
@@ -4227,7 +4233,7 @@
       </c>
       <c r="D5" s="103"/>
     </row>
-    <row r="6" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="97">
         <v>4</v>
       </c>
@@ -4240,7 +4246,7 @@
       </c>
       <c r="D6" s="103"/>
     </row>
-    <row r="7" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="106">
         <v>5</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="101">
         <v>6</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="101">
         <v>7</v>
       </c>
@@ -4282,7 +4288,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="106">
         <v>8</v>
       </c>
@@ -4296,7 +4302,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="130">
         <v>9</v>
       </c>
@@ -4310,7 +4316,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="101">
         <v>10</v>
       </c>
@@ -4324,7 +4330,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="106">
         <v>11</v>
       </c>
@@ -4338,7 +4344,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="101">
         <v>12</v>
       </c>
@@ -4353,7 +4359,7 @@
       </c>
       <c r="E14" s="123"/>
     </row>
-    <row r="15" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="96">
         <v>13</v>
       </c>
@@ -4365,7 +4371,7 @@
       </c>
       <c r="D15" s="103"/>
     </row>
-    <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="112">
         <v>14</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="106">
         <v>15</v>
       </c>
@@ -4393,7 +4399,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="106">
         <v>16</v>
       </c>
@@ -4407,7 +4413,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="106">
         <v>17</v>
       </c>
@@ -4421,7 +4427,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="101">
         <v>18</v>
       </c>
@@ -4435,7 +4441,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="102">
         <v>19</v>
       </c>
@@ -4449,7 +4455,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="136">
         <v>20</v>
       </c>
@@ -4461,13 +4467,13 @@
       </c>
       <c r="D22" s="137"/>
     </row>
-    <row r="23" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="98"/>
       <c r="B23" s="99"/>
       <c r="C23" s="100"/>
       <c r="D23" s="105"/>
     </row>
-    <row r="24" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="158" t="s">
         <v>131</v>
       </c>
@@ -4475,7 +4481,7 @@
       <c r="C24" s="159"/>
       <c r="D24" s="160"/>
     </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="76" t="s">
         <v>132</v>
       </c>
@@ -4487,7 +4493,7 @@
       </c>
       <c r="D25" s="79"/>
     </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="68" t="s">
         <v>132</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="76" t="s">
         <v>132</v>
       </c>
@@ -4513,7 +4519,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="68" t="s">
         <v>132</v>
       </c>
@@ -4527,7 +4533,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
         <v>132</v>
       </c>
@@ -4539,7 +4545,7 @@
       </c>
       <c r="D29" s="78"/>
     </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
         <v>132</v>
       </c>
@@ -4552,7 +4558,7 @@
       <c r="D30" s="79"/>
       <c r="F30" s="123"/>
     </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="68" t="s">
         <v>132</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
         <v>132</v>
       </c>
@@ -4578,7 +4584,7 @@
       </c>
       <c r="D32" s="79"/>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="76" t="s">
         <v>132</v>
       </c>
@@ -4590,7 +4596,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="68" t="s">
         <v>134</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
         <v>134</v>
       </c>
@@ -4616,7 +4622,7 @@
       </c>
       <c r="D35" s="79"/>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="76" t="s">
         <v>134</v>
       </c>
@@ -4628,7 +4634,7 @@
       </c>
       <c r="D36" s="79"/>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="68" t="s">
         <v>134</v>
       </c>
@@ -4642,7 +4648,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="68" t="s">
         <v>134</v>
       </c>
@@ -4656,7 +4662,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="76" t="s">
         <v>134</v>
       </c>
@@ -4668,7 +4674,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="76" t="s">
         <v>134</v>
       </c>
@@ -4680,7 +4686,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="68" t="s">
         <v>134</v>
       </c>
@@ -4694,7 +4700,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="76" t="s">
         <v>134</v>
       </c>
@@ -4708,13 +4714,13 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="76"/>
       <c r="B43" s="77"/>
       <c r="C43" s="78"/>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A44" s="154" t="s">
         <v>35</v>
       </c>
@@ -4725,7 +4731,7 @@
       </c>
       <c r="D44" s="79"/>
     </row>
-    <row r="45" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A45" s="156" t="s">
         <v>96</v>
       </c>
@@ -4736,7 +4742,7 @@
       </c>
       <c r="D45" s="79"/>
     </row>
-    <row r="46" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="151" t="s">
         <v>97</v>
       </c>
@@ -4747,13 +4753,13 @@
       </c>
       <c r="D46" s="79"/>
     </row>
-    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="158"/>
       <c r="B47" s="159"/>
       <c r="C47" s="159"/>
       <c r="D47" s="160"/>
     </row>
-    <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="158" t="s">
         <v>138</v>
       </c>
@@ -4761,7 +4767,7 @@
       <c r="C48" s="159"/>
       <c r="D48" s="160"/>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="115" t="s">
         <v>132</v>
       </c>
@@ -4775,7 +4781,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="115" t="s">
         <v>132</v>
       </c>
@@ -4789,7 +4795,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="117" t="s">
         <v>134</v>
       </c>
@@ -4803,7 +4809,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="161" t="s">
         <v>139</v>
       </c>
@@ -4839,26 +4845,26 @@
   </sheetPr>
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="129" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="129" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="165" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="166"/>
       <c r="D1" s="167"/>
     </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>125</v>
       </c>
@@ -4869,7 +4875,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="97">
         <v>1</v>
       </c>
@@ -4881,7 +4887,7 @@
       </c>
       <c r="D3" s="126"/>
     </row>
-    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="97">
         <v>2</v>
       </c>
@@ -4893,7 +4899,7 @@
       </c>
       <c r="D4" s="126"/>
     </row>
-    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="97">
         <v>3</v>
       </c>
@@ -4905,26 +4911,28 @@
       </c>
       <c r="D5" s="126"/>
     </row>
-    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="97"/>
       <c r="B6" s="37"/>
       <c r="C6" s="5"/>
       <c r="D6" s="126"/>
     </row>
-    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="97">
+    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="106">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="108">
         <v>35000</v>
       </c>
-      <c r="D7" s="126"/>
-    </row>
-    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="97">
+      <c r="D7" s="168" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="101">
         <v>6</v>
       </c>
       <c r="B8" s="89" t="s">
@@ -4937,7 +4945,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="97">
         <v>7</v>
       </c>
@@ -4949,19 +4957,21 @@
       </c>
       <c r="D9" s="126"/>
     </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97">
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="106">
         <v>8</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="108">
         <v>73000</v>
       </c>
-      <c r="D10" s="126"/>
-    </row>
-    <row r="11" spans="1:4" ht="45" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="97">
         <v>9</v>
       </c>
@@ -4973,7 +4983,7 @@
       </c>
       <c r="D11" s="126"/>
     </row>
-    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="97">
         <v>10</v>
       </c>
@@ -4985,7 +4995,7 @@
       </c>
       <c r="D12" s="126"/>
     </row>
-    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="97">
         <v>11</v>
       </c>
@@ -4997,19 +5007,21 @@
       </c>
       <c r="D13" s="126"/>
     </row>
-    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97">
+    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="106">
         <v>12</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="93">
+      <c r="C14" s="111">
         <v>26000</v>
       </c>
-      <c r="D14" s="126"/>
-    </row>
-    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="97">
         <v>13</v>
       </c>
@@ -5022,7 +5034,7 @@
       </c>
       <c r="D15" s="126"/>
     </row>
-    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="97">
         <v>14</v>
       </c>
@@ -5034,7 +5046,7 @@
       </c>
       <c r="D16" s="126"/>
     </row>
-    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="97">
         <v>15</v>
       </c>
@@ -5046,32 +5058,36 @@
       </c>
       <c r="D17" s="126"/>
     </row>
-    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="97">
+    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="106">
         <v>16</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="93">
+      <c r="C18" s="111">
         <v>23000</v>
       </c>
-      <c r="D18" s="126"/>
-    </row>
-    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="97">
+      <c r="D18" s="168" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="106">
         <v>17</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="93">
+      <c r="C19" s="111">
         <v>17000</v>
       </c>
-      <c r="D19" s="126"/>
-    </row>
-    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="97">
+      <c r="D19" s="168" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="101">
         <v>18</v>
       </c>
       <c r="B20" s="59" t="s">
@@ -5084,19 +5100,21 @@
         <v>931</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="97">
+    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="101">
         <v>19</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="93">
+      <c r="C21" s="25">
         <v>20000</v>
       </c>
-      <c r="D21" s="126"/>
-    </row>
-    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="127">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="97">
         <v>20</v>
       </c>
@@ -5109,7 +5127,7 @@
       </c>
       <c r="D22" s="126"/>
     </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="97">
         <v>21</v>
       </c>
@@ -5121,12 +5139,12 @@
       </c>
       <c r="D23" s="126"/>
     </row>
-    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="87"/>
       <c r="C24" s="93"/>
       <c r="D24" s="126"/>
     </row>
-    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="158" t="s">
         <v>131</v>
       </c>
@@ -5134,7 +5152,7 @@
       <c r="C25" s="159"/>
       <c r="D25" s="160"/>
     </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="76" t="s">
         <v>132</v>
       </c>
@@ -5146,7 +5164,7 @@
       </c>
       <c r="D26" s="79"/>
     </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="76" t="s">
         <v>132</v>
       </c>
@@ -5158,7 +5176,7 @@
       </c>
       <c r="D27" s="79"/>
     </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
         <v>132</v>
       </c>
@@ -5170,7 +5188,7 @@
       </c>
       <c r="D28" s="79"/>
     </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="76" t="s">
         <v>134</v>
       </c>
@@ -5182,7 +5200,7 @@
       </c>
       <c r="D29" s="79"/>
     </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="76" t="s">
         <v>160</v>
       </c>
@@ -5194,7 +5212,7 @@
       </c>
       <c r="D30" s="78"/>
     </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
         <v>132</v>
       </c>
@@ -5206,7 +5224,7 @@
       </c>
       <c r="D31" s="79"/>
     </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="140" t="s">
         <v>132</v>
       </c>
@@ -5219,7 +5237,7 @@
       </c>
       <c r="D32" s="81"/>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="76" t="s">
         <v>132</v>
       </c>
@@ -5231,7 +5249,7 @@
       </c>
       <c r="D33" s="79"/>
     </row>
-    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="76" t="s">
         <v>134</v>
       </c>
@@ -5243,7 +5261,7 @@
       </c>
       <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="76" t="s">
         <v>134</v>
       </c>
@@ -5255,7 +5273,7 @@
       </c>
       <c r="D35" s="79"/>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="76" t="s">
         <v>134</v>
       </c>
@@ -5269,7 +5287,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="76" t="s">
         <v>157</v>
       </c>
@@ -5283,7 +5301,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="76" t="s">
         <v>157</v>
       </c>
@@ -5295,7 +5313,7 @@
       </c>
       <c r="D38" s="79"/>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="76" t="s">
         <v>157</v>
       </c>
@@ -5307,7 +5325,7 @@
       </c>
       <c r="D39" s="79"/>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="76" t="s">
         <v>157</v>
       </c>
@@ -5319,7 +5337,7 @@
       </c>
       <c r="D40" s="79"/>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="76" t="s">
         <v>157</v>
       </c>
@@ -5333,13 +5351,13 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="76"/>
       <c r="B42" s="77"/>
       <c r="C42" s="78"/>
       <c r="D42" s="79"/>
     </row>
-    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A43" s="154" t="s">
         <v>35</v>
       </c>
@@ -5350,7 +5368,7 @@
       </c>
       <c r="D43" s="79"/>
     </row>
-    <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A44" s="156" t="s">
         <v>96</v>
       </c>
@@ -5361,7 +5379,7 @@
       </c>
       <c r="D44" s="79"/>
     </row>
-    <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="151" t="s">
         <v>97</v>
       </c>
@@ -5372,13 +5390,13 @@
       </c>
       <c r="D45" s="79"/>
     </row>
-    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="158"/>
       <c r="B46" s="159"/>
       <c r="C46" s="159"/>
       <c r="D46" s="160"/>
     </row>
-    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="158" t="s">
         <v>159</v>
       </c>
@@ -5386,7 +5404,7 @@
       <c r="C47" s="159"/>
       <c r="D47" s="160"/>
     </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="68" t="s">
         <v>132</v>
       </c>
@@ -5400,7 +5418,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="68" t="s">
         <v>132</v>
       </c>
@@ -5414,7 +5432,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="68" t="s">
         <v>132</v>
       </c>
@@ -5428,7 +5446,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="68" t="s">
         <v>134</v>
       </c>
@@ -5442,7 +5460,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="68" t="s">
         <v>134</v>
       </c>
@@ -5456,7 +5474,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="68" t="s">
         <v>134</v>
       </c>
@@ -5470,7 +5488,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="68" t="s">
         <v>157</v>
       </c>
@@ -5483,7 +5501,7 @@
       </c>
       <c r="D54" s="71"/>
     </row>
-    <row r="55" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="68" t="s">
         <v>134</v>
       </c>
@@ -5497,7 +5515,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="161" t="s">
         <v>139</v>
       </c>
@@ -5536,22 +5554,22 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="129"/>
+    <col min="2" max="2" width="76.625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="129"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B1" s="165" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="166"/>
       <c r="D1" s="167"/>
     </row>
-    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="B2" s="2" t="s">
         <v>145</v>
       </c>
@@ -5562,7 +5580,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="97">
         <v>1</v>
       </c>
@@ -5574,7 +5592,7 @@
       </c>
       <c r="D3" s="126"/>
     </row>
-    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="97">
         <v>2</v>
       </c>
@@ -5586,7 +5604,7 @@
       </c>
       <c r="D4" s="126"/>
     </row>
-    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="97">
         <v>3</v>
       </c>
@@ -5598,7 +5616,7 @@
       </c>
       <c r="D5" s="126"/>
     </row>
-    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="97">
         <v>4</v>
       </c>
@@ -5610,7 +5628,7 @@
       </c>
       <c r="D6" s="126"/>
     </row>
-    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="97">
         <v>5</v>
       </c>
@@ -5622,7 +5640,7 @@
       </c>
       <c r="D7" s="126"/>
     </row>
-    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="97">
         <v>6</v>
       </c>
@@ -5634,7 +5652,7 @@
       </c>
       <c r="D8" s="126"/>
     </row>
-    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="97">
         <v>7</v>
       </c>
@@ -5646,7 +5664,7 @@
       </c>
       <c r="D9" s="126"/>
     </row>
-    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="97">
         <v>8</v>
       </c>
@@ -5658,7 +5676,7 @@
       </c>
       <c r="D10" s="126"/>
     </row>
-    <row r="11" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="97">
         <v>9</v>
       </c>
@@ -5670,7 +5688,7 @@
       </c>
       <c r="D11" s="135"/>
     </row>
-    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="97">
         <v>10</v>
       </c>
@@ -5682,7 +5700,7 @@
       </c>
       <c r="D12" s="135"/>
     </row>
-    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="97">
         <v>11</v>
       </c>
@@ -5694,7 +5712,7 @@
       </c>
       <c r="D13" s="126"/>
     </row>
-    <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="97">
         <v>12</v>
       </c>
@@ -5706,7 +5724,7 @@
       </c>
       <c r="D14" s="126"/>
     </row>
-    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="97">
         <v>13</v>
       </c>
@@ -5718,7 +5736,7 @@
       </c>
       <c r="D15" s="126"/>
     </row>
-    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="97">
         <v>14</v>
       </c>
@@ -5730,7 +5748,7 @@
       </c>
       <c r="D16" s="126"/>
     </row>
-    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="97">
         <v>15</v>
       </c>
@@ -5742,7 +5760,7 @@
       </c>
       <c r="D17" s="126"/>
     </row>
-    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="97">
         <v>16</v>
       </c>
@@ -5754,7 +5772,7 @@
       </c>
       <c r="D18" s="126"/>
     </row>
-    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="97">
         <v>17</v>
       </c>
@@ -5766,7 +5784,7 @@
       </c>
       <c r="D19" s="126"/>
     </row>
-    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="97">
         <v>18</v>
       </c>
@@ -5778,7 +5796,7 @@
       </c>
       <c r="D20" s="126"/>
     </row>
-    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="97">
         <v>19</v>
       </c>
@@ -5790,7 +5808,7 @@
       </c>
       <c r="D21" s="126"/>
     </row>
-    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="97">
         <v>20</v>
       </c>
@@ -5802,7 +5820,7 @@
       </c>
       <c r="D22" s="135"/>
     </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="97">
         <v>21</v>
       </c>
@@ -5815,12 +5833,12 @@
       </c>
       <c r="D23" s="135"/>
     </row>
-    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="87"/>
       <c r="C24" s="94"/>
       <c r="D24" s="126"/>
     </row>
-    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="21" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
excluindo algumas meds de junho
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE1A308-A612-1B49-A0F6-4462FDFDB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA9ECD-7516-BA4C-8E77-5988C92E44AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" firstSheet="1" activeTab="6" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -24,6 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FEVEREIRO!$A$1:$E$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">JUNHO!$A$1:$E$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1551,9 +1552,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1570,6 +1568,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2401,7 +2402,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="143">
+      <c r="A11" s="149">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2410,20 +2411,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="144" t="s">
+      <c r="D11" s="143" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
+      <c r="A12" s="149"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="145"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2455,7 +2456,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="143">
+      <c r="A15" s="149">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2464,31 +2465,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="144" t="s">
+      <c r="D15" s="143" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="146"/>
+      <c r="D16" s="145"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
+      <c r="A17" s="149"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="145"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2522,7 +2523,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143">
+      <c r="A20" s="149">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2531,20 +2532,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="144" t="s">
+      <c r="D20" s="143" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="145"/>
+      <c r="D21" s="144"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2645,11 +2646,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="147"/>
+      <c r="D28" s="146"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="143">
+      <c r="A29" s="149">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2658,40 +2659,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="148"/>
+      <c r="D29" s="147"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="143"/>
+      <c r="A30" s="149"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="148"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="143"/>
+      <c r="A31" s="149"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="148"/>
+      <c r="D31" s="147"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="143"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="149"/>
+      <c r="D32" s="148"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2707,15 +2708,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -4839,8 +4840,8 @@
   </sheetPr>
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5521,7 +5522,7 @@
     <mergeCell ref="A46:D46"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="61" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="53" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Projecao de Julho atualizada
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E9F9F4-10F9-564F-9739-3DB71D716332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20DAE5-B75A-1B4A-A896-2919C123DDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="172">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -495,9 +495,6 @@
     <t>FBS VIADUTO - ROLO DIA 01/07 + ROLO DIA 03/07</t>
   </si>
   <si>
-    <t>GATHI - TRATOR DE ESTEIRAS + MOBILIZACAO</t>
-  </si>
-  <si>
     <t>JHSF VILLAGE - ISABELLA</t>
   </si>
   <si>
@@ -541,6 +538,30 @@
   </si>
   <si>
     <t>DISEL</t>
+  </si>
+  <si>
+    <t>WM LOCAÇÕES - RETRO - DEVOLVEU DIA 19/07</t>
+  </si>
+  <si>
+    <t>ALEXANDRE CABRAL - SOROCABA - ESCAVADEIRA 13 TON - DEV. 18/07</t>
+  </si>
+  <si>
+    <t>DENILSON - RETRO JCB - 20/07</t>
+  </si>
+  <si>
+    <t>ALCANCE - 1º QUINZENA JULHO DE 2024</t>
+  </si>
+  <si>
+    <t>ALCANCE - 2º QUINZENA JULHO DE 2024</t>
+  </si>
+  <si>
+    <t>JHSF - PRÓ GOLF - PAROU DIA 16/07</t>
+  </si>
+  <si>
+    <t>AFONSO FRANÇA ASHLAND - 11/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATHI - TRATOR DE ESTEIRAS </t>
   </si>
 </sst>
 </file>
@@ -4470,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="93">
         <v>6000</v>
@@ -4514,7 +4535,7 @@
         <v>191666</v>
       </c>
       <c r="D26" s="138" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4573,13 +4594,13 @@
         <v>132</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C31" s="139">
         <v>168000</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4902,7 +4923,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5">
         <v>35000</v>
@@ -4938,7 +4959,7 @@
         <v>35000</v>
       </c>
       <c r="D7" s="141" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -5142,7 +5163,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C23" s="93">
         <v>15000</v>
@@ -5212,7 +5233,7 @@
     </row>
     <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B30" s="77" t="s">
         <v>120</v>
@@ -5239,7 +5260,7 @@
         <v>132</v>
       </c>
       <c r="B32" s="80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="113">
         <f>168000*0.15</f>
@@ -5299,10 +5320,10 @@
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B37" s="77" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="78">
         <v>17000</v>
@@ -5313,7 +5334,7 @@
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B38" s="77" t="s">
         <v>122</v>
@@ -5325,7 +5346,7 @@
     </row>
     <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B39" s="77" t="s">
         <v>109</v>
@@ -5337,10 +5358,10 @@
     </row>
     <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C40" s="78">
         <v>6000</v>
@@ -5349,7 +5370,7 @@
     </row>
     <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B41" s="77" t="s">
         <v>110</v>
@@ -5408,7 +5429,7 @@
     </row>
     <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B47" s="162"/>
       <c r="C47" s="162"/>
@@ -5425,7 +5446,7 @@
         <v>191666</v>
       </c>
       <c r="D48" s="138" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -5447,13 +5468,13 @@
         <v>132</v>
       </c>
       <c r="B50" s="69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C50" s="139">
         <v>142800</v>
       </c>
       <c r="D50" s="70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -5500,10 +5521,10 @@
     </row>
     <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C54" s="70">
         <f>(35000/31)*3</f>
@@ -5558,15 +5579,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="2" max="2" width="84.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="129"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
@@ -5595,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="C3" s="5">
         <v>169725.81</v>
@@ -5607,7 +5628,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5">
         <v>35000</v>
@@ -5619,7 +5640,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="5">
         <v>341000</v>
@@ -5631,7 +5652,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="5">
         <v>85000</v>
@@ -5655,7 +5676,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="C8" s="133">
         <v>41750</v>
@@ -5667,7 +5688,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="C9" s="5">
         <v>40000</v>
@@ -5775,10 +5796,11 @@
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="C18" s="93">
-        <v>14000</v>
+        <f>(19/31)*14000</f>
+        <v>8580.645161290322</v>
       </c>
       <c r="D18" s="126"/>
     </row>
@@ -5787,10 +5809,11 @@
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="C19" s="93">
-        <v>23000</v>
+        <f>(18/31)*23000</f>
+        <v>13354.83870967742</v>
       </c>
       <c r="D19" s="126"/>
     </row>
@@ -5835,34 +5858,58 @@
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C23" s="93">
-        <f>40000+5000</f>
-        <v>45000</v>
+        <v>55000</v>
       </c>
       <c r="D23" s="135"/>
     </row>
     <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="87"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="126"/>
-    </row>
-    <row r="25" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="21" t="s">
+      <c r="A24" s="97">
+        <v>22</v>
+      </c>
+      <c r="B24" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="93">
+        <f>(17000/31)*12</f>
+        <v>6580.645161290322</v>
+      </c>
+      <c r="D24" s="135"/>
+    </row>
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="97">
+        <v>23</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="93">
+        <v>45935.48</v>
+      </c>
+      <c r="D25" s="135"/>
+    </row>
+    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="87"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="126"/>
+    </row>
+    <row r="27" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="22">
-        <f>SUM(C3:C24)</f>
-        <v>1222378.81</v>
-      </c>
-      <c r="D25" s="128"/>
+      <c r="C27" s="22">
+        <f>SUM(C3:C26)</f>
+        <v>1269830.4190322582</v>
+      </c>
+      <c r="D27" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Medicao Julho JHSF PARQUES
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20DAE5-B75A-1B4A-A896-2919C123DDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12788E7A-8B1E-1C48-B8F9-CB392D028C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="173">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t xml:space="preserve">GATHI - TRATOR DE ESTEIRAS </t>
+  </si>
+  <si>
+    <t>JHSF - PARQUES - 23/07 + MOB.ESCAVADEIRA</t>
   </si>
 </sst>
 </file>
@@ -1588,9 +1591,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,6 +1607,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2438,7 +2441,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="146">
+      <c r="A11" s="152">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2447,20 +2450,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="147" t="s">
+      <c r="D11" s="146" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="148"/>
+      <c r="D12" s="147"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2492,7 +2495,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="146">
+      <c r="A15" s="152">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2501,31 +2504,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="147" t="s">
+      <c r="D15" s="146" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="146"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="149"/>
+      <c r="D16" s="148"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="146"/>
+      <c r="A17" s="152"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="148"/>
+      <c r="D17" s="147"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2562,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="146">
+      <c r="A20" s="152">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2568,20 +2571,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="147" t="s">
+      <c r="D20" s="146" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="146"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="148"/>
+      <c r="D21" s="147"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2682,11 +2685,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="150"/>
+      <c r="D28" s="149"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="146">
+      <c r="A29" s="152">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2695,40 +2698,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="151"/>
+      <c r="D29" s="150"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="146"/>
+      <c r="A30" s="152"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="151"/>
+      <c r="D30" s="150"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="146"/>
+      <c r="A31" s="152"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="151"/>
+      <c r="D31" s="150"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="146"/>
+      <c r="A32" s="152"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="152"/>
+      <c r="D32" s="151"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2744,15 +2747,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -5579,10 +5582,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5652,10 +5655,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C6" s="5">
-        <v>85000</v>
+        <v>27177.42</v>
       </c>
       <c r="D6" s="126"/>
     </row>
@@ -5664,10 +5667,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6">
-        <v>35000</v>
+        <v>151</v>
+      </c>
+      <c r="C7" s="5">
+        <v>85000</v>
       </c>
       <c r="D7" s="126"/>
     </row>
@@ -5676,10 +5679,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="133">
-        <v>41750</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>35000</v>
       </c>
       <c r="D8" s="126"/>
     </row>
@@ -5687,11 +5690,11 @@
       <c r="A9" s="97">
         <v>7</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="5">
-        <v>40000</v>
+      <c r="B9" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="133">
+        <v>41750</v>
       </c>
       <c r="D9" s="126"/>
     </row>
@@ -5700,34 +5703,34 @@
         <v>8</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="C10" s="5">
-        <v>73000</v>
+        <v>40000</v>
       </c>
       <c r="D10" s="126"/>
     </row>
-    <row r="11" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="97">
         <v>9</v>
       </c>
-      <c r="B11" s="124" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="125">
-        <v>85500</v>
-      </c>
-      <c r="D11" s="135"/>
-    </row>
-    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5">
+        <v>73000</v>
+      </c>
+      <c r="D11" s="126"/>
+    </row>
+    <row r="12" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="97">
         <v>10</v>
       </c>
-      <c r="B12" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12" s="91">
-        <v>36403</v>
+      <c r="B12" s="124" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="125">
+        <v>85500</v>
       </c>
       <c r="D12" s="135"/>
     </row>
@@ -5736,22 +5739,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="86" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="C13" s="91">
-        <v>30000</v>
-      </c>
-      <c r="D13" s="126"/>
+        <v>36403</v>
+      </c>
+      <c r="D13" s="135"/>
     </row>
     <row r="14" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="97">
         <v>12</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="92">
-        <v>27000</v>
+      <c r="B14" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="91">
+        <v>30000</v>
       </c>
       <c r="D14" s="126"/>
     </row>
@@ -5759,11 +5762,11 @@
       <c r="A15" s="97">
         <v>13</v>
       </c>
-      <c r="B15" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="93">
-        <v>26000</v>
+      <c r="B15" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="92">
+        <v>27000</v>
       </c>
       <c r="D15" s="126"/>
     </row>
@@ -5772,10 +5775,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="93">
-        <v>46000</v>
+        <v>26000</v>
       </c>
       <c r="D16" s="126"/>
     </row>
@@ -5784,10 +5787,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C17" s="93">
-        <v>15000</v>
+        <v>46000</v>
       </c>
       <c r="D17" s="126"/>
     </row>
@@ -5796,11 +5799,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>164</v>
+        <v>109</v>
       </c>
       <c r="C18" s="93">
-        <f>(19/31)*14000</f>
-        <v>8580.645161290322</v>
+        <v>15000</v>
       </c>
       <c r="D18" s="126"/>
     </row>
@@ -5809,11 +5811,11 @@
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" s="93">
-        <f>(18/31)*23000</f>
-        <v>13354.83870967742</v>
+        <f>(19/31)*14000</f>
+        <v>8580.645161290322</v>
       </c>
       <c r="D19" s="126"/>
     </row>
@@ -5822,10 +5824,11 @@
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="C20" s="93">
-        <v>17000</v>
+        <f>(18/31)*23000</f>
+        <v>13354.83870967742</v>
       </c>
       <c r="D20" s="126"/>
     </row>
@@ -5834,10 +5837,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C21" s="93">
-        <v>20000</v>
+        <v>17000</v>
       </c>
       <c r="D21" s="126"/>
     </row>
@@ -5846,22 +5849,22 @@
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="C22" s="93">
-        <v>17000</v>
-      </c>
-      <c r="D22" s="135"/>
+        <v>20000</v>
+      </c>
+      <c r="D22" s="126"/>
     </row>
     <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="97">
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="C23" s="93">
-        <v>55000</v>
+        <v>17000</v>
       </c>
       <c r="D23" s="135"/>
     </row>
@@ -5870,11 +5873,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C24" s="93">
-        <f>(17000/31)*12</f>
-        <v>6580.645161290322</v>
+        <v>55000</v>
       </c>
       <c r="D24" s="135"/>
     </row>
@@ -5883,27 +5885,40 @@
         <v>23</v>
       </c>
       <c r="B25" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="93">
+        <f>(17000/31)*12</f>
+        <v>6580.645161290322</v>
+      </c>
+      <c r="D25" s="135"/>
+    </row>
+    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97">
+        <v>24</v>
+      </c>
+      <c r="B26" s="87" t="s">
         <v>170</v>
       </c>
-      <c r="C25" s="93">
+      <c r="C26" s="93">
         <v>45935.48</v>
       </c>
-      <c r="D25" s="135"/>
-    </row>
-    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="87"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="126"/>
-    </row>
-    <row r="27" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="21" t="s">
+      <c r="D26" s="135"/>
+    </row>
+    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="87"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="126"/>
+    </row>
+    <row r="28" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="22">
-        <f>SUM(C3:C26)</f>
-        <v>1269830.4190322582</v>
-      </c>
-      <c r="D27" s="128"/>
+      <c r="C28" s="22">
+        <f>SUM(C3:C27)</f>
+        <v>1297007.8390322581</v>
+      </c>
+      <c r="D28" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
pro golf quina e village parques
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12788E7A-8B1E-1C48-B8F9-CB392D028C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC17E1C9-8986-3545-A2CB-238603451990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -24,6 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FEVEREIRO!$A$1:$E$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JULHO!$A$1:$E$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="177">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -555,16 +556,28 @@
     <t>ALCANCE - 2º QUINZENA JULHO DE 2024</t>
   </si>
   <si>
-    <t>JHSF - PRÓ GOLF - PAROU DIA 16/07</t>
-  </si>
-  <si>
     <t>AFONSO FRANÇA ASHLAND - 11/07</t>
   </si>
   <si>
     <t xml:space="preserve">GATHI - TRATOR DE ESTEIRAS </t>
   </si>
   <si>
-    <t>JHSF - PARQUES - 23/07 + MOB.ESCAVADEIRA</t>
+    <t>BERINHA PEDRAS - ROLO - FOI 23/07 + MOB</t>
+  </si>
+  <si>
+    <t>Berinha Agosto tem que fechar 15.000 do rolo = 21/30 * 15000 = 10.500 + 1.000 de desmob = 11..500</t>
+  </si>
+  <si>
+    <t>JHSF - PARQUES - 23/07 + MOB.ESCAVADEIRA + 24/07 CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEANDRO QUINA - MRV - ROLO DYNAPAC SÉRIE 8466 </t>
+  </si>
+  <si>
+    <t>LEANDRO QUINA D4  -SOLOTEC - SÉRIE 536 - 25/07</t>
+  </si>
+  <si>
+    <t>JHSF - PRÓ GOLF - PAROU DIA 16/07 - Trator dia 29/07</t>
   </si>
 </sst>
 </file>
@@ -1591,6 +1604,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,9 +1623,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2441,7 +2454,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="152">
+      <c r="A11" s="146">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2450,20 +2463,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="146" t="s">
+      <c r="D11" s="147" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="146"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="147"/>
+      <c r="D12" s="148"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2495,7 +2508,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="152">
+      <c r="A15" s="146">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2504,31 +2517,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="146" t="s">
+      <c r="D15" s="147" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
+      <c r="A16" s="146"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="148"/>
+      <c r="D16" s="149"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="152"/>
+      <c r="A17" s="146"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="147"/>
+      <c r="D17" s="148"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2562,7 +2575,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152">
+      <c r="A20" s="146">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2571,20 +2584,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="146" t="s">
+      <c r="D20" s="147" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="152"/>
+      <c r="A21" s="146"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="147"/>
+      <c r="D21" s="148"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2685,11 +2698,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="149"/>
+      <c r="D28" s="150"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="152">
+      <c r="A29" s="146">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2698,40 +2711,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="150"/>
+      <c r="D29" s="151"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="152"/>
+      <c r="A30" s="146"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="150"/>
+      <c r="D30" s="151"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="152"/>
+      <c r="A31" s="146"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="150"/>
+      <c r="D31" s="151"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="152"/>
+      <c r="A32" s="146"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="151"/>
+      <c r="D32" s="152"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2747,15 +2760,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -5582,10 +5595,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5594,6 +5607,7 @@
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="129"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
@@ -5619,10 +5633,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C3" s="5">
-        <v>169725.81</v>
+        <v>175612.9</v>
       </c>
       <c r="D3" s="126"/>
     </row>
@@ -5655,10 +5669,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C6" s="5">
-        <v>27177.42</v>
+        <v>36725.81</v>
       </c>
       <c r="D6" s="126"/>
     </row>
@@ -5782,7 +5796,7 @@
       </c>
       <c r="D16" s="126"/>
     </row>
-    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="97">
         <v>15</v>
       </c>
@@ -5794,7 +5808,7 @@
       </c>
       <c r="D17" s="126"/>
     </row>
-    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="97">
         <v>16</v>
       </c>
@@ -5806,7 +5820,7 @@
       </c>
       <c r="D18" s="126"/>
     </row>
-    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="97">
         <v>17</v>
       </c>
@@ -5819,7 +5833,7 @@
       </c>
       <c r="D19" s="126"/>
     </row>
-    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="97">
         <v>18</v>
       </c>
@@ -5832,99 +5846,127 @@
       </c>
       <c r="D20" s="126"/>
     </row>
-    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="97">
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="C21" s="93">
         <v>17000</v>
       </c>
       <c r="D21" s="126"/>
     </row>
-    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="97">
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C22" s="93">
-        <v>20000</v>
+        <v>10306.450000000001</v>
       </c>
       <c r="D22" s="126"/>
     </row>
-    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="97">
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="C23" s="93">
-        <v>17000</v>
-      </c>
-      <c r="D23" s="135"/>
-    </row>
-    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20000</v>
+      </c>
+      <c r="D23" s="126"/>
+    </row>
+    <row r="24" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="97">
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="C24" s="93">
-        <v>55000</v>
+        <v>17000</v>
       </c>
       <c r="D24" s="135"/>
     </row>
-    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="97">
         <v>23</v>
       </c>
       <c r="B25" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="93">
+        <v>55000</v>
+      </c>
+      <c r="D25" s="135"/>
+    </row>
+    <row r="26" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97">
+        <v>24</v>
+      </c>
+      <c r="B26" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="93">
+      <c r="C26" s="93">
         <f>(17000/31)*12</f>
         <v>6580.645161290322</v>
       </c>
-      <c r="D25" s="135"/>
-    </row>
-    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="97">
-        <v>24</v>
-      </c>
-      <c r="B26" s="87" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="93">
+      <c r="D26" s="135"/>
+    </row>
+    <row r="27" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="97">
+        <v>25</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="93">
         <v>45935.48</v>
       </c>
-      <c r="D26" s="135"/>
-    </row>
-    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="87"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="126"/>
-    </row>
-    <row r="28" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="21" t="s">
+      <c r="D27" s="135"/>
+    </row>
+    <row r="28" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97">
+        <v>26</v>
+      </c>
+      <c r="B28" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="93">
+        <f>(15000/30)*9 + 1000</f>
+        <v>5500</v>
+      </c>
+      <c r="D28" s="135"/>
+      <c r="F28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="87"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="126"/>
+    </row>
+    <row r="30" spans="1:6" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="22">
-        <f>SUM(C3:C27)</f>
-        <v>1297007.8390322581</v>
-      </c>
-      <c r="D28" s="128"/>
+      <c r="C30" s="22">
+        <f>SUM(C3:C29)</f>
+        <v>1328249.7690322581</v>
+      </c>
+      <c r="D30" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pro golg agosto updated
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D56211-760D-E843-98B1-26B44AA8D25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD79A570-C266-3A4C-A0C2-44A82ACE18D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" firstSheet="1" activeTab="8" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
   <sheets>
     <sheet name="JANEIRO" sheetId="3" r:id="rId1"/>
@@ -21,10 +21,12 @@
     <sheet name="MAIO" sheetId="6" r:id="rId6"/>
     <sheet name="JUNHO" sheetId="7" r:id="rId7"/>
     <sheet name="JULHO" sheetId="8" r:id="rId8"/>
+    <sheet name="AGOSTO" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">AGOSTO!$A$1:$E$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FEVEREIRO!$A$1:$E$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">JULHO!$A$1:$E$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">JULHO!$A$1:$E$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="198">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -484,9 +486,6 @@
     <t>JOÃO VICTOR  - PATROL 140 K  SÉRIE 5531 09/06 - 24/06</t>
   </si>
   <si>
-    <t>JULHO DE 2024 - MUDAR</t>
-  </si>
-  <si>
     <t xml:space="preserve">FBS FRANCISCO MORATO </t>
   </si>
   <si>
@@ -596,6 +595,54 @@
   </si>
   <si>
     <t>JHSF - PARQUES - 23/07 + MOB.ESCAVADEIRA + 24/07 CB + CB E RETRO 30/07</t>
+  </si>
+  <si>
+    <t>1319 / 1322 / 1330</t>
+  </si>
+  <si>
+    <t>JHSF DIESEL - 5 NOTAS</t>
+  </si>
+  <si>
+    <t>JHSF STATES - ERICA - PAGO PARCIALMENTE - TRATOR</t>
+  </si>
+  <si>
+    <t>ATRASADOS EMITIDOS DE JULHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JHSF - PRÓ GOLF - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JHSF - PARQUES - </t>
+  </si>
+  <si>
+    <t>ALCANCE - 1º QUINZENA AGOSTO DE 2024</t>
+  </si>
+  <si>
+    <t>ALCANCE - 2º QUINZENA AGOSTO DE 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBS VIADUTO - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEANDRO QUINA D4  -SOLOTEC - SÉRIE 536 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENILSON - RETRO JCB - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFONSO FRANÇA ASHLAND - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERINHA PEDRAS - ROLO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGOSTO DE 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JULHO DE 2024 </t>
+  </si>
+  <si>
+    <t>ASSOCIACAO FAZ.BOA VISTA TRATOR D51 - 01/08</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1418,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1659,9 +1706,6 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1671,15 +1715,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1696,6 +1743,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2107,10 +2157,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="156"/>
+      <c r="B1" s="157"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
@@ -2409,10 +2459,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="156"/>
+      <c r="C1" s="157"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2545,7 +2595,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="157">
+      <c r="A11" s="164">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2560,7 +2610,7 @@
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
+      <c r="A12" s="164"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2649,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="157">
+      <c r="A15" s="164">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2614,7 +2664,7 @@
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="157"/>
+      <c r="A16" s="164"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2625,7 +2675,7 @@
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="157"/>
+      <c r="A17" s="164"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +2716,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="157">
+      <c r="A20" s="164">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2681,7 +2731,7 @@
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="157"/>
+      <c r="A21" s="164"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
@@ -2793,7 +2843,7 @@
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="157">
+      <c r="A29" s="164">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2806,7 +2856,7 @@
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="157"/>
+      <c r="A30" s="164"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
@@ -2817,7 +2867,7 @@
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="157"/>
+      <c r="A31" s="164"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
@@ -2828,7 +2878,7 @@
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="157"/>
+      <c r="A32" s="164"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
@@ -2851,15 +2901,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -2893,10 +2943,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="156" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="156"/>
+      <c r="C1" s="157"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -2996,7 +3046,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="164">
+      <c r="A11" s="165">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3007,7 +3057,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="164"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3027,7 +3077,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="164">
+      <c r="A14" s="165">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3038,7 +3088,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="164"/>
+      <c r="A15" s="165"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3047,7 +3097,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="164"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3056,7 +3106,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="164"/>
+      <c r="A17" s="165"/>
       <c r="B17" s="10" t="s">
         <v>88</v>
       </c>
@@ -3065,7 +3115,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="164"/>
+      <c r="A18" s="165"/>
       <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
@@ -3096,7 +3146,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="164">
+      <c r="A21" s="165">
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -3107,7 +3157,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="164"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="16" t="s">
         <v>73</v>
       </c>
@@ -3204,7 +3254,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="164">
+      <c r="A31" s="165">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3215,7 +3265,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164"/>
+      <c r="A32" s="165"/>
       <c r="B32" s="19" t="s">
         <v>55</v>
       </c>
@@ -3224,7 +3274,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="164"/>
+      <c r="A33" s="165"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -3365,10 +3415,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="156"/>
+      <c r="C1" s="157"/>
     </row>
     <row r="2" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -3467,7 +3517,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="164">
+      <c r="A11" s="165">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3478,7 +3528,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="164"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3548,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="164">
+      <c r="A14" s="165">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3509,7 +3559,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="164"/>
+      <c r="A15" s="165"/>
       <c r="B15" s="10" t="s">
         <v>71</v>
       </c>
@@ -3518,7 +3568,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="164"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
@@ -3527,7 +3577,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="164"/>
+      <c r="A17" s="165"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
@@ -3536,7 +3586,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="164"/>
+      <c r="A18" s="165"/>
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
@@ -3567,7 +3617,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="164">
+      <c r="A21" s="165">
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3578,7 +3628,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="164"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="16" t="s">
         <v>74</v>
       </c>
@@ -3675,7 +3725,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="164">
+      <c r="A31" s="165">
         <v>24</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -3686,7 +3736,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164"/>
+      <c r="A32" s="165"/>
       <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
@@ -3695,7 +3745,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="164"/>
+      <c r="A33" s="165"/>
       <c r="B33" s="19" t="s">
         <v>76</v>
       </c>
@@ -3771,18 +3821,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
     </row>
     <row r="2" spans="1:4" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="168" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="167"/>
+      <c r="B2" s="168"/>
       <c r="C2" s="84" t="s">
         <v>2</v>
       </c>
@@ -4244,10 +4294,10 @@
       <c r="D40" s="79"/>
     </row>
     <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="168" t="s">
+      <c r="A41" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="169"/>
+      <c r="B41" s="170"/>
       <c r="C41" s="82">
         <f>SUM(C3:C40)</f>
         <v>2994400.49</v>
@@ -4255,10 +4305,10 @@
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="170" t="s">
+      <c r="A42" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="171"/>
+      <c r="B42" s="172"/>
       <c r="C42" s="65">
         <f>SUM(C3:C27)</f>
         <v>1708991.02</v>
@@ -4266,10 +4316,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="165" t="s">
+      <c r="A43" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="166"/>
+      <c r="B43" s="167"/>
       <c r="C43" s="83">
         <f>SUM(C28:C40)</f>
         <v>1285409.4700000002</v>
@@ -4302,8 +4352,8 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4314,11 +4364,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="179" t="s">
+      <c r="B1" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
     </row>
     <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -4598,7 +4648,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="93">
         <v>6000</v>
@@ -4612,12 +4662,12 @@
       <c r="D23" s="105"/>
     </row>
     <row r="24" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="172" t="s">
+      <c r="A24" s="173" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="173"/>
-      <c r="C24" s="173"/>
-      <c r="D24" s="174"/>
+      <c r="B24" s="174"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="175"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="76" t="s">
@@ -4642,7 +4692,7 @@
         <v>191666</v>
       </c>
       <c r="D26" s="138" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4701,13 +4751,13 @@
         <v>132</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C31" s="139">
         <v>168000</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4859,10 +4909,10 @@
       <c r="D43" s="79"/>
     </row>
     <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A44" s="168" t="s">
+      <c r="A44" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="169"/>
+      <c r="B44" s="170"/>
       <c r="C44" s="82">
         <f>SUM(C3:C23)+SUM(C25:C43)</f>
         <v>2859542.4567741938</v>
@@ -4870,10 +4920,10 @@
       <c r="D44" s="79"/>
     </row>
     <row r="45" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A45" s="170" t="s">
+      <c r="A45" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="171"/>
+      <c r="B45" s="172"/>
       <c r="C45" s="65">
         <f>SUM(C3:C22)</f>
         <v>625891.25677419361</v>
@@ -4881,10 +4931,10 @@
       <c r="D45" s="79"/>
     </row>
     <row r="46" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="165" t="s">
+      <c r="A46" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="166"/>
+      <c r="B46" s="167"/>
       <c r="C46" s="83">
         <f>SUM(C25:C43)</f>
         <v>2233651.2000000002</v>
@@ -4892,18 +4942,18 @@
       <c r="D46" s="79"/>
     </row>
     <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="172"/>
-      <c r="B47" s="173"/>
-      <c r="C47" s="173"/>
-      <c r="D47" s="174"/>
+      <c r="A47" s="173"/>
+      <c r="B47" s="174"/>
+      <c r="C47" s="174"/>
+      <c r="D47" s="175"/>
     </row>
     <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="172" t="s">
+      <c r="A48" s="173" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="173"/>
-      <c r="C48" s="173"/>
-      <c r="D48" s="174"/>
+      <c r="B48" s="174"/>
+      <c r="C48" s="174"/>
+      <c r="D48" s="175"/>
     </row>
     <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="115" t="s">
@@ -4948,15 +4998,15 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="175" t="s">
+      <c r="A52" s="176" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="176"/>
-      <c r="C52" s="177">
+      <c r="B52" s="177"/>
+      <c r="C52" s="178">
         <f>SUM(C49:C51)</f>
         <v>47612.9</v>
       </c>
-      <c r="D52" s="178"/>
+      <c r="D52" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4983,8 +5033,8 @@
   </sheetPr>
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4996,11 +5046,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="179" t="s">
+      <c r="B1" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
@@ -5024,7 +5074,7 @@
         <v>334000</v>
       </c>
       <c r="D3" s="127" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -5032,7 +5082,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="5">
         <v>35000</v>
@@ -5068,7 +5118,7 @@
         <v>35000</v>
       </c>
       <c r="D7" s="141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -5096,7 +5146,7 @@
         <v>40000</v>
       </c>
       <c r="D9" s="127" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -5175,7 +5225,7 @@
         <v>49065.14</v>
       </c>
       <c r="D15" s="127" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -5278,7 +5328,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C23" s="93">
         <v>15000</v>
@@ -5291,12 +5341,12 @@
       <c r="D24" s="126"/>
     </row>
     <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="172" t="s">
+      <c r="A25" s="173" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="173"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="174"/>
+      <c r="B25" s="174"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="175"/>
     </row>
     <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="76" t="s">
@@ -5348,7 +5398,7 @@
     </row>
     <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" s="77" t="s">
         <v>120</v>
@@ -5375,7 +5425,7 @@
         <v>132</v>
       </c>
       <c r="B32" s="80" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C32" s="113">
         <f>168000*0.15</f>
@@ -5435,10 +5485,10 @@
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B37" s="77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="78">
         <v>17000</v>
@@ -5449,7 +5499,7 @@
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" s="77" t="s">
         <v>122</v>
@@ -5461,7 +5511,7 @@
     </row>
     <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="77" t="s">
         <v>109</v>
@@ -5473,10 +5523,10 @@
     </row>
     <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B40" s="77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="78">
         <v>6000</v>
@@ -5485,7 +5535,7 @@
     </row>
     <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B41" s="77" t="s">
         <v>110</v>
@@ -5504,10 +5554,10 @@
       <c r="D42" s="79"/>
     </row>
     <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="168" t="s">
+      <c r="A43" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="169"/>
+      <c r="B43" s="170"/>
       <c r="C43" s="82">
         <f>SUM(C3:C24)+SUM(C26:C42)</f>
         <v>2557948.7333333334</v>
@@ -5515,10 +5565,10 @@
       <c r="D43" s="79"/>
     </row>
     <row r="44" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A44" s="170" t="s">
+      <c r="A44" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="171"/>
+      <c r="B44" s="172"/>
       <c r="C44" s="65">
         <f>SUM(C3:C23)</f>
         <v>1072948.4733333334</v>
@@ -5526,10 +5576,10 @@
       <c r="D44" s="79"/>
     </row>
     <row r="45" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="166"/>
+      <c r="B45" s="167"/>
       <c r="C45" s="83">
         <f>SUM(C26:C42)</f>
         <v>1485000.26</v>
@@ -5537,18 +5587,18 @@
       <c r="D45" s="79"/>
     </row>
     <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="172"/>
-      <c r="B46" s="173"/>
-      <c r="C46" s="173"/>
-      <c r="D46" s="174"/>
+      <c r="A46" s="173"/>
+      <c r="B46" s="174"/>
+      <c r="C46" s="174"/>
+      <c r="D46" s="175"/>
     </row>
     <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="172" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="173"/>
-      <c r="C47" s="173"/>
-      <c r="D47" s="174"/>
+      <c r="A47" s="173" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="174"/>
+      <c r="C47" s="174"/>
+      <c r="D47" s="175"/>
     </row>
     <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="68" t="s">
@@ -5561,7 +5611,7 @@
         <v>191666</v>
       </c>
       <c r="D48" s="138" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -5583,13 +5633,13 @@
         <v>132</v>
       </c>
       <c r="B50" s="69" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C50" s="139">
         <v>142800</v>
       </c>
       <c r="D50" s="70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -5636,10 +5686,10 @@
     </row>
     <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B54" s="69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C54" s="70">
         <f>(35000/31)*3</f>
@@ -5662,15 +5712,15 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="175" t="s">
+      <c r="A56" s="176" t="s">
         <v>139</v>
       </c>
-      <c r="B56" s="176"/>
-      <c r="C56" s="177">
+      <c r="B56" s="177"/>
+      <c r="C56" s="178">
         <f>SUM(C48:C55)</f>
         <v>866586.42677419353</v>
       </c>
-      <c r="D56" s="178"/>
+      <c r="D56" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5696,7 +5746,7 @@
   </sheetPr>
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5711,15 +5761,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B1" s="179" t="s">
+      <c r="B1" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
     </row>
     <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>2</v>
@@ -5733,11 +5783,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="5">
-        <f>177412.9+1800</f>
-        <v>179212.9</v>
+        <v>175612.9</v>
       </c>
       <c r="D3" s="126"/>
     </row>
@@ -5746,7 +5795,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="5">
         <v>35000</v>
@@ -5758,7 +5807,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="5">
         <v>341000</v>
@@ -5770,10 +5819,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" s="5">
-        <v>41500</v>
+        <v>41177.42</v>
       </c>
       <c r="D6" s="126"/>
     </row>
@@ -5782,7 +5831,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="5">
         <v>85000</v>
@@ -5794,10 +5843,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6">
-        <v>35000</v>
+        <v>183</v>
+      </c>
+      <c r="C8" s="5">
+        <v>15000</v>
       </c>
       <c r="D8" s="126"/>
     </row>
@@ -5806,10 +5855,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" s="133">
-        <v>41750</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>35000</v>
       </c>
       <c r="D9" s="126"/>
     </row>
@@ -5817,11 +5866,11 @@
       <c r="A10" s="97">
         <v>8</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="5">
-        <v>40000</v>
+      <c r="B10" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="133">
+        <v>41750</v>
       </c>
       <c r="D10" s="126"/>
     </row>
@@ -5830,34 +5879,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="C11" s="5">
-        <v>73000</v>
+        <v>40000</v>
       </c>
       <c r="D11" s="126"/>
     </row>
-    <row r="12" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="97">
         <v>10</v>
       </c>
-      <c r="B12" s="124" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="125">
-        <v>85500</v>
-      </c>
-      <c r="D12" s="135"/>
-    </row>
-    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5">
+        <v>73000</v>
+      </c>
+      <c r="D12" s="126"/>
+    </row>
+    <row r="13" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="97">
         <v>11</v>
       </c>
-      <c r="B13" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="91">
-        <v>36403</v>
+      <c r="B13" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="125">
+        <v>85500</v>
       </c>
       <c r="D13" s="135"/>
     </row>
@@ -5866,22 +5915,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="86" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="C14" s="91">
-        <v>30000</v>
-      </c>
-      <c r="D14" s="126"/>
+        <v>36403</v>
+      </c>
+      <c r="D14" s="135"/>
     </row>
     <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="97">
         <v>13</v>
       </c>
-      <c r="B15" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="92">
-        <v>27000</v>
+      <c r="B15" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="91">
+        <v>30000</v>
       </c>
       <c r="D15" s="126"/>
     </row>
@@ -5889,11 +5938,11 @@
       <c r="A16" s="97">
         <v>14</v>
       </c>
-      <c r="B16" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="93">
-        <v>26000</v>
+      <c r="B16" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="92">
+        <v>27000</v>
       </c>
       <c r="D16" s="126"/>
     </row>
@@ -5902,10 +5951,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="93">
-        <v>46000</v>
+        <v>26000</v>
       </c>
       <c r="D17" s="126"/>
     </row>
@@ -5914,10 +5963,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C18" s="93">
-        <v>15000</v>
+        <v>46000</v>
       </c>
       <c r="D18" s="126"/>
     </row>
@@ -5926,11 +5975,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="C19" s="93">
-        <f>(19/31)*14000</f>
-        <v>8580.645161290322</v>
+        <v>15000</v>
       </c>
       <c r="D19" s="126"/>
     </row>
@@ -5939,11 +5987,11 @@
         <v>18</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C20" s="93">
-        <f>(18/31)*23000</f>
-        <v>13354.83870967742</v>
+        <f>(19/31)*14000</f>
+        <v>8580.645161290322</v>
       </c>
       <c r="D20" s="126"/>
     </row>
@@ -5952,10 +6000,11 @@
         <v>19</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C21" s="93">
-        <v>17000</v>
+        <f>(18/31)*23000</f>
+        <v>13354.83870967742</v>
       </c>
       <c r="D21" s="126"/>
     </row>
@@ -5964,10 +6013,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C22" s="93">
-        <v>10306.450000000001</v>
+        <v>17000</v>
       </c>
       <c r="D22" s="126"/>
     </row>
@@ -5976,10 +6025,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="C23" s="93">
-        <v>20000</v>
+        <v>10306.450000000001</v>
       </c>
       <c r="D23" s="126"/>
     </row>
@@ -5988,22 +6037,22 @@
         <v>22</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="C24" s="93">
-        <v>17000</v>
-      </c>
-      <c r="D24" s="135"/>
+        <v>20000</v>
+      </c>
+      <c r="D24" s="126"/>
     </row>
     <row r="25" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="97">
         <v>23</v>
       </c>
       <c r="B25" s="87" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C25" s="93">
-        <v>55000</v>
+        <v>17000</v>
       </c>
       <c r="D25" s="135"/>
     </row>
@@ -6012,11 +6061,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="87" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C26" s="93">
-        <f>(17000/31)*12</f>
-        <v>6580.645161290322</v>
+        <v>55000</v>
       </c>
       <c r="D26" s="135"/>
     </row>
@@ -6025,10 +6073,11 @@
         <v>25</v>
       </c>
       <c r="B27" s="87" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C27" s="93">
-        <v>45935.48</v>
+        <f>(17000/31)*12</f>
+        <v>6580.645161290322</v>
       </c>
       <c r="D27" s="135"/>
     </row>
@@ -6037,62 +6086,62 @@
         <v>26</v>
       </c>
       <c r="B28" s="87" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C28" s="93">
+        <v>45935.48</v>
+      </c>
+      <c r="D28" s="135"/>
+    </row>
+    <row r="29" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="97">
+        <v>27</v>
+      </c>
+      <c r="B29" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="93">
         <f>(15000/30)*9 + 1000</f>
         <v>5500</v>
       </c>
-      <c r="D28" s="135"/>
-      <c r="F28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="87"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="126"/>
-    </row>
-    <row r="30" spans="1:6" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="21" t="s">
+      <c r="D29" s="135"/>
+      <c r="F29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="87"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="126"/>
+    </row>
+    <row r="31" spans="1:6" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="22">
-        <f>SUM(C3:C29)</f>
-        <v>1336623.959032258</v>
-      </c>
-      <c r="D30" s="128"/>
-    </row>
-    <row r="31" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="172" t="s">
+      <c r="C31" s="22">
+        <f>SUM(C3:C30)</f>
+        <v>1347701.3790322582</v>
+      </c>
+      <c r="D31" s="128"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="173" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="173"/>
-      <c r="C32" s="173"/>
-      <c r="D32" s="174"/>
-    </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="78">
-        <v>76525.679999999993</v>
-      </c>
-      <c r="D33" s="79"/>
+      <c r="B33" s="174"/>
+      <c r="C33" s="174"/>
+      <c r="D33" s="175"/>
     </row>
     <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
         <v>132</v>
       </c>
       <c r="B34" s="77" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C34" s="78">
-        <v>29742</v>
+        <v>76525.679999999993</v>
       </c>
       <c r="D34" s="79"/>
     </row>
@@ -6101,115 +6150,115 @@
         <v>132</v>
       </c>
       <c r="B35" s="77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" s="78">
-        <v>141000</v>
+        <v>29742</v>
       </c>
       <c r="D35" s="79"/>
     </row>
     <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="81">
-        <v>42300</v>
+        <v>132</v>
+      </c>
+      <c r="B36" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="78">
+        <v>141000</v>
       </c>
       <c r="D36" s="79"/>
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="76" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="88">
-        <v>209620</v>
-      </c>
-      <c r="D37" s="78"/>
+        <v>134</v>
+      </c>
+      <c r="B37" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="81">
+        <v>42300</v>
+      </c>
+      <c r="D37" s="79"/>
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="88">
+        <v>209620</v>
+      </c>
+      <c r="D38" s="78"/>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="B38" s="77" t="s">
+      <c r="B39" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="78">
+      <c r="C39" s="78">
         <v>223642.86</v>
       </c>
-      <c r="D38" s="79"/>
-    </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="140" t="s">
+      <c r="D39" s="79"/>
+    </row>
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="140" t="s">
         <v>132</v>
       </c>
-      <c r="B39" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" s="113">
+      <c r="B40" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="113">
         <f>168000*0.15</f>
         <v>25200</v>
       </c>
-      <c r="D39" s="81"/>
-    </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A40" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="78">
-        <v>77000</v>
-      </c>
-      <c r="D40" s="79"/>
+      <c r="D40" s="81"/>
     </row>
     <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="76" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" s="77" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C41" s="78">
-        <v>18000</v>
+        <v>77000</v>
       </c>
       <c r="D41" s="79"/>
     </row>
     <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="76" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="B42" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="78">
+        <v>18000</v>
+      </c>
+      <c r="D42" s="79"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="78">
+      <c r="C43" s="78">
         <v>55000</v>
       </c>
-      <c r="D42" s="79"/>
-    </row>
-    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B43" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="C43" s="150">
-        <v>35000</v>
-      </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="79"/>
     </row>
     <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B44" s="152" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="151" t="s">
         <v>130</v>
       </c>
       <c r="C44" s="150">
@@ -6219,10 +6268,10 @@
     </row>
     <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="78">
         <v>6000</v>
@@ -6231,15 +6280,15 @@
     </row>
     <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46" s="153" t="s">
-        <v>157</v>
+        <v>180</v>
+      </c>
+      <c r="B46" s="152" t="s">
+        <v>156</v>
       </c>
       <c r="C46" s="150">
         <v>15000</v>
       </c>
-      <c r="D46" s="154"/>
+      <c r="D46" s="153"/>
     </row>
     <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="76" t="s">
@@ -6257,10 +6306,10 @@
     </row>
     <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C48" s="78">
         <v>17000</v>
@@ -6271,7 +6320,7 @@
     </row>
     <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49" s="77" t="s">
         <v>110</v>
@@ -6285,7 +6334,7 @@
     </row>
     <row r="50" spans="1:4" ht="44" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B50" s="149" t="s">
         <v>143</v>
@@ -6297,9 +6346,9 @@
     </row>
     <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="153" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="152" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="150">
@@ -6309,9 +6358,9 @@
     </row>
     <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B52" s="153" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="152" t="s">
         <v>21</v>
       </c>
       <c r="C52" s="150">
@@ -6321,9 +6370,9 @@
     </row>
     <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B53" s="153" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="152" t="s">
         <v>29</v>
       </c>
       <c r="C53" s="150">
@@ -6333,16 +6382,16 @@
     </row>
     <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B54" s="153" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="152" t="s">
         <v>129</v>
       </c>
       <c r="C54" s="150">
         <f>(17000/30)* 23</f>
         <v>13033.333333333332</v>
       </c>
-      <c r="D54" s="154"/>
+      <c r="D54" s="153"/>
     </row>
     <row r="55" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="145"/>
@@ -6351,51 +6400,51 @@
       <c r="D55" s="148"/>
     </row>
     <row r="56" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A56" s="168" t="s">
+      <c r="A56" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="169"/>
-      <c r="C56" s="182">
-        <f>SUM(C3:C28)+SUM(C33:C55)</f>
-        <v>2673321.1623655912</v>
-      </c>
-      <c r="D56" s="183"/>
+      <c r="B56" s="170"/>
+      <c r="C56" s="183">
+        <f>SUM(C3:C29)+SUM(C34:C55)</f>
+        <v>2649398.5823655915</v>
+      </c>
+      <c r="D56" s="184"/>
     </row>
     <row r="57" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A57" s="170" t="s">
+      <c r="A57" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="171"/>
-      <c r="C57" s="184">
-        <f>SUM(C3:C28)</f>
-        <v>1336623.959032258</v>
-      </c>
-      <c r="D57" s="185"/>
+      <c r="B57" s="172"/>
+      <c r="C57" s="185">
+        <f>SUM(C3:C29)</f>
+        <v>1347701.3790322582</v>
+      </c>
+      <c r="D57" s="186"/>
     </row>
     <row r="58" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="165" t="s">
+      <c r="A58" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="166"/>
-      <c r="C58" s="186">
-        <f>SUM(C33:C55)</f>
-        <v>1336697.2033333334</v>
-      </c>
-      <c r="D58" s="187"/>
+      <c r="B58" s="167"/>
+      <c r="C58" s="187">
+        <f>SUM(C34:C55)</f>
+        <v>1301697.2033333334</v>
+      </c>
+      <c r="D58" s="188"/>
     </row>
     <row r="59" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="172"/>
-      <c r="B59" s="173"/>
-      <c r="C59" s="173"/>
-      <c r="D59" s="174"/>
+      <c r="A59" s="173"/>
+      <c r="B59" s="174"/>
+      <c r="C59" s="174"/>
+      <c r="D59" s="175"/>
     </row>
     <row r="60" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="172" t="s">
-        <v>179</v>
-      </c>
-      <c r="B60" s="173"/>
-      <c r="C60" s="173"/>
-      <c r="D60" s="174"/>
+      <c r="A60" s="173" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" s="174"/>
+      <c r="C60" s="174"/>
+      <c r="D60" s="175"/>
     </row>
     <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="68" t="s">
@@ -6408,12 +6457,12 @@
         <v>514388</v>
       </c>
       <c r="D61" s="71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B62" s="71" t="s">
         <v>109</v>
@@ -6425,11 +6474,20 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A63" s="68"/>
-      <c r="B63" s="69"/>
-      <c r="C63" s="139"/>
-      <c r="D63" s="70"/>
+    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A63" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="154" t="s">
+        <v>184</v>
+      </c>
+      <c r="C63" s="155">
+        <f>35000+3387.1</f>
+        <v>38387.1</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="68"/>
@@ -6462,15 +6520,15 @@
       <c r="D68" s="71"/>
     </row>
     <row r="69" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="175" t="s">
+      <c r="A69" s="176" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="176"/>
-      <c r="C69" s="177">
+      <c r="B69" s="177"/>
+      <c r="C69" s="178">
         <f>SUM(C61:C68)</f>
-        <v>527936.39</v>
-      </c>
-      <c r="D69" s="178"/>
+        <v>566323.49</v>
+      </c>
+      <c r="D69" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -6481,7 +6539,7 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
@@ -6489,6 +6547,640 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="53" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73594EBD-4785-184A-9F94-33329D79440C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="129" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="180" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
+    </row>
+    <row r="2" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="134" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="97">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="5">
+        <v>65205.02</v>
+      </c>
+      <c r="D3" s="135"/>
+    </row>
+    <row r="4" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="97">
+        <v>2</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="5">
+        <v>35000</v>
+      </c>
+      <c r="D4" s="126"/>
+    </row>
+    <row r="5" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="97">
+        <v>3</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="5">
+        <v>341000</v>
+      </c>
+      <c r="D5" s="126"/>
+    </row>
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="97">
+        <v>4</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="5">
+        <v>191000</v>
+      </c>
+      <c r="D6" s="135"/>
+    </row>
+    <row r="7" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="97">
+        <v>5</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="5">
+        <v>141612.9</v>
+      </c>
+      <c r="D7" s="126"/>
+    </row>
+    <row r="8" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="97">
+        <v>6</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="5">
+        <v>15000</v>
+      </c>
+      <c r="D8" s="126"/>
+    </row>
+    <row r="9" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="97">
+        <v>7</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="5">
+        <f>15000+2500+2500</f>
+        <v>20000</v>
+      </c>
+      <c r="D9" s="126"/>
+    </row>
+    <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="97">
+        <v>8</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>38000</v>
+      </c>
+      <c r="D10" s="126"/>
+    </row>
+    <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="97">
+        <v>9</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="133">
+        <v>30000</v>
+      </c>
+      <c r="D11" s="126"/>
+    </row>
+    <row r="12" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="97">
+        <v>10</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="5">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="126"/>
+    </row>
+    <row r="13" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="97">
+        <v>11</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5">
+        <v>73000</v>
+      </c>
+      <c r="D13" s="126"/>
+    </row>
+    <row r="14" spans="1:4" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="97">
+        <v>12</v>
+      </c>
+      <c r="B14" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="125">
+        <v>85500</v>
+      </c>
+      <c r="D14" s="135"/>
+    </row>
+    <row r="15" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="97">
+        <v>13</v>
+      </c>
+      <c r="B15" s="86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="91">
+        <v>33000</v>
+      </c>
+      <c r="D15" s="135"/>
+    </row>
+    <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="97">
+        <v>14</v>
+      </c>
+      <c r="B16" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="91">
+        <v>30000</v>
+      </c>
+      <c r="D16" s="126"/>
+    </row>
+    <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="97">
+        <v>15</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="92">
+        <v>27000</v>
+      </c>
+      <c r="D17" s="126"/>
+    </row>
+    <row r="18" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="97">
+        <v>16</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="93">
+        <v>26000</v>
+      </c>
+      <c r="D18" s="126"/>
+    </row>
+    <row r="19" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="97">
+        <v>17</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="93">
+        <v>46000</v>
+      </c>
+      <c r="D19" s="126"/>
+    </row>
+    <row r="20" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="97">
+        <v>18</v>
+      </c>
+      <c r="B20" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="93">
+        <v>15000</v>
+      </c>
+      <c r="D20" s="126"/>
+    </row>
+    <row r="21" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="97">
+        <v>19</v>
+      </c>
+      <c r="B21" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D21" s="126"/>
+    </row>
+    <row r="22" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="97">
+        <v>20</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="93">
+        <v>39000</v>
+      </c>
+      <c r="D22" s="135"/>
+    </row>
+    <row r="23" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="97">
+        <v>21</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="93">
+        <v>20000</v>
+      </c>
+      <c r="D23" s="126"/>
+    </row>
+    <row r="24" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="97">
+        <v>22</v>
+      </c>
+      <c r="B24" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D24" s="135"/>
+    </row>
+    <row r="25" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="97">
+        <v>23</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="93">
+        <v>55000</v>
+      </c>
+      <c r="D25" s="135"/>
+    </row>
+    <row r="26" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97">
+        <v>24</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" s="93">
+        <v>17000</v>
+      </c>
+      <c r="D26" s="135"/>
+    </row>
+    <row r="27" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="97">
+        <v>25</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" s="93">
+        <v>56000</v>
+      </c>
+      <c r="D27" s="135"/>
+    </row>
+    <row r="28" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97">
+        <v>26</v>
+      </c>
+      <c r="B28" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="93">
+        <v>11500</v>
+      </c>
+      <c r="D28" s="135"/>
+    </row>
+    <row r="29" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="87"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="126"/>
+    </row>
+    <row r="30" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="22">
+        <f>SUM(C3:C29)</f>
+        <v>1474817.92</v>
+      </c>
+      <c r="D30" s="128"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="173" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="174"/>
+      <c r="C32" s="174"/>
+      <c r="D32" s="175"/>
+    </row>
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="76"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="79"/>
+    </row>
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="79"/>
+    </row>
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="79"/>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="79"/>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="76"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="88"/>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="76"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="79"/>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="140"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="81"/>
+    </row>
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="76"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="79"/>
+    </row>
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="79"/>
+    </row>
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="76"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="79"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="151"/>
+      <c r="C43" s="150"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="79"/>
+    </row>
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="152"/>
+      <c r="C45" s="150"/>
+      <c r="D45" s="153"/>
+    </row>
+    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="76"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="114"/>
+    </row>
+    <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A47" s="76"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="79"/>
+    </row>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="76"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="79"/>
+    </row>
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="150"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="152"/>
+      <c r="C50" s="150"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="152"/>
+      <c r="C51" s="150"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="152"/>
+      <c r="C52" s="150"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="152"/>
+      <c r="C53" s="150"/>
+      <c r="D53" s="153"/>
+    </row>
+    <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A54" s="145"/>
+      <c r="B54" s="146"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
+    </row>
+    <row r="55" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A55" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="170"/>
+      <c r="C55" s="183">
+        <f>SUM(C3:C28)+SUM(C33:C54)</f>
+        <v>1474817.92</v>
+      </c>
+      <c r="D55" s="184"/>
+    </row>
+    <row r="56" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A56" s="171" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="172"/>
+      <c r="C56" s="185">
+        <f>SUM(C3:C28)</f>
+        <v>1474817.92</v>
+      </c>
+      <c r="D56" s="186"/>
+    </row>
+    <row r="57" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="166" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="167"/>
+      <c r="C57" s="187">
+        <f>SUM(C33:C54)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="188"/>
+    </row>
+    <row r="58" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="173"/>
+      <c r="B58" s="174"/>
+      <c r="C58" s="174"/>
+      <c r="D58" s="175"/>
+    </row>
+    <row r="59" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="173" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="174"/>
+      <c r="C59" s="174"/>
+      <c r="D59" s="175"/>
+    </row>
+    <row r="60" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" s="68"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="71"/>
+    </row>
+    <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A61" s="68"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="144"/>
+      <c r="D61" s="71"/>
+    </row>
+    <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A62" s="23"/>
+      <c r="B62" s="154"/>
+      <c r="C62" s="155"/>
+      <c r="D62" s="23"/>
+    </row>
+    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A63" s="68"/>
+      <c r="B63" s="69"/>
+      <c r="C63" s="70"/>
+      <c r="D63" s="71"/>
+    </row>
+    <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A64" s="68"/>
+      <c r="B64" s="69"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="71"/>
+    </row>
+    <row r="65" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A65" s="68"/>
+      <c r="B65" s="69"/>
+      <c r="C65" s="70"/>
+      <c r="D65" s="71"/>
+    </row>
+    <row r="66" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A66" s="68"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="71"/>
+    </row>
+    <row r="67" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="68"/>
+      <c r="B67" s="69"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="71"/>
+    </row>
+    <row r="68" spans="1:4" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="176" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" s="177"/>
+      <c r="C68" s="178">
+        <f>SUM(C60:C67)</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="179"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="53" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EMITIDOS E ATRASADOS ATUALIZADOS
</commit_message>
<xml_diff>
--- a/PROJEÇOES 2024.xlsx
+++ b/PROJEÇOES 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanribeiro/Desktop/CAMACON/Projecoes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D809D114-8889-4549-B706-14357E424B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD061D1-585A-9344-873C-BD1FFFC2634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="1" activeTab="7" xr2:uid="{8AC508E4-8243-894E-B483-3EA694431501}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="208">
   <si>
     <t xml:space="preserve">PROJEÇÃO FATURAMENTO </t>
   </si>
@@ -664,6 +664,15 @@
   </si>
   <si>
     <t>WL COMERCIO - ESCAV.336 - 09/08</t>
+  </si>
+  <si>
+    <t>509 / 510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511 / </t>
+  </si>
+  <si>
+    <t>JOBS - UNIFICADO - Emitiu parcial - R$ 25.859 - Resta R$ 50.666,68</t>
   </si>
 </sst>
 </file>
@@ -1808,6 +1817,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1824,9 +1836,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2688,7 +2697,7 @@
       <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="171">
+      <c r="A11" s="165">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2697,20 +2706,20 @@
       <c r="C11" s="9">
         <v>100000</v>
       </c>
-      <c r="D11" s="165" t="s">
+      <c r="D11" s="166" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="171"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="9">
         <v>100000</v>
       </c>
-      <c r="D12" s="166"/>
+      <c r="D12" s="167"/>
       <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -2742,7 +2751,7 @@
       <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="171">
+      <c r="A15" s="165">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2751,31 +2760,31 @@
       <c r="C15" s="5">
         <v>38500</v>
       </c>
-      <c r="D15" s="165" t="s">
+      <c r="D15" s="166" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="171"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11">
         <v>38500</v>
       </c>
-      <c r="D16" s="167"/>
+      <c r="D16" s="168"/>
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="171"/>
+      <c r="A17" s="165"/>
       <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="D17" s="166"/>
+      <c r="D17" s="167"/>
       <c r="E17" s="30"/>
     </row>
     <row r="18" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2809,7 +2818,7 @@
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="171">
+      <c r="A20" s="165">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2818,20 +2827,20 @@
       <c r="C20" s="17">
         <v>16500</v>
       </c>
-      <c r="D20" s="165" t="s">
+      <c r="D20" s="166" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="171"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18">
         <v>16500</v>
       </c>
-      <c r="D21" s="166"/>
+      <c r="D21" s="167"/>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -2932,11 +2941,11 @@
       <c r="C28" s="20">
         <v>45000</v>
       </c>
-      <c r="D28" s="168"/>
+      <c r="D28" s="169"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="171">
+      <c r="A29" s="165">
         <v>21</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -2945,40 +2954,40 @@
       <c r="C29" s="20">
         <v>7241.4</v>
       </c>
-      <c r="D29" s="169"/>
+      <c r="D29" s="170"/>
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="171"/>
+      <c r="A30" s="165"/>
       <c r="B30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="20">
         <v>2500</v>
       </c>
-      <c r="D30" s="169"/>
+      <c r="D30" s="170"/>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="171"/>
+      <c r="A31" s="165"/>
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="20">
         <v>16000</v>
       </c>
-      <c r="D31" s="169"/>
+      <c r="D31" s="170"/>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="171"/>
+      <c r="A32" s="165"/>
       <c r="B32" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="20">
         <v>2552</v>
       </c>
-      <c r="D32" s="170"/>
+      <c r="D32" s="171"/>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2994,6 +3003,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A20:A21"/>
@@ -3002,7 +3012,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D28:D32"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{5DD56C73-7B4A-5C47-BC0C-7377640F43B7}"/>
@@ -5839,8 +5848,8 @@
   </sheetPr>
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5960,16 +5969,18 @@
       <c r="D9" s="126"/>
     </row>
     <row r="10" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97">
+      <c r="A10" s="101">
         <v>8</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="133">
+      <c r="C10" s="9">
         <v>52250</v>
       </c>
-      <c r="D10" s="126"/>
+      <c r="D10" s="127" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="97">
@@ -6032,16 +6043,16 @@
       <c r="D15" s="126"/>
     </row>
     <row r="16" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97">
+      <c r="A16" s="101">
         <v>14</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="92">
+      <c r="C16" s="122">
         <v>27000</v>
       </c>
-      <c r="D16" s="126"/>
+      <c r="D16" s="127"/>
     </row>
     <row r="17" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="97">
@@ -6230,16 +6241,19 @@
       <c r="D33" s="182"/>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="78">
-        <v>76525.679999999993</v>
-      </c>
-      <c r="D34" s="79"/>
+      <c r="B34" s="69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" s="70">
+        <f>76525.68-25859</f>
+        <v>50666.679999999993</v>
+      </c>
+      <c r="D34" s="71" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="76" t="s">
@@ -6434,7 +6448,7 @@
       <c r="B50" s="177"/>
       <c r="C50" s="190">
         <f>SUM(C3:C29)+SUM(C34:C49)</f>
-        <v>2239929.9223655914</v>
+        <v>2214070.9223655914</v>
       </c>
       <c r="D50" s="191"/>
     </row>
@@ -6456,7 +6470,7 @@
       <c r="B52" s="174"/>
       <c r="C52" s="194">
         <f>SUM(C34:C49)</f>
-        <v>961986.60333333327</v>
+        <v>936127.60333333327</v>
       </c>
       <c r="D52" s="195"/>
     </row>
@@ -7293,18 +7307,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>